<commit_message>
Updated office_ee.xlsx HVAC to air loop from PTAC
</commit_message>
<xml_diff>
--- a/projects/office_ee.xlsx
+++ b/projects/office_ee.xlsx
@@ -16,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$126</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$125</definedName>
     <definedName name="AnalysisType">Lookups!$A$17:$A$23</definedName>
     <definedName name="instance_defs">Lookups!$A$2:$D$9</definedName>
     <definedName name="instance_types">Lookups!$A$2:$A$9</definedName>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2574" uniqueCount="839">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2568" uniqueCount="835">
   <si>
     <t>type</t>
   </si>
@@ -2407,30 +2407,12 @@
     <t>calibration_data</t>
   </si>
   <si>
-    <t>Add Ptac</t>
-  </si>
-  <si>
-    <t>AddPTAC</t>
-  </si>
-  <si>
     <t>Heating Efficiency</t>
   </si>
   <si>
     <t>heating_efficiency</t>
   </si>
   <si>
-    <t>Heating Fuel Type</t>
-  </si>
-  <si>
-    <t>heating_fuel_type</t>
-  </si>
-  <si>
-    <t>Gas</t>
-  </si>
-  <si>
-    <t>|Gas,Electric|</t>
-  </si>
-  <si>
     <t>Cooling COP</t>
   </si>
   <si>
@@ -2558,6 +2540,12 @@
   </si>
   <si>
     <t>Replace All T12 Lamps with 25W T8 Lamps</t>
+  </si>
+  <si>
+    <t>AddSys3PSZACNgrid</t>
+  </si>
+  <si>
+    <t>Add Sys 3 - PSZ-AC Ngrid</t>
   </si>
 </sst>
 </file>
@@ -6957,7 +6945,7 @@
         <v>25</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>811</v>
+        <v>805</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>770</v>
@@ -6968,7 +6956,7 @@
         <v>26</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>812</v>
+        <v>806</v>
       </c>
       <c r="E14" s="31" t="s">
         <v>770</v>
@@ -7206,7 +7194,7 @@
         <v>787</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>813</v>
+        <v>807</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -7237,11 +7225,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y199"/>
+  <dimension ref="A1:Y198"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B96" sqref="B96"/>
+      <pane ySplit="3" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7922,13 +7910,13 @@
         <v>1</v>
       </c>
       <c r="B33" s="38" t="s">
-        <v>788</v>
+        <v>834</v>
       </c>
       <c r="C33" s="38" t="s">
-        <v>789</v>
+        <v>833</v>
       </c>
       <c r="D33" s="38" t="s">
-        <v>789</v>
+        <v>833</v>
       </c>
       <c r="E33" s="38" t="s">
         <v>68</v>
@@ -7939,10 +7927,10 @@
         <v>21</v>
       </c>
       <c r="D34" s="30" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="F34" s="30" t="s">
         <v>64</v>
@@ -7956,72 +7944,80 @@
         <v>21</v>
       </c>
       <c r="D35" s="30" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="F35" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H35" s="30" t="s">
-        <v>794</v>
-      </c>
-      <c r="I35" s="30" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D36" s="30" t="s">
-        <v>796</v>
-      </c>
-      <c r="E36" s="30" t="s">
-        <v>797</v>
-      </c>
-      <c r="F36" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="H36" s="30">
+      <c r="H35" s="30">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="38" t="b">
+    <row r="36" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="38" t="b">
         <v>1</v>
       </c>
-      <c r="B37" s="38" t="s">
+      <c r="B36" s="38" t="s">
         <v>680</v>
       </c>
-      <c r="C37" s="38" t="s">
+      <c r="C36" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="D37" s="38" t="s">
+      <c r="D36" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="E37" s="38" t="s">
+      <c r="E36" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="G37" s="39"/>
-      <c r="H37" s="39"/>
+      <c r="G36" s="39"/>
+      <c r="H36" s="39"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B37" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" s="31" t="s">
+        <v>683</v>
+      </c>
+      <c r="E37" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="F37" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H37" s="31">
+        <v>0.4</v>
+      </c>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="P37" s="40"/>
+      <c r="Q37" s="2"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B38" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D38" s="31" t="s">
-        <v>683</v>
+        <v>667</v>
       </c>
       <c r="E38" s="31" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F38" s="31" t="s">
         <v>619</v>
       </c>
+      <c r="G38" s="31" t="s">
+        <v>668</v>
+      </c>
       <c r="H38" s="31">
-        <v>0.4</v>
+        <v>30</v>
       </c>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
@@ -8037,19 +8033,19 @@
         <v>21</v>
       </c>
       <c r="D39" s="31" t="s">
-        <v>667</v>
+        <v>672</v>
       </c>
       <c r="E39" s="31" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F39" s="31" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="G39" s="31" t="s">
         <v>668</v>
       </c>
-      <c r="H39" s="31">
-        <v>30</v>
+      <c r="H39" s="31" t="s">
+        <v>669</v>
       </c>
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
@@ -8060,68 +8056,68 @@
       <c r="P39" s="40"/>
       <c r="Q39" s="2"/>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B40" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D40" s="31" t="s">
-        <v>672</v>
-      </c>
-      <c r="E40" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="F40" s="31" t="s">
-        <v>618</v>
-      </c>
-      <c r="G40" s="31" t="s">
-        <v>668</v>
-      </c>
-      <c r="H40" s="31" t="s">
-        <v>669</v>
-      </c>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
-      <c r="N40" s="3"/>
-      <c r="P40" s="40"/>
-      <c r="Q40" s="2"/>
-    </row>
-    <row r="41" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="38" t="b">
+    <row r="40" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="38" t="b">
         <v>1</v>
       </c>
-      <c r="B41" s="38" t="s">
+      <c r="B40" s="38" t="s">
         <v>687</v>
       </c>
-      <c r="C41" s="38" t="s">
+      <c r="C40" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="D41" s="38" t="s">
+      <c r="D40" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="E41" s="38" t="s">
+      <c r="E40" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="G41" s="39"/>
-      <c r="H41" s="39"/>
+      <c r="G40" s="39"/>
+      <c r="H40" s="39"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B41" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" s="31" t="s">
+        <v>684</v>
+      </c>
+      <c r="E41" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="F41" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H41" s="31">
+        <v>0.4</v>
+      </c>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="P41" s="40"/>
+      <c r="Q41" s="2"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B42" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D42" s="31" t="s">
-        <v>684</v>
+        <v>667</v>
       </c>
       <c r="E42" s="31" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F42" s="31" t="s">
         <v>619</v>
       </c>
+      <c r="G42" s="31" t="s">
+        <v>668</v>
+      </c>
       <c r="H42" s="31">
-        <v>0.4</v>
+        <v>30</v>
       </c>
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
@@ -8137,19 +8133,19 @@
         <v>21</v>
       </c>
       <c r="D43" s="31" t="s">
-        <v>667</v>
+        <v>673</v>
       </c>
       <c r="E43" s="31" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F43" s="31" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="G43" s="31" t="s">
         <v>668</v>
       </c>
-      <c r="H43" s="31">
-        <v>30</v>
+      <c r="H43" s="31" t="s">
+        <v>82</v>
       </c>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
@@ -8160,68 +8156,68 @@
       <c r="P43" s="40"/>
       <c r="Q43" s="2"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B44" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D44" s="31" t="s">
-        <v>673</v>
-      </c>
-      <c r="E44" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="F44" s="31" t="s">
-        <v>618</v>
-      </c>
-      <c r="G44" s="31" t="s">
-        <v>668</v>
-      </c>
-      <c r="H44" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
-      <c r="L44" s="3"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="3"/>
-      <c r="P44" s="40"/>
-      <c r="Q44" s="2"/>
-    </row>
-    <row r="45" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="38" t="b">
+    <row r="44" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="38" t="b">
         <v>1</v>
       </c>
-      <c r="B45" s="38" t="s">
+      <c r="B44" s="38" t="s">
         <v>688</v>
       </c>
-      <c r="C45" s="38" t="s">
+      <c r="C44" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="D45" s="38" t="s">
+      <c r="D44" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="E45" s="38" t="s">
+      <c r="E44" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="G45" s="39"/>
-      <c r="H45" s="39"/>
+      <c r="G44" s="39"/>
+      <c r="H44" s="39"/>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B45" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" s="31" t="s">
+        <v>685</v>
+      </c>
+      <c r="E45" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="F45" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H45" s="31">
+        <v>0.4</v>
+      </c>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="3"/>
+      <c r="P45" s="40"/>
+      <c r="Q45" s="2"/>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B46" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D46" s="31" t="s">
-        <v>685</v>
+        <v>667</v>
       </c>
       <c r="E46" s="31" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F46" s="31" t="s">
         <v>619</v>
       </c>
+      <c r="G46" s="31" t="s">
+        <v>668</v>
+      </c>
       <c r="H46" s="31">
-        <v>0.4</v>
+        <v>30</v>
       </c>
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
@@ -8237,19 +8233,19 @@
         <v>21</v>
       </c>
       <c r="D47" s="31" t="s">
-        <v>667</v>
+        <v>674</v>
       </c>
       <c r="E47" s="31" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F47" s="31" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="G47" s="31" t="s">
         <v>668</v>
       </c>
-      <c r="H47" s="31">
-        <v>30</v>
+      <c r="H47" s="31" t="s">
+        <v>670</v>
       </c>
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
@@ -8260,68 +8256,68 @@
       <c r="P47" s="40"/>
       <c r="Q47" s="2"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B48" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D48" s="31" t="s">
-        <v>674</v>
-      </c>
-      <c r="E48" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="F48" s="31" t="s">
-        <v>618</v>
-      </c>
-      <c r="G48" s="31" t="s">
-        <v>668</v>
-      </c>
-      <c r="H48" s="31" t="s">
-        <v>670</v>
-      </c>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
-      <c r="L48" s="3"/>
-      <c r="M48" s="3"/>
-      <c r="N48" s="3"/>
-      <c r="P48" s="40"/>
-      <c r="Q48" s="2"/>
-    </row>
-    <row r="49" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="38" t="b">
+    <row r="48" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="38" t="b">
         <v>1</v>
       </c>
-      <c r="B49" s="38" t="s">
+      <c r="B48" s="38" t="s">
         <v>681</v>
       </c>
-      <c r="C49" s="38" t="s">
+      <c r="C48" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="D49" s="38" t="s">
+      <c r="D48" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="E49" s="38" t="s">
+      <c r="E48" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="G49" s="39"/>
-      <c r="H49" s="39"/>
+      <c r="G48" s="39"/>
+      <c r="H48" s="39"/>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B49" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D49" s="31" t="s">
+        <v>686</v>
+      </c>
+      <c r="E49" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="F49" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="H49" s="31">
+        <v>0.4</v>
+      </c>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3"/>
+      <c r="N49" s="3"/>
+      <c r="P49" s="40"/>
+      <c r="Q49" s="2"/>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B50" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D50" s="31" t="s">
-        <v>686</v>
+        <v>667</v>
       </c>
       <c r="E50" s="31" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F50" s="31" t="s">
         <v>619</v>
       </c>
+      <c r="G50" s="31" t="s">
+        <v>668</v>
+      </c>
       <c r="H50" s="31">
-        <v>0.4</v>
+        <v>30</v>
       </c>
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
@@ -8337,19 +8333,19 @@
         <v>21</v>
       </c>
       <c r="D51" s="31" t="s">
-        <v>667</v>
+        <v>675</v>
       </c>
       <c r="E51" s="31" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F51" s="31" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="G51" s="31" t="s">
         <v>668</v>
       </c>
-      <c r="H51" s="31">
-        <v>30</v>
+      <c r="H51" s="31" t="s">
+        <v>671</v>
       </c>
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
@@ -8360,68 +8356,58 @@
       <c r="P51" s="40"/>
       <c r="Q51" s="2"/>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B52" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D52" s="31" t="s">
-        <v>675</v>
-      </c>
-      <c r="E52" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="F52" s="31" t="s">
+    <row r="52" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="B52" s="38" t="s">
+        <v>691</v>
+      </c>
+      <c r="C52" s="38" t="s">
+        <v>690</v>
+      </c>
+      <c r="D52" s="38" t="s">
+        <v>690</v>
+      </c>
+      <c r="E52" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="G52" s="39"/>
+      <c r="H52" s="39"/>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B53" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D53" s="31" t="s">
+        <v>693</v>
+      </c>
+      <c r="E53" s="31" t="s">
+        <v>692</v>
+      </c>
+      <c r="F53" s="31" t="s">
         <v>618</v>
       </c>
-      <c r="G52" s="31" t="s">
-        <v>668</v>
-      </c>
-      <c r="H52" s="31" t="s">
-        <v>671</v>
-      </c>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
-      <c r="K52" s="3"/>
-      <c r="L52" s="3"/>
-      <c r="M52" s="3"/>
-      <c r="N52" s="3"/>
-      <c r="P52" s="40"/>
-      <c r="Q52" s="2"/>
-    </row>
-    <row r="53" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="B53" s="38" t="s">
-        <v>691</v>
-      </c>
-      <c r="C53" s="38" t="s">
-        <v>690</v>
-      </c>
-      <c r="D53" s="38" t="s">
-        <v>690</v>
-      </c>
-      <c r="E53" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="G53" s="39"/>
-      <c r="H53" s="39"/>
+      <c r="H53" s="31" t="s">
+        <v>702</v>
+      </c>
+      <c r="I53" s="31"/>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B54" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D54" s="31" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="E54" s="31" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="F54" s="31" t="s">
         <v>618</v>
       </c>
       <c r="H54" s="31" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="I54" s="31"/>
     </row>
@@ -8430,16 +8416,16 @@
         <v>21</v>
       </c>
       <c r="D55" s="31" t="s">
-        <v>695</v>
+        <v>698</v>
       </c>
       <c r="E55" s="31" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="F55" s="31" t="s">
         <v>618</v>
       </c>
-      <c r="H55" s="31" t="s">
-        <v>703</v>
+      <c r="H55" s="41" t="s">
+        <v>701</v>
       </c>
       <c r="I55" s="31"/>
     </row>
@@ -8448,109 +8434,108 @@
         <v>21</v>
       </c>
       <c r="D56" s="31" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="E56" s="31" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="F56" s="31" t="s">
         <v>618</v>
       </c>
       <c r="H56" s="41" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="I56" s="31"/>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B57" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D57" s="31" t="s">
-        <v>699</v>
-      </c>
-      <c r="E57" s="31" t="s">
-        <v>697</v>
-      </c>
-      <c r="F57" s="31" t="s">
-        <v>618</v>
-      </c>
-      <c r="H57" s="41" t="s">
-        <v>700</v>
-      </c>
-      <c r="I57" s="31"/>
+    <row r="57" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="B57" s="38" t="s">
+        <v>705</v>
+      </c>
+      <c r="C57" s="38" t="s">
+        <v>704</v>
+      </c>
+      <c r="D57" s="38" t="s">
+        <v>704</v>
+      </c>
+      <c r="E57" s="38" t="s">
+        <v>233</v>
+      </c>
+      <c r="G57" s="39"/>
+      <c r="H57" s="39"/>
     </row>
     <row r="58" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="38" t="b">
         <v>1</v>
       </c>
       <c r="B58" s="38" t="s">
-        <v>705</v>
+        <v>775</v>
       </c>
       <c r="C58" s="38" t="s">
-        <v>704</v>
+        <v>76</v>
       </c>
       <c r="D58" s="38" t="s">
-        <v>704</v>
+        <v>76</v>
       </c>
       <c r="E58" s="38" t="s">
-        <v>233</v>
+        <v>68</v>
       </c>
       <c r="G58" s="39"/>
       <c r="H58" s="39"/>
     </row>
-    <row r="59" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="B59" s="38" t="s">
-        <v>775</v>
-      </c>
-      <c r="C59" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="D59" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="E59" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="G59" s="39"/>
-      <c r="H59" s="39"/>
-    </row>
-    <row r="60" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="D60" s="43" t="s">
+    <row r="59" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D59" s="43" t="s">
         <v>776</v>
       </c>
-      <c r="E60" s="43" t="s">
+      <c r="E59" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="F60" s="43" t="s">
+      <c r="F59" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="H60" s="43">
+      <c r="H59" s="43">
         <v>0.44400000000000001</v>
       </c>
-      <c r="J60" s="43">
+      <c r="J59" s="43">
         <v>0.3</v>
       </c>
-      <c r="K60" s="43">
+      <c r="K59" s="43">
         <v>0.5</v>
       </c>
-      <c r="L60" s="43">
+      <c r="L59" s="43">
         <v>0.4</v>
       </c>
-      <c r="M60" s="43">
-        <f>(K60+J60)/6</f>
+      <c r="M59" s="43">
+        <f>(K59+J59)/6</f>
         <v>0.13333333333333333</v>
       </c>
-      <c r="N60" s="43">
+      <c r="N59" s="43">
         <v>0.01</v>
       </c>
-      <c r="Q60" s="43" t="s">
+      <c r="Q59" s="43" t="s">
         <v>777</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D60" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="E60" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="F60" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="H60" s="30">
+        <v>30</v>
       </c>
     </row>
     <row r="61" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -8558,91 +8543,91 @@
         <v>21</v>
       </c>
       <c r="D61" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="E61" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="F61" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="H61" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="I61" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="B62" s="38" t="s">
+        <v>778</v>
+      </c>
+      <c r="C62" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="D62" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="E62" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="G62" s="39"/>
+      <c r="H62" s="39"/>
+    </row>
+    <row r="63" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D63" s="43" t="s">
+        <v>779</v>
+      </c>
+      <c r="E63" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="F63" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="H63" s="43">
+        <v>0.2</v>
+      </c>
+      <c r="J63" s="43">
+        <v>0.3</v>
+      </c>
+      <c r="K63" s="43">
+        <v>0.5</v>
+      </c>
+      <c r="L63" s="43">
+        <v>0.4</v>
+      </c>
+      <c r="M63" s="43">
+        <f>(K63+J63)/6</f>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="N63" s="43">
+        <v>0.01</v>
+      </c>
+      <c r="Q63" s="43" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D64" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="E61" s="30" t="s">
+      <c r="E64" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="F61" s="30" t="s">
+      <c r="F64" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="H61" s="30">
+      <c r="H64" s="30">
         <v>30</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D62" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="E62" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="F62" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H62" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="I62" s="30" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="B63" s="38" t="s">
-        <v>778</v>
-      </c>
-      <c r="C63" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="D63" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="E63" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="G63" s="39"/>
-      <c r="H63" s="39"/>
-    </row>
-    <row r="64" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="D64" s="43" t="s">
-        <v>779</v>
-      </c>
-      <c r="E64" s="43" t="s">
-        <v>77</v>
-      </c>
-      <c r="F64" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="H64" s="43">
-        <v>0.2</v>
-      </c>
-      <c r="J64" s="43">
-        <v>0.3</v>
-      </c>
-      <c r="K64" s="43">
-        <v>0.5</v>
-      </c>
-      <c r="L64" s="43">
-        <v>0.4</v>
-      </c>
-      <c r="M64" s="43">
-        <f>(K64+J64)/6</f>
-        <v>0.13333333333333333</v>
-      </c>
-      <c r="N64" s="43">
-        <v>0.01</v>
-      </c>
-      <c r="Q64" s="43" t="s">
-        <v>777</v>
       </c>
     </row>
     <row r="65" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -8650,91 +8635,91 @@
         <v>21</v>
       </c>
       <c r="D65" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="E65" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="F65" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="H65" s="30" t="s">
+        <v>670</v>
+      </c>
+      <c r="I65" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="B66" s="38" t="s">
+        <v>780</v>
+      </c>
+      <c r="C66" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="D66" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="E66" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="G66" s="39"/>
+      <c r="H66" s="39"/>
+    </row>
+    <row r="67" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D67" s="43" t="s">
+        <v>781</v>
+      </c>
+      <c r="E67" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="F67" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="H67" s="43">
+        <v>0.3</v>
+      </c>
+      <c r="J67" s="43">
+        <v>0.3</v>
+      </c>
+      <c r="K67" s="43">
+        <v>0.5</v>
+      </c>
+      <c r="L67" s="43">
+        <v>0.4</v>
+      </c>
+      <c r="M67" s="43">
+        <f>(K67+J67)/6</f>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="N67" s="43">
+        <v>0.01</v>
+      </c>
+      <c r="Q67" s="43" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D68" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="E65" s="30" t="s">
+      <c r="E68" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="F65" s="30" t="s">
+      <c r="F68" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="H65" s="30">
+      <c r="H68" s="30">
         <v>30</v>
-      </c>
-    </row>
-    <row r="66" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D66" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="E66" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="F66" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H66" s="30" t="s">
-        <v>670</v>
-      </c>
-      <c r="I66" s="30" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="67" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="B67" s="38" t="s">
-        <v>780</v>
-      </c>
-      <c r="C67" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="D67" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="E67" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="G67" s="39"/>
-      <c r="H67" s="39"/>
-    </row>
-    <row r="68" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="D68" s="43" t="s">
-        <v>781</v>
-      </c>
-      <c r="E68" s="43" t="s">
-        <v>77</v>
-      </c>
-      <c r="F68" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="H68" s="43">
-        <v>0.3</v>
-      </c>
-      <c r="J68" s="43">
-        <v>0.3</v>
-      </c>
-      <c r="K68" s="43">
-        <v>0.5</v>
-      </c>
-      <c r="L68" s="43">
-        <v>0.4</v>
-      </c>
-      <c r="M68" s="43">
-        <f>(K68+J68)/6</f>
-        <v>0.13333333333333333</v>
-      </c>
-      <c r="N68" s="43">
-        <v>0.01</v>
-      </c>
-      <c r="Q68" s="43" t="s">
-        <v>777</v>
       </c>
     </row>
     <row r="69" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -8742,123 +8727,124 @@
         <v>21</v>
       </c>
       <c r="D69" s="30" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E69" s="30" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F69" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="H69" s="30" t="s">
+        <v>671</v>
+      </c>
+      <c r="I69" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="B70" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="C70" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="D70" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="E70" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="G70" s="39"/>
+      <c r="H70" s="39"/>
+    </row>
+    <row r="71" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D71" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="E71" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F71" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="H71" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="I71" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="O71" s="31"/>
+    </row>
+    <row r="72" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D72" s="44" t="s">
+        <v>782</v>
+      </c>
+      <c r="E72" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="F72" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="H69" s="30">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="70" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D70" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="E70" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="F70" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H70" s="30" t="s">
-        <v>671</v>
-      </c>
-      <c r="I70" s="30" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="71" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="B71" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="C71" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="D71" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="E71" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="G71" s="39"/>
-      <c r="H71" s="39"/>
-    </row>
-    <row r="72" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D72" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="E72" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="F72" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H72" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="I72" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="O72" s="31"/>
-    </row>
-    <row r="73" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="D73" s="44" t="s">
-        <v>782</v>
-      </c>
-      <c r="E73" s="43" t="s">
-        <v>70</v>
-      </c>
-      <c r="F73" s="43" t="s">
+      <c r="H72" s="43">
+        <v>-20</v>
+      </c>
+      <c r="J72" s="45">
+        <v>-100</v>
+      </c>
+      <c r="K72" s="45">
+        <v>100</v>
+      </c>
+      <c r="L72" s="45">
+        <v>0</v>
+      </c>
+      <c r="M72" s="45">
+        <f>(K72-J72)/6</f>
+        <v>33.333333333333336</v>
+      </c>
+      <c r="N72" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q72" s="43" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D73" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="E73" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="F73" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="H73" s="43">
-        <v>-20</v>
-      </c>
-      <c r="J73" s="45">
-        <v>-100</v>
-      </c>
-      <c r="K73" s="45">
-        <v>100</v>
-      </c>
-      <c r="L73" s="45">
-        <v>0</v>
-      </c>
-      <c r="M73" s="45">
-        <f>(K73-J73)/6</f>
-        <v>33.333333333333336</v>
-      </c>
-      <c r="N73" s="45">
-        <v>2.5</v>
-      </c>
-      <c r="Q73" s="43" t="s">
-        <v>777</v>
-      </c>
+      <c r="H73" s="30">
+        <v>0</v>
+      </c>
+      <c r="O73" s="31"/>
     </row>
     <row r="74" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D74" s="30" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E74" s="30" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="F74" s="30" t="s">
         <v>64</v>
@@ -8873,122 +8859,130 @@
         <v>21</v>
       </c>
       <c r="D75" s="30" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="E75" s="30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F75" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="H75" s="30">
+        <v>1</v>
+      </c>
+      <c r="O75" s="31"/>
+    </row>
+    <row r="76" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="B76" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="C76" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="D76" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="E76" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="G76" s="39"/>
+      <c r="H76" s="39"/>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A77" s="30"/>
+      <c r="B77" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C77" s="30"/>
+      <c r="D77" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="E77" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F77" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="G77" s="30"/>
+      <c r="H77" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="I77" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="J77" s="3"/>
+      <c r="K77" s="3"/>
+      <c r="L77" s="3"/>
+      <c r="M77" s="3"/>
+      <c r="N77" s="3"/>
+      <c r="P77" s="40"/>
+    </row>
+    <row r="78" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D78" s="43" t="s">
+        <v>783</v>
+      </c>
+      <c r="E78" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="F78" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="H75" s="30">
-        <v>0</v>
-      </c>
-      <c r="O75" s="31"/>
-    </row>
-    <row r="76" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D76" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="E76" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="F76" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="H76" s="30">
-        <v>1</v>
-      </c>
-      <c r="O76" s="31"/>
-    </row>
-    <row r="77" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="B77" s="38" t="s">
-        <v>67</v>
-      </c>
-      <c r="C77" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="D77" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="E77" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="G77" s="39"/>
-      <c r="H77" s="39"/>
-    </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A78" s="30"/>
-      <c r="B78" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C78" s="30"/>
-      <c r="D78" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="E78" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="F78" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="G78" s="30"/>
-      <c r="H78" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="I78" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="J78" s="3"/>
-      <c r="K78" s="3"/>
-      <c r="L78" s="3"/>
-      <c r="M78" s="3"/>
-      <c r="N78" s="3"/>
-      <c r="P78" s="40"/>
-    </row>
-    <row r="79" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="D79" s="43" t="s">
-        <v>783</v>
-      </c>
-      <c r="E79" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="F79" s="43" t="s">
+      <c r="H78" s="43">
+        <v>30</v>
+      </c>
+      <c r="I78" s="46"/>
+      <c r="J78" s="45">
+        <v>-40</v>
+      </c>
+      <c r="K78" s="45">
+        <v>40</v>
+      </c>
+      <c r="L78" s="45">
+        <v>-1</v>
+      </c>
+      <c r="M78" s="45">
+        <f>(K78-J78)/6</f>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="N78" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="P78" s="47"/>
+      <c r="Q78" s="43" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A79" s="30"/>
+      <c r="B79" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C79" s="30"/>
+      <c r="D79" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="E79" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="F79" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="H79" s="43">
-        <v>30</v>
-      </c>
-      <c r="I79" s="46"/>
-      <c r="J79" s="45">
-        <v>-40</v>
-      </c>
-      <c r="K79" s="45">
-        <v>40</v>
-      </c>
-      <c r="L79" s="45">
-        <v>-1</v>
-      </c>
-      <c r="M79" s="45">
-        <f>(K79-J79)/6</f>
-        <v>13.333333333333334</v>
-      </c>
-      <c r="N79" s="45">
-        <v>2.5</v>
-      </c>
-      <c r="P79" s="47"/>
-      <c r="Q79" s="43" t="s">
-        <v>24</v>
-      </c>
+      <c r="G79" s="30"/>
+      <c r="H79" s="30">
+        <v>0</v>
+      </c>
+      <c r="J79" s="3"/>
+      <c r="K79" s="3"/>
+      <c r="L79" s="3"/>
+      <c r="M79" s="3"/>
+      <c r="N79" s="3"/>
+      <c r="P79" s="40"/>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" s="30"/>
@@ -8996,11 +8990,11 @@
         <v>21</v>
       </c>
       <c r="C80" s="30"/>
-      <c r="D80" s="48" t="s">
-        <v>47</v>
+      <c r="D80" s="30" t="s">
+        <v>49</v>
       </c>
       <c r="E80" s="30" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F80" s="30" t="s">
         <v>64</v>
@@ -9023,13 +9017,13 @@
       </c>
       <c r="C81" s="30"/>
       <c r="D81" s="30" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E81" s="30" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F81" s="30" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G81" s="30"/>
       <c r="H81" s="30">
@@ -9049,17 +9043,17 @@
       </c>
       <c r="C82" s="30"/>
       <c r="D82" s="30" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E82" s="30" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F82" s="30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G82" s="30"/>
-      <c r="H82" s="30">
-        <v>0</v>
+      <c r="H82" s="30" t="b">
+        <v>1</v>
       </c>
       <c r="J82" s="3"/>
       <c r="K82" s="3"/>
@@ -9075,17 +9069,17 @@
       </c>
       <c r="C83" s="30"/>
       <c r="D83" s="30" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E83" s="30" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F83" s="30" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G83" s="30"/>
-      <c r="H83" s="30" t="b">
-        <v>1</v>
+      <c r="H83" s="30">
+        <v>15</v>
       </c>
       <c r="J83" s="3"/>
       <c r="K83" s="3"/>
@@ -9101,17 +9095,17 @@
       </c>
       <c r="C84" s="30"/>
       <c r="D84" s="30" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E84" s="30" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F84" s="30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G84" s="30"/>
       <c r="H84" s="30">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="J84" s="3"/>
       <c r="K84" s="3"/>
@@ -9127,17 +9121,17 @@
       </c>
       <c r="C85" s="30"/>
       <c r="D85" s="30" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E85" s="30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F85" s="30" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G85" s="30"/>
       <c r="H85" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J85" s="3"/>
       <c r="K85" s="3"/>
@@ -9146,44 +9140,42 @@
       <c r="N85" s="3"/>
       <c r="P85" s="40"/>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A86" s="30"/>
-      <c r="B86" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C86" s="30"/>
-      <c r="D86" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="E86" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="F86" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G86" s="30"/>
-      <c r="H86" s="30">
+    <row r="86" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="49" t="b">
         <v>1</v>
       </c>
-      <c r="J86" s="3"/>
-      <c r="K86" s="3"/>
-      <c r="L86" s="3"/>
-      <c r="M86" s="3"/>
-      <c r="N86" s="3"/>
-      <c r="P86" s="40"/>
+      <c r="B86" s="49" t="s">
+        <v>804</v>
+      </c>
+      <c r="C86" s="49" t="s">
+        <v>803</v>
+      </c>
+      <c r="D86" s="49" t="s">
+        <v>803</v>
+      </c>
+      <c r="E86" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="J86" s="50"/>
+      <c r="K86" s="51"/>
+      <c r="L86" s="51"/>
+      <c r="M86" s="51"/>
+      <c r="N86" s="51"/>
+      <c r="O86" s="51"/>
+      <c r="Q86" s="52"/>
     </row>
     <row r="87" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="49" t="b">
         <v>1</v>
       </c>
       <c r="B87" s="49" t="s">
-        <v>810</v>
+        <v>832</v>
       </c>
       <c r="C87" s="49" t="s">
-        <v>809</v>
+        <v>831</v>
       </c>
       <c r="D87" s="49" t="s">
-        <v>809</v>
+        <v>831</v>
       </c>
       <c r="E87" s="49" t="s">
         <v>68</v>
@@ -9196,105 +9188,101 @@
       <c r="O87" s="51"/>
       <c r="Q87" s="52"/>
     </row>
-    <row r="88" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="49" t="b">
+    <row r="88" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="B88" s="49" t="s">
-        <v>838</v>
-      </c>
-      <c r="C88" s="49" t="s">
-        <v>837</v>
-      </c>
-      <c r="D88" s="49" t="s">
-        <v>837</v>
-      </c>
-      <c r="E88" s="49" t="s">
+      <c r="B88" s="22" t="s">
+        <v>801</v>
+      </c>
+      <c r="C88" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="D88" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="E88" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="J88" s="50"/>
-      <c r="K88" s="51"/>
-      <c r="L88" s="51"/>
-      <c r="M88" s="51"/>
-      <c r="N88" s="51"/>
-      <c r="O88" s="51"/>
-      <c r="Q88" s="52"/>
-    </row>
-    <row r="89" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="B89" s="22" t="s">
-        <v>807</v>
-      </c>
-      <c r="C89" s="22" t="s">
-        <v>286</v>
-      </c>
-      <c r="D89" s="22" t="s">
-        <v>286</v>
-      </c>
-      <c r="E89" s="22" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="90" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="18"/>
-      <c r="B90" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D90" s="30" t="s">
+    </row>
+    <row r="89" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="18"/>
+      <c r="B89" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D89" s="30" t="s">
         <v>373</v>
       </c>
-      <c r="E90" s="30" t="s">
+      <c r="E89" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="F90" s="30" t="s">
+      <c r="F89" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="H90" s="30" t="s">
+      <c r="H89" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="I90" s="30" t="s">
+      <c r="I89" s="30" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="91" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="43" t="s">
+    <row r="90" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B90" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="D91" s="43" t="s">
-        <v>808</v>
-      </c>
-      <c r="E91" s="43" t="s">
+      <c r="D90" s="43" t="s">
+        <v>802</v>
+      </c>
+      <c r="E90" s="43" t="s">
         <v>288</v>
       </c>
-      <c r="F91" s="43" t="s">
+      <c r="F90" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="G91" s="43" t="s">
-        <v>798</v>
-      </c>
-      <c r="H91" s="43">
-        <v>0</v>
-      </c>
-      <c r="J91" s="43">
-        <v>0</v>
-      </c>
-      <c r="K91" s="43">
+      <c r="G90" s="43" t="s">
+        <v>792</v>
+      </c>
+      <c r="H90" s="43">
+        <v>0</v>
+      </c>
+      <c r="J90" s="43">
+        <v>0</v>
+      </c>
+      <c r="K90" s="43">
         <v>40</v>
       </c>
-      <c r="L91" s="43">
+      <c r="L90" s="43">
         <v>-1</v>
       </c>
-      <c r="M91" s="45">
-        <f>(K91-J91)/6</f>
+      <c r="M90" s="45">
+        <f>(K90-J90)/6</f>
         <v>6.666666666666667</v>
       </c>
-      <c r="N91" s="45">
+      <c r="N90" s="45">
         <v>2.5</v>
       </c>
-      <c r="Q91" s="43" t="s">
+      <c r="Q90" s="43" t="s">
         <v>777</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D91" s="30" t="s">
+        <v>793</v>
+      </c>
+      <c r="E91" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="F91" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G91" s="30" t="s">
+        <v>792</v>
+      </c>
+      <c r="H91" s="30">
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -9302,16 +9290,16 @@
         <v>21</v>
       </c>
       <c r="D92" s="30" t="s">
-        <v>799</v>
+        <v>794</v>
       </c>
       <c r="E92" s="30" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F92" s="30" t="s">
         <v>64</v>
       </c>
       <c r="G92" s="30" t="s">
-        <v>798</v>
+        <v>792</v>
       </c>
       <c r="H92" s="30">
         <v>0</v>
@@ -9322,16 +9310,16 @@
         <v>21</v>
       </c>
       <c r="D93" s="30" t="s">
-        <v>800</v>
+        <v>795</v>
       </c>
       <c r="E93" s="30" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F93" s="30" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G93" s="30" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="H93" s="30">
         <v>0</v>
@@ -9342,18 +9330,15 @@
         <v>21</v>
       </c>
       <c r="D94" s="30" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="E94" s="30" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F94" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G94" s="30" t="s">
-        <v>802</v>
-      </c>
-      <c r="H94" s="30">
+        <v>63</v>
+      </c>
+      <c r="H94" s="30" t="b">
         <v>0</v>
       </c>
     </row>
@@ -9362,16 +9347,19 @@
         <v>21</v>
       </c>
       <c r="D95" s="30" t="s">
-        <v>803</v>
+        <v>798</v>
       </c>
       <c r="E95" s="30" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F95" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="H95" s="30" t="b">
-        <v>0</v>
+        <v>65</v>
+      </c>
+      <c r="G95" s="30" t="s">
+        <v>796</v>
+      </c>
+      <c r="H95" s="30">
+        <v>15</v>
       </c>
     </row>
     <row r="96" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -9379,19 +9367,19 @@
         <v>21</v>
       </c>
       <c r="D96" s="30" t="s">
-        <v>804</v>
+        <v>799</v>
       </c>
       <c r="E96" s="30" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F96" s="30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G96" s="30" t="s">
-        <v>802</v>
+        <v>792</v>
       </c>
       <c r="H96" s="30">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="2:9" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -9399,40 +9387,24 @@
         <v>21</v>
       </c>
       <c r="D97" s="30" t="s">
-        <v>805</v>
+        <v>800</v>
       </c>
       <c r="E97" s="30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F97" s="30" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G97" s="30" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="H97" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="2:9" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D98" s="30" t="s">
-        <v>806</v>
-      </c>
-      <c r="E98" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="F98" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G98" s="30" t="s">
-        <v>802</v>
-      </c>
-      <c r="H98" s="30">
         <v>1</v>
       </c>
+    </row>
+    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H98" s="31"/>
+      <c r="I98" s="31"/>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H99" s="31"/>
@@ -9478,11 +9450,11 @@
       <c r="H109" s="31"/>
       <c r="I109" s="31"/>
     </row>
-    <row r="110" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:9" ht="409.6" x14ac:dyDescent="0">
       <c r="H110" s="31"/>
       <c r="I110" s="31"/>
     </row>
-    <row r="111" spans="2:9" ht="409.6" x14ac:dyDescent="0">
+    <row r="111" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H111" s="31"/>
       <c r="I111" s="31"/>
     </row>
@@ -9834,12 +9806,8 @@
       <c r="H198" s="31"/>
       <c r="I198" s="31"/>
     </row>
-    <row r="199" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H199" s="31"/>
-      <c r="I199" s="31"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A2:Z126"/>
+  <autoFilter ref="A2:Z125"/>
   <mergeCells count="1">
     <mergeCell ref="T1:Y1"/>
   </mergeCells>
@@ -10084,7 +10052,7 @@
       </c>
       <c r="B8" s="30"/>
       <c r="C8" s="30" t="s">
-        <v>814</v>
+        <v>808</v>
       </c>
       <c r="D8" s="30" t="s">
         <v>708</v>
@@ -10112,7 +10080,7 @@
       </c>
       <c r="B9" s="30"/>
       <c r="C9" s="30" t="s">
-        <v>815</v>
+        <v>809</v>
       </c>
       <c r="D9" s="30" t="s">
         <v>710</v>
@@ -10140,7 +10108,7 @@
       </c>
       <c r="B10" s="30"/>
       <c r="C10" s="30" t="s">
-        <v>816</v>
+        <v>810</v>
       </c>
       <c r="D10" s="30" t="s">
         <v>708</v>
@@ -10168,7 +10136,7 @@
       </c>
       <c r="B11" s="30"/>
       <c r="C11" s="30" t="s">
-        <v>817</v>
+        <v>811</v>
       </c>
       <c r="D11" s="30" t="s">
         <v>708</v>
@@ -10196,7 +10164,7 @@
       </c>
       <c r="B12" s="30"/>
       <c r="C12" s="30" t="s">
-        <v>818</v>
+        <v>812</v>
       </c>
       <c r="D12" s="30" t="s">
         <v>708</v>
@@ -10224,7 +10192,7 @@
       </c>
       <c r="B13" s="30"/>
       <c r="C13" s="30" t="s">
-        <v>819</v>
+        <v>813</v>
       </c>
       <c r="D13" s="30" t="s">
         <v>708</v>
@@ -10252,7 +10220,7 @@
       </c>
       <c r="B14" s="30"/>
       <c r="C14" s="30" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="D14" s="30" t="s">
         <v>708</v>
@@ -10280,7 +10248,7 @@
       </c>
       <c r="B15" s="30"/>
       <c r="C15" s="30" t="s">
-        <v>821</v>
+        <v>815</v>
       </c>
       <c r="D15" s="30" t="s">
         <v>708</v>
@@ -10308,7 +10276,7 @@
       </c>
       <c r="B16" s="30"/>
       <c r="C16" s="30" t="s">
-        <v>822</v>
+        <v>816</v>
       </c>
       <c r="D16" s="30" t="s">
         <v>708</v>
@@ -10336,7 +10304,7 @@
       </c>
       <c r="B17" s="30"/>
       <c r="C17" s="30" t="s">
-        <v>823</v>
+        <v>817</v>
       </c>
       <c r="D17" s="30" t="s">
         <v>708</v>
@@ -10364,7 +10332,7 @@
       </c>
       <c r="B18" s="30"/>
       <c r="C18" s="30" t="s">
-        <v>824</v>
+        <v>818</v>
       </c>
       <c r="D18" s="30" t="s">
         <v>708</v>
@@ -10392,7 +10360,7 @@
       </c>
       <c r="B19" s="30"/>
       <c r="C19" s="30" t="s">
-        <v>825</v>
+        <v>819</v>
       </c>
       <c r="D19" s="30" t="s">
         <v>708</v>
@@ -10420,7 +10388,7 @@
       </c>
       <c r="B20" s="30"/>
       <c r="C20" s="30" t="s">
-        <v>826</v>
+        <v>820</v>
       </c>
       <c r="D20" s="30" t="s">
         <v>708</v>
@@ -10448,7 +10416,7 @@
       </c>
       <c r="B21" s="30"/>
       <c r="C21" s="30" t="s">
-        <v>827</v>
+        <v>821</v>
       </c>
       <c r="D21" s="30" t="s">
         <v>724</v>
@@ -10476,7 +10444,7 @@
       </c>
       <c r="B22" s="30"/>
       <c r="C22" s="30" t="s">
-        <v>828</v>
+        <v>822</v>
       </c>
       <c r="D22" s="30" t="s">
         <v>724</v>
@@ -10504,7 +10472,7 @@
       </c>
       <c r="B23" s="30"/>
       <c r="C23" s="30" t="s">
-        <v>829</v>
+        <v>823</v>
       </c>
       <c r="D23" s="30" t="s">
         <v>724</v>
@@ -10532,7 +10500,7 @@
       </c>
       <c r="B24" s="30"/>
       <c r="C24" s="30" t="s">
-        <v>830</v>
+        <v>824</v>
       </c>
       <c r="D24" s="30" t="s">
         <v>724</v>
@@ -10560,7 +10528,7 @@
       </c>
       <c r="B25" s="30"/>
       <c r="C25" s="30" t="s">
-        <v>831</v>
+        <v>825</v>
       </c>
       <c r="D25" s="30" t="s">
         <v>724</v>
@@ -10588,7 +10556,7 @@
       </c>
       <c r="B26" s="30"/>
       <c r="C26" s="30" t="s">
-        <v>832</v>
+        <v>826</v>
       </c>
       <c r="D26" s="30" t="s">
         <v>724</v>
@@ -10616,7 +10584,7 @@
       </c>
       <c r="B27" s="30"/>
       <c r="C27" s="30" t="s">
-        <v>833</v>
+        <v>827</v>
       </c>
       <c r="D27" s="30" t="s">
         <v>724</v>
@@ -10644,7 +10612,7 @@
       </c>
       <c r="B28" s="30"/>
       <c r="C28" s="30" t="s">
-        <v>834</v>
+        <v>828</v>
       </c>
       <c r="D28" s="30" t="s">
         <v>724</v>
@@ -10672,7 +10640,7 @@
       </c>
       <c r="B29" s="30"/>
       <c r="C29" s="30" t="s">
-        <v>835</v>
+        <v>829</v>
       </c>
       <c r="D29" s="30" t="s">
         <v>724</v>
@@ -10700,7 +10668,7 @@
       </c>
       <c r="B30" s="30"/>
       <c r="C30" s="30" t="s">
-        <v>836</v>
+        <v>830</v>
       </c>
       <c r="D30" s="30" t="s">
         <v>724</v>

</xml_diff>

<commit_message>
Updated office_ee.xlsx to use existing measures
This adds EE for DCV and Economizers. I know National grid just wants a
specific economizer type, but I'm not sure which one. For now I used
FixedEnthalpy.
</commit_message>
<xml_diff>
--- a/projects/office_ee.xlsx
+++ b/projects/office_ee.xlsx
@@ -16,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$125</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$130</definedName>
     <definedName name="AnalysisType">Lookups!$A$17:$A$23</definedName>
     <definedName name="instance_defs">Lookups!$A$2:$D$9</definedName>
     <definedName name="instance_types">Lookups!$A$2:$A$9</definedName>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2568" uniqueCount="835">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2686" uniqueCount="852">
   <si>
     <t>type</t>
   </si>
@@ -2546,6 +2546,57 @@
   </si>
   <si>
     <t>Add Sys 3 - PSZ-AC Ngrid</t>
+  </si>
+  <si>
+    <t>Choose an Air Loop to Alter</t>
+  </si>
+  <si>
+    <t>Remove Baseline Costs From Effected AirLoopHVACOutdoorAirSystems</t>
+  </si>
+  <si>
+    <t>Material and Installation Costs per Air Loop to Enable Demand Controlled Ventilation</t>
+  </si>
+  <si>
+    <t>Demolition Costs per Air Loop to Enable Demand Controlled Ventilation</t>
+  </si>
+  <si>
+    <t>FixedEnthalpy</t>
+  </si>
+  <si>
+    <t>|FixedDryBulb,FixedEnthalpy,DifferentialDryBulb,DifferentialEnthalpy,FixedDewPointAndDryBulb,NoEconomizer|</t>
+  </si>
+  <si>
+    <t>Economizer Control Type</t>
+  </si>
+  <si>
+    <t>Economizer Maximum Limit Dry-Bulb Temperature</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Btu/lb</t>
+  </si>
+  <si>
+    <t>Economizer Maximum Enthalpy</t>
+  </si>
+  <si>
+    <t>Economizer Maximum Limit Dewpoint Temperature</t>
+  </si>
+  <si>
+    <t>Economizer Minimum Limit Dry-Bulb Temperature</t>
+  </si>
+  <si>
+    <t>Material and Installation Costs per Air Loop to Enable Economizer</t>
+  </si>
+  <si>
+    <t>Demolition Costs per Air Loop to Enable Economizer</t>
+  </si>
+  <si>
+    <t>O &amp; M Costs per Air Loop for Economizer</t>
+  </si>
+  <si>
+    <t>O &amp; M Costs per Air Loop for Demand Controlled Ventilation</t>
   </si>
 </sst>
 </file>
@@ -7225,11 +7276,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y198"/>
+  <dimension ref="A1:Y203"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
+      <pane ySplit="3" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9382,7 +9433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="2:9" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B97" s="30" t="s">
         <v>21</v>
       </c>
@@ -9402,127 +9453,533 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H98" s="31"/>
-      <c r="I98" s="31"/>
-    </row>
-    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H99" s="31"/>
-      <c r="I99" s="31"/>
-    </row>
-    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H100" s="31"/>
+    <row r="98" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="B98" s="49" t="s">
+        <v>209</v>
+      </c>
+      <c r="C98" s="49" t="s">
+        <v>210</v>
+      </c>
+      <c r="D98" s="49" t="s">
+        <v>210</v>
+      </c>
+      <c r="E98" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="J98" s="50"/>
+      <c r="K98" s="51"/>
+      <c r="L98" s="51"/>
+      <c r="M98" s="51"/>
+      <c r="N98" s="51"/>
+      <c r="O98" s="51"/>
+      <c r="Q98" s="52"/>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B99" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D99" s="31" t="s">
+        <v>835</v>
+      </c>
+      <c r="E99" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="F99" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="H99" s="31" t="s">
+        <v>417</v>
+      </c>
+      <c r="I99" s="30" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B100" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D100" s="31" t="s">
+        <v>836</v>
+      </c>
+      <c r="E100" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="F100" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="H100" s="31" t="b">
+        <v>0</v>
+      </c>
       <c r="I100" s="31"/>
     </row>
-    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H101" s="31"/>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B101" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D101" s="31" t="s">
+        <v>837</v>
+      </c>
+      <c r="E101" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="F101" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="H101" s="31">
+        <v>0</v>
+      </c>
       <c r="I101" s="31"/>
     </row>
-    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H102" s="31"/>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B102" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D102" s="31" t="s">
+        <v>838</v>
+      </c>
+      <c r="E102" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="F102" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="H102" s="31">
+        <v>0</v>
+      </c>
       <c r="I102" s="31"/>
     </row>
-    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H103" s="31"/>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B103" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D103" s="31" t="s">
+        <v>795</v>
+      </c>
+      <c r="E103" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="F103" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G103" s="30" t="s">
+        <v>796</v>
+      </c>
+      <c r="H103" s="31">
+        <v>0</v>
+      </c>
       <c r="I103" s="31"/>
     </row>
-    <row r="104" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H104" s="31"/>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B104" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D104" s="31" t="s">
+        <v>797</v>
+      </c>
+      <c r="E104" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="F104" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="G104" s="30"/>
+      <c r="H104" s="31" t="b">
+        <v>0</v>
+      </c>
       <c r="I104" s="31"/>
     </row>
-    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H105" s="31"/>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B105" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D105" s="30" t="s">
+        <v>798</v>
+      </c>
+      <c r="E105" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F105" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G105" s="30" t="s">
+        <v>796</v>
+      </c>
+      <c r="H105" s="31">
+        <v>15</v>
+      </c>
       <c r="I105" s="31"/>
     </row>
-    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H106" s="31"/>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B106" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D106" s="30" t="s">
+        <v>851</v>
+      </c>
+      <c r="E106" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F106" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G106" s="30" t="s">
+        <v>792</v>
+      </c>
+      <c r="H106" s="31">
+        <v>0</v>
+      </c>
       <c r="I106" s="31"/>
     </row>
-    <row r="107" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H107" s="31"/>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B107" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D107" s="30" t="s">
+        <v>800</v>
+      </c>
+      <c r="E107" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="F107" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G107" s="30" t="s">
+        <v>796</v>
+      </c>
+      <c r="H107" s="31">
+        <v>1</v>
+      </c>
       <c r="I107" s="31"/>
     </row>
-    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H108" s="31"/>
-      <c r="I108" s="31"/>
-    </row>
-    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H109" s="31"/>
-      <c r="I109" s="31"/>
-    </row>
-    <row r="110" spans="2:9" ht="409.6" x14ac:dyDescent="0">
-      <c r="H110" s="31"/>
-      <c r="I110" s="31"/>
-    </row>
-    <row r="111" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H111" s="31"/>
+    <row r="108" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="B108" s="49" t="s">
+        <v>216</v>
+      </c>
+      <c r="C108" s="49" t="s">
+        <v>217</v>
+      </c>
+      <c r="D108" s="49" t="s">
+        <v>217</v>
+      </c>
+      <c r="E108" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="J108" s="50"/>
+      <c r="K108" s="51"/>
+      <c r="L108" s="51"/>
+      <c r="M108" s="51"/>
+      <c r="N108" s="51"/>
+      <c r="O108" s="51"/>
+      <c r="Q108" s="52"/>
+    </row>
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B109" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D109" s="31" t="s">
+        <v>835</v>
+      </c>
+      <c r="E109" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="F109" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="H109" s="31" t="s">
+        <v>417</v>
+      </c>
+      <c r="I109" s="30" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B110" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D110" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="E110" s="31" t="s">
+        <v>219</v>
+      </c>
+      <c r="F110" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="H110" s="31" t="s">
+        <v>839</v>
+      </c>
+      <c r="I110" s="30" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B111" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D111" s="31" t="s">
+        <v>842</v>
+      </c>
+      <c r="E111" s="31" t="s">
+        <v>221</v>
+      </c>
+      <c r="F111" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G111" s="31" t="s">
+        <v>843</v>
+      </c>
+      <c r="H111" s="31">
+        <v>69</v>
+      </c>
       <c r="I111" s="31"/>
     </row>
-    <row r="112" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H112" s="31"/>
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B112" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D112" s="31" t="s">
+        <v>845</v>
+      </c>
+      <c r="E112" s="31" t="s">
+        <v>223</v>
+      </c>
+      <c r="F112" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G112" s="31" t="s">
+        <v>844</v>
+      </c>
+      <c r="H112" s="31">
+        <v>28</v>
+      </c>
       <c r="I112" s="31"/>
     </row>
-    <row r="113" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H113" s="31"/>
+    <row r="113" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B113" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D113" s="31" t="s">
+        <v>846</v>
+      </c>
+      <c r="E113" s="31" t="s">
+        <v>225</v>
+      </c>
+      <c r="F113" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G113" s="31" t="s">
+        <v>843</v>
+      </c>
+      <c r="H113" s="31">
+        <v>55</v>
+      </c>
       <c r="I113" s="31"/>
     </row>
-    <row r="114" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H114" s="31"/>
+    <row r="114" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B114" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D114" s="31" t="s">
+        <v>847</v>
+      </c>
+      <c r="E114" s="31" t="s">
+        <v>227</v>
+      </c>
+      <c r="F114" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G114" s="31" t="s">
+        <v>843</v>
+      </c>
+      <c r="H114" s="31">
+        <v>-148</v>
+      </c>
       <c r="I114" s="31"/>
     </row>
-    <row r="115" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H115" s="31"/>
+    <row r="115" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B115" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D115" s="31" t="s">
+        <v>836</v>
+      </c>
+      <c r="E115" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="F115" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="H115" s="31" t="b">
+        <v>0</v>
+      </c>
       <c r="I115" s="31"/>
     </row>
-    <row r="116" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H116" s="31"/>
+    <row r="116" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B116" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D116" s="31" t="s">
+        <v>848</v>
+      </c>
+      <c r="E116" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="F116" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="H116" s="31">
+        <v>0</v>
+      </c>
       <c r="I116" s="31"/>
     </row>
-    <row r="117" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H117" s="31"/>
+    <row r="117" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B117" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D117" s="31" t="s">
+        <v>849</v>
+      </c>
+      <c r="E117" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="F117" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="H117" s="31">
+        <v>0</v>
+      </c>
       <c r="I117" s="31"/>
     </row>
-    <row r="118" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H118" s="31"/>
+    <row r="118" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B118" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D118" s="31" t="s">
+        <v>795</v>
+      </c>
+      <c r="E118" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="F118" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G118" s="30" t="s">
+        <v>796</v>
+      </c>
+      <c r="H118" s="31">
+        <v>0</v>
+      </c>
       <c r="I118" s="31"/>
     </row>
-    <row r="119" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H119" s="31"/>
+    <row r="119" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B119" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D119" s="31" t="s">
+        <v>797</v>
+      </c>
+      <c r="E119" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="F119" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="G119" s="30"/>
+      <c r="H119" s="31" t="b">
+        <v>0</v>
+      </c>
       <c r="I119" s="31"/>
     </row>
-    <row r="120" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H120" s="31"/>
+    <row r="120" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B120" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D120" s="30" t="s">
+        <v>798</v>
+      </c>
+      <c r="E120" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F120" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G120" s="30" t="s">
+        <v>796</v>
+      </c>
+      <c r="H120" s="31">
+        <v>15</v>
+      </c>
       <c r="I120" s="31"/>
     </row>
-    <row r="121" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H121" s="31"/>
+    <row r="121" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B121" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D121" s="30" t="s">
+        <v>850</v>
+      </c>
+      <c r="E121" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F121" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G121" s="30" t="s">
+        <v>792</v>
+      </c>
+      <c r="H121" s="31">
+        <v>0</v>
+      </c>
       <c r="I121" s="31"/>
     </row>
-    <row r="122" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H122" s="31"/>
+    <row r="122" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B122" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D122" s="30" t="s">
+        <v>800</v>
+      </c>
+      <c r="E122" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="F122" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G122" s="30" t="s">
+        <v>796</v>
+      </c>
+      <c r="H122" s="31">
+        <v>1</v>
+      </c>
       <c r="I122" s="31"/>
     </row>
-    <row r="123" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H123" s="31"/>
       <c r="I123" s="31"/>
     </row>
-    <row r="124" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H124" s="31"/>
       <c r="I124" s="31"/>
     </row>
-    <row r="125" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H125" s="31"/>
       <c r="I125" s="31"/>
     </row>
-    <row r="126" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H126" s="31"/>
       <c r="I126" s="31"/>
     </row>
-    <row r="127" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H127" s="31"/>
       <c r="I127" s="31"/>
     </row>
-    <row r="128" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H128" s="31"/>
       <c r="I128" s="31"/>
     </row>
@@ -9806,8 +10263,28 @@
       <c r="H198" s="31"/>
       <c r="I198" s="31"/>
     </row>
+    <row r="199" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H199" s="31"/>
+      <c r="I199" s="31"/>
+    </row>
+    <row r="200" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H200" s="31"/>
+      <c r="I200" s="31"/>
+    </row>
+    <row r="201" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H201" s="31"/>
+      <c r="I201" s="31"/>
+    </row>
+    <row r="202" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H202" s="31"/>
+      <c r="I202" s="31"/>
+    </row>
+    <row r="203" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H203" s="31"/>
+      <c r="I203" s="31"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:Z125"/>
+  <autoFilter ref="A2:Z130"/>
   <mergeCells count="1">
     <mergeCell ref="T1:Y1"/>
   </mergeCells>

</xml_diff>

<commit_message>
Updating office_ee.xlsx to run full year after calibration
The run period was set to less than a year for calibration. This hooks
up measure I wrote on Friday to change it back to fully year. All
measures added tonight have been tested through server workflow, and in
most cases model has been inspected to confirm changes.
</commit_message>
<xml_diff>
--- a/projects/office_ee.xlsx
+++ b/projects/office_ee.xlsx
@@ -16,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$130</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$135</definedName>
     <definedName name="AnalysisType">Lookups!$A$17:$A$23</definedName>
     <definedName name="instance_defs">Lookups!$A$2:$D$9</definedName>
     <definedName name="instance_types">Lookups!$A$2:$A$9</definedName>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2686" uniqueCount="852">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2710" uniqueCount="864">
   <si>
     <t>type</t>
   </si>
@@ -2597,6 +2597,42 @@
   </si>
   <si>
     <t>O &amp; M Costs per Air Loop for Demand Controlled Ventilation</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>SetRunPeriod</t>
+  </si>
+  <si>
+    <t>Set Run Period</t>
+  </si>
+  <si>
+    <t>begin_month</t>
+  </si>
+  <si>
+    <t>begin_day</t>
+  </si>
+  <si>
+    <t>end_month</t>
+  </si>
+  <si>
+    <t>end_day</t>
+  </si>
+  <si>
+    <t>Begin Month</t>
+  </si>
+  <si>
+    <t>Begin Day</t>
+  </si>
+  <si>
+    <t>End Month</t>
+  </si>
+  <si>
+    <t>End Day</t>
   </si>
 </sst>
 </file>
@@ -7276,11 +7312,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y203"/>
+  <dimension ref="A1:Y208"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C104" sqref="C104"/>
+      <pane ySplit="3" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E89" sqref="E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9196,13 +9232,13 @@
         <v>1</v>
       </c>
       <c r="B86" s="49" t="s">
-        <v>804</v>
+        <v>855</v>
       </c>
       <c r="C86" s="49" t="s">
-        <v>803</v>
+        <v>854</v>
       </c>
       <c r="D86" s="49" t="s">
-        <v>803</v>
+        <v>854</v>
       </c>
       <c r="E86" s="49" t="s">
         <v>68</v>
@@ -9215,45 +9251,46 @@
       <c r="O86" s="51"/>
       <c r="Q86" s="52"/>
     </row>
-    <row r="87" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="49" t="b">
+    <row r="87" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="18"/>
+      <c r="B87" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D87" s="30" t="s">
+        <v>860</v>
+      </c>
+      <c r="E87" s="30" t="s">
+        <v>856</v>
+      </c>
+      <c r="F87" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G87" s="30" t="s">
+        <v>852</v>
+      </c>
+      <c r="H87" s="30">
         <v>1</v>
       </c>
-      <c r="B87" s="49" t="s">
-        <v>832</v>
-      </c>
-      <c r="C87" s="49" t="s">
-        <v>831</v>
-      </c>
-      <c r="D87" s="49" t="s">
-        <v>831</v>
-      </c>
-      <c r="E87" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="J87" s="50"/>
-      <c r="K87" s="51"/>
-      <c r="L87" s="51"/>
-      <c r="M87" s="51"/>
-      <c r="N87" s="51"/>
-      <c r="O87" s="51"/>
-      <c r="Q87" s="52"/>
-    </row>
-    <row r="88" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="22" t="b">
+    </row>
+    <row r="88" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="18"/>
+      <c r="B88" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D88" s="30" t="s">
+        <v>861</v>
+      </c>
+      <c r="E88" s="30" t="s">
+        <v>857</v>
+      </c>
+      <c r="F88" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G88" s="30" t="s">
+        <v>853</v>
+      </c>
+      <c r="H88" s="30">
         <v>1</v>
-      </c>
-      <c r="B88" s="22" t="s">
-        <v>801</v>
-      </c>
-      <c r="C88" s="22" t="s">
-        <v>286</v>
-      </c>
-      <c r="D88" s="22" t="s">
-        <v>286</v>
-      </c>
-      <c r="E88" s="22" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="89" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -9262,155 +9299,165 @@
         <v>21</v>
       </c>
       <c r="D89" s="30" t="s">
+        <v>862</v>
+      </c>
+      <c r="E89" s="30" t="s">
+        <v>858</v>
+      </c>
+      <c r="F89" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G89" s="30" t="s">
+        <v>852</v>
+      </c>
+      <c r="H89" s="30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="18"/>
+      <c r="B90" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D90" s="30" t="s">
+        <v>863</v>
+      </c>
+      <c r="E90" s="30" t="s">
+        <v>859</v>
+      </c>
+      <c r="F90" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G90" s="30" t="s">
+        <v>853</v>
+      </c>
+      <c r="H90" s="30">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="B91" s="49" t="s">
+        <v>804</v>
+      </c>
+      <c r="C91" s="49" t="s">
+        <v>803</v>
+      </c>
+      <c r="D91" s="49" t="s">
+        <v>803</v>
+      </c>
+      <c r="E91" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="J91" s="50"/>
+      <c r="K91" s="51"/>
+      <c r="L91" s="51"/>
+      <c r="M91" s="51"/>
+      <c r="N91" s="51"/>
+      <c r="O91" s="51"/>
+      <c r="Q91" s="52"/>
+    </row>
+    <row r="92" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="B92" s="49" t="s">
+        <v>832</v>
+      </c>
+      <c r="C92" s="49" t="s">
+        <v>831</v>
+      </c>
+      <c r="D92" s="49" t="s">
+        <v>831</v>
+      </c>
+      <c r="E92" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="J92" s="50"/>
+      <c r="K92" s="51"/>
+      <c r="L92" s="51"/>
+      <c r="M92" s="51"/>
+      <c r="N92" s="51"/>
+      <c r="O92" s="51"/>
+      <c r="Q92" s="52"/>
+    </row>
+    <row r="93" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="B93" s="22" t="s">
+        <v>801</v>
+      </c>
+      <c r="C93" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="D93" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="E93" s="22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="18"/>
+      <c r="B94" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D94" s="30" t="s">
         <v>373</v>
       </c>
-      <c r="E89" s="30" t="s">
+      <c r="E94" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="F89" s="30" t="s">
+      <c r="F94" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="H89" s="30" t="s">
+      <c r="H94" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="I89" s="30" t="s">
+      <c r="I94" s="30" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="90" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="43" t="s">
+    <row r="95" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B95" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="D90" s="43" t="s">
+      <c r="D95" s="43" t="s">
         <v>802</v>
       </c>
-      <c r="E90" s="43" t="s">
+      <c r="E95" s="43" t="s">
         <v>288</v>
       </c>
-      <c r="F90" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="G90" s="43" t="s">
+      <c r="F95" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="G95" s="43" t="s">
         <v>792</v>
       </c>
-      <c r="H90" s="43">
-        <v>0</v>
-      </c>
-      <c r="J90" s="43">
-        <v>0</v>
-      </c>
-      <c r="K90" s="43">
+      <c r="H95" s="43">
+        <v>0</v>
+      </c>
+      <c r="J95" s="43">
+        <v>0</v>
+      </c>
+      <c r="K95" s="43">
         <v>40</v>
       </c>
-      <c r="L90" s="43">
+      <c r="L95" s="43">
         <v>-1</v>
       </c>
-      <c r="M90" s="45">
-        <f>(K90-J90)/6</f>
+      <c r="M95" s="45">
+        <f>(K95-J95)/6</f>
         <v>6.666666666666667</v>
       </c>
-      <c r="N90" s="45">
+      <c r="N95" s="45">
         <v>2.5</v>
       </c>
-      <c r="Q90" s="43" t="s">
+      <c r="Q95" s="43" t="s">
         <v>777</v>
-      </c>
-    </row>
-    <row r="91" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D91" s="30" t="s">
-        <v>793</v>
-      </c>
-      <c r="E91" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="F91" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G91" s="30" t="s">
-        <v>792</v>
-      </c>
-      <c r="H91" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B92" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D92" s="30" t="s">
-        <v>794</v>
-      </c>
-      <c r="E92" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="F92" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G92" s="30" t="s">
-        <v>792</v>
-      </c>
-      <c r="H92" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D93" s="30" t="s">
-        <v>795</v>
-      </c>
-      <c r="E93" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="F93" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G93" s="30" t="s">
-        <v>796</v>
-      </c>
-      <c r="H93" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D94" s="30" t="s">
-        <v>797</v>
-      </c>
-      <c r="E94" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="F94" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="H94" s="30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D95" s="30" t="s">
-        <v>798</v>
-      </c>
-      <c r="E95" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="F95" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G95" s="30" t="s">
-        <v>796</v>
-      </c>
-      <c r="H95" s="30">
-        <v>15</v>
       </c>
     </row>
     <row r="96" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -9418,10 +9465,10 @@
         <v>21</v>
       </c>
       <c r="D96" s="30" t="s">
-        <v>799</v>
+        <v>793</v>
       </c>
       <c r="E96" s="30" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="F96" s="30" t="s">
         <v>64</v>
@@ -9438,177 +9485,177 @@
         <v>21</v>
       </c>
       <c r="D97" s="30" t="s">
+        <v>794</v>
+      </c>
+      <c r="E97" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="F97" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G97" s="30" t="s">
+        <v>792</v>
+      </c>
+      <c r="H97" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B98" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D98" s="30" t="s">
+        <v>795</v>
+      </c>
+      <c r="E98" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="F98" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G98" s="30" t="s">
+        <v>796</v>
+      </c>
+      <c r="H98" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B99" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D99" s="30" t="s">
+        <v>797</v>
+      </c>
+      <c r="E99" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="F99" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="H99" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B100" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D100" s="30" t="s">
+        <v>798</v>
+      </c>
+      <c r="E100" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F100" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G100" s="30" t="s">
+        <v>796</v>
+      </c>
+      <c r="H100" s="30">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B101" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D101" s="30" t="s">
+        <v>799</v>
+      </c>
+      <c r="E101" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F101" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G101" s="30" t="s">
+        <v>792</v>
+      </c>
+      <c r="H101" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B102" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D102" s="30" t="s">
         <v>800</v>
       </c>
-      <c r="E97" s="30" t="s">
+      <c r="E102" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="F97" s="30" t="s">
+      <c r="F102" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="G97" s="30" t="s">
+      <c r="G102" s="30" t="s">
         <v>796</v>
       </c>
-      <c r="H97" s="30">
+      <c r="H102" s="30">
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="49" t="b">
+    <row r="103" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="49" t="b">
         <v>1</v>
       </c>
-      <c r="B98" s="49" t="s">
+      <c r="B103" s="49" t="s">
         <v>209</v>
       </c>
-      <c r="C98" s="49" t="s">
+      <c r="C103" s="49" t="s">
         <v>210</v>
       </c>
-      <c r="D98" s="49" t="s">
+      <c r="D103" s="49" t="s">
         <v>210</v>
       </c>
-      <c r="E98" s="49" t="s">
+      <c r="E103" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="J98" s="50"/>
-      <c r="K98" s="51"/>
-      <c r="L98" s="51"/>
-      <c r="M98" s="51"/>
-      <c r="N98" s="51"/>
-      <c r="O98" s="51"/>
-      <c r="Q98" s="52"/>
-    </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B99" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D99" s="31" t="s">
-        <v>835</v>
-      </c>
-      <c r="E99" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="F99" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H99" s="31" t="s">
-        <v>417</v>
-      </c>
-      <c r="I99" s="30" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B100" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D100" s="31" t="s">
-        <v>836</v>
-      </c>
-      <c r="E100" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="F100" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="H100" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="I100" s="31"/>
-    </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B101" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D101" s="31" t="s">
-        <v>837</v>
-      </c>
-      <c r="E101" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="F101" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="H101" s="31">
-        <v>0</v>
-      </c>
-      <c r="I101" s="31"/>
-    </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B102" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D102" s="31" t="s">
-        <v>838</v>
-      </c>
-      <c r="E102" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="F102" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="H102" s="31">
-        <v>0</v>
-      </c>
-      <c r="I102" s="31"/>
-    </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B103" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D103" s="31" t="s">
-        <v>795</v>
-      </c>
-      <c r="E103" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="F103" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G103" s="30" t="s">
-        <v>796</v>
-      </c>
-      <c r="H103" s="31">
-        <v>0</v>
-      </c>
-      <c r="I103" s="31"/>
+      <c r="J103" s="50"/>
+      <c r="K103" s="51"/>
+      <c r="L103" s="51"/>
+      <c r="M103" s="51"/>
+      <c r="N103" s="51"/>
+      <c r="O103" s="51"/>
+      <c r="Q103" s="52"/>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B104" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D104" s="31" t="s">
-        <v>797</v>
+        <v>835</v>
       </c>
       <c r="E104" s="31" t="s">
-        <v>54</v>
+        <v>126</v>
       </c>
       <c r="F104" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="G104" s="30"/>
-      <c r="H104" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="I104" s="31"/>
+        <v>62</v>
+      </c>
+      <c r="H104" s="31" t="s">
+        <v>417</v>
+      </c>
+      <c r="I104" s="30" t="s">
+        <v>418</v>
+      </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B105" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D105" s="30" t="s">
-        <v>798</v>
-      </c>
-      <c r="E105" s="30" t="s">
-        <v>56</v>
+      <c r="D105" s="31" t="s">
+        <v>836</v>
+      </c>
+      <c r="E105" s="31" t="s">
+        <v>91</v>
       </c>
       <c r="F105" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G105" s="30" t="s">
-        <v>796</v>
-      </c>
-      <c r="H105" s="31">
-        <v>15</v>
+        <v>63</v>
+      </c>
+      <c r="H105" s="31" t="b">
+        <v>0</v>
       </c>
       <c r="I105" s="31"/>
     </row>
@@ -9616,17 +9663,14 @@
       <c r="B106" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D106" s="30" t="s">
-        <v>851</v>
-      </c>
-      <c r="E106" s="30" t="s">
-        <v>58</v>
+      <c r="D106" s="31" t="s">
+        <v>837</v>
+      </c>
+      <c r="E106" s="31" t="s">
+        <v>128</v>
       </c>
       <c r="F106" s="30" t="s">
         <v>64</v>
-      </c>
-      <c r="G106" s="30" t="s">
-        <v>792</v>
       </c>
       <c r="H106" s="31">
         <v>0</v>
@@ -9637,105 +9681,99 @@
       <c r="B107" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D107" s="30" t="s">
-        <v>800</v>
-      </c>
-      <c r="E107" s="30" t="s">
-        <v>60</v>
+      <c r="D107" s="31" t="s">
+        <v>838</v>
+      </c>
+      <c r="E107" s="31" t="s">
+        <v>50</v>
       </c>
       <c r="F107" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="H107" s="31">
+        <v>0</v>
+      </c>
+      <c r="I107" s="31"/>
+    </row>
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B108" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D108" s="31" t="s">
+        <v>795</v>
+      </c>
+      <c r="E108" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="F108" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="G107" s="30" t="s">
+      <c r="G108" s="30" t="s">
         <v>796</v>
       </c>
-      <c r="H107" s="31">
-        <v>1</v>
-      </c>
-      <c r="I107" s="31"/>
-    </row>
-    <row r="108" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B108" s="49" t="s">
-        <v>216</v>
-      </c>
-      <c r="C108" s="49" t="s">
-        <v>217</v>
-      </c>
-      <c r="D108" s="49" t="s">
-        <v>217</v>
-      </c>
-      <c r="E108" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="J108" s="50"/>
-      <c r="K108" s="51"/>
-      <c r="L108" s="51"/>
-      <c r="M108" s="51"/>
-      <c r="N108" s="51"/>
-      <c r="O108" s="51"/>
-      <c r="Q108" s="52"/>
+      <c r="H108" s="31">
+        <v>0</v>
+      </c>
+      <c r="I108" s="31"/>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B109" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D109" s="31" t="s">
-        <v>835</v>
+        <v>797</v>
       </c>
       <c r="E109" s="31" t="s">
-        <v>126</v>
+        <v>54</v>
       </c>
       <c r="F109" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H109" s="31" t="s">
-        <v>417</v>
-      </c>
-      <c r="I109" s="30" t="s">
-        <v>418</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="G109" s="30"/>
+      <c r="H109" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I109" s="31"/>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B110" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D110" s="31" t="s">
-        <v>841</v>
-      </c>
-      <c r="E110" s="31" t="s">
-        <v>219</v>
+      <c r="D110" s="30" t="s">
+        <v>798</v>
+      </c>
+      <c r="E110" s="30" t="s">
+        <v>56</v>
       </c>
       <c r="F110" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H110" s="31" t="s">
-        <v>839</v>
-      </c>
-      <c r="I110" s="30" t="s">
-        <v>840</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="G110" s="30" t="s">
+        <v>796</v>
+      </c>
+      <c r="H110" s="31">
+        <v>15</v>
+      </c>
+      <c r="I110" s="31"/>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B111" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D111" s="31" t="s">
-        <v>842</v>
-      </c>
-      <c r="E111" s="31" t="s">
-        <v>221</v>
+      <c r="D111" s="30" t="s">
+        <v>851</v>
+      </c>
+      <c r="E111" s="30" t="s">
+        <v>58</v>
       </c>
       <c r="F111" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="G111" s="31" t="s">
-        <v>843</v>
+      <c r="G111" s="30" t="s">
+        <v>792</v>
       </c>
       <c r="H111" s="31">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="I111" s="31"/>
     </row>
@@ -9743,243 +9781,329 @@
       <c r="B112" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D112" s="31" t="s">
+      <c r="D112" s="30" t="s">
+        <v>800</v>
+      </c>
+      <c r="E112" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="F112" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G112" s="30" t="s">
+        <v>796</v>
+      </c>
+      <c r="H112" s="31">
+        <v>1</v>
+      </c>
+      <c r="I112" s="31"/>
+    </row>
+    <row r="113" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="B113" s="49" t="s">
+        <v>216</v>
+      </c>
+      <c r="C113" s="49" t="s">
+        <v>217</v>
+      </c>
+      <c r="D113" s="49" t="s">
+        <v>217</v>
+      </c>
+      <c r="E113" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="J113" s="50"/>
+      <c r="K113" s="51"/>
+      <c r="L113" s="51"/>
+      <c r="M113" s="51"/>
+      <c r="N113" s="51"/>
+      <c r="O113" s="51"/>
+      <c r="Q113" s="52"/>
+    </row>
+    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B114" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D114" s="31" t="s">
+        <v>835</v>
+      </c>
+      <c r="E114" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="F114" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="H114" s="31" t="s">
+        <v>417</v>
+      </c>
+      <c r="I114" s="30" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B115" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D115" s="31" t="s">
+        <v>841</v>
+      </c>
+      <c r="E115" s="31" t="s">
+        <v>219</v>
+      </c>
+      <c r="F115" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="H115" s="31" t="s">
+        <v>839</v>
+      </c>
+      <c r="I115" s="30" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B116" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D116" s="31" t="s">
+        <v>842</v>
+      </c>
+      <c r="E116" s="31" t="s">
+        <v>221</v>
+      </c>
+      <c r="F116" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G116" s="31" t="s">
+        <v>843</v>
+      </c>
+      <c r="H116" s="31">
+        <v>69</v>
+      </c>
+      <c r="I116" s="31"/>
+    </row>
+    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B117" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D117" s="31" t="s">
         <v>845</v>
       </c>
-      <c r="E112" s="31" t="s">
+      <c r="E117" s="31" t="s">
         <v>223</v>
       </c>
-      <c r="F112" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G112" s="31" t="s">
+      <c r="F117" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G117" s="31" t="s">
         <v>844</v>
       </c>
-      <c r="H112" s="31">
+      <c r="H117" s="31">
         <v>28</v>
       </c>
-      <c r="I112" s="31"/>
-    </row>
-    <row r="113" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B113" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D113" s="31" t="s">
+      <c r="I117" s="31"/>
+    </row>
+    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B118" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D118" s="31" t="s">
         <v>846</v>
       </c>
-      <c r="E113" s="31" t="s">
+      <c r="E118" s="31" t="s">
         <v>225</v>
       </c>
-      <c r="F113" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G113" s="31" t="s">
+      <c r="F118" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G118" s="31" t="s">
         <v>843</v>
       </c>
-      <c r="H113" s="31">
+      <c r="H118" s="31">
         <v>55</v>
       </c>
-      <c r="I113" s="31"/>
-    </row>
-    <row r="114" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B114" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D114" s="31" t="s">
+      <c r="I118" s="31"/>
+    </row>
+    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B119" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D119" s="31" t="s">
         <v>847</v>
       </c>
-      <c r="E114" s="31" t="s">
+      <c r="E119" s="31" t="s">
         <v>227</v>
       </c>
-      <c r="F114" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G114" s="31" t="s">
+      <c r="F119" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G119" s="31" t="s">
         <v>843</v>
       </c>
-      <c r="H114" s="31">
+      <c r="H119" s="31">
         <v>-148</v>
       </c>
-      <c r="I114" s="31"/>
-    </row>
-    <row r="115" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B115" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D115" s="31" t="s">
+      <c r="I119" s="31"/>
+    </row>
+    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B120" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D120" s="31" t="s">
         <v>836</v>
       </c>
-      <c r="E115" s="31" t="s">
+      <c r="E120" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="F115" s="30" t="s">
+      <c r="F120" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="H115" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="I115" s="31"/>
-    </row>
-    <row r="116" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B116" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D116" s="31" t="s">
+      <c r="H120" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I120" s="31"/>
+    </row>
+    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B121" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D121" s="31" t="s">
         <v>848</v>
       </c>
-      <c r="E116" s="31" t="s">
+      <c r="E121" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="F116" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="H116" s="31">
-        <v>0</v>
-      </c>
-      <c r="I116" s="31"/>
-    </row>
-    <row r="117" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B117" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D117" s="31" t="s">
+      <c r="F121" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="H121" s="31">
+        <v>0</v>
+      </c>
+      <c r="I121" s="31"/>
+    </row>
+    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B122" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D122" s="31" t="s">
         <v>849</v>
       </c>
-      <c r="E117" s="31" t="s">
+      <c r="E122" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="F117" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="H117" s="31">
-        <v>0</v>
-      </c>
-      <c r="I117" s="31"/>
-    </row>
-    <row r="118" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B118" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D118" s="31" t="s">
+      <c r="F122" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="H122" s="31">
+        <v>0</v>
+      </c>
+      <c r="I122" s="31"/>
+    </row>
+    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B123" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D123" s="31" t="s">
         <v>795</v>
       </c>
-      <c r="E118" s="31" t="s">
+      <c r="E123" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="F118" s="30" t="s">
+      <c r="F123" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="G118" s="30" t="s">
+      <c r="G123" s="30" t="s">
         <v>796</v>
       </c>
-      <c r="H118" s="31">
-        <v>0</v>
-      </c>
-      <c r="I118" s="31"/>
-    </row>
-    <row r="119" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B119" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D119" s="31" t="s">
+      <c r="H123" s="31">
+        <v>0</v>
+      </c>
+      <c r="I123" s="31"/>
+    </row>
+    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B124" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D124" s="31" t="s">
         <v>797</v>
       </c>
-      <c r="E119" s="31" t="s">
+      <c r="E124" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="F119" s="30" t="s">
+      <c r="F124" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="G119" s="30"/>
-      <c r="H119" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="I119" s="31"/>
-    </row>
-    <row r="120" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B120" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D120" s="30" t="s">
+      <c r="G124" s="30"/>
+      <c r="H124" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I124" s="31"/>
+    </row>
+    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B125" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D125" s="30" t="s">
         <v>798</v>
       </c>
-      <c r="E120" s="30" t="s">
+      <c r="E125" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="F120" s="30" t="s">
+      <c r="F125" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="G120" s="30" t="s">
+      <c r="G125" s="30" t="s">
         <v>796</v>
       </c>
-      <c r="H120" s="31">
+      <c r="H125" s="31">
         <v>15</v>
       </c>
-      <c r="I120" s="31"/>
-    </row>
-    <row r="121" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B121" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D121" s="30" t="s">
+      <c r="I125" s="31"/>
+    </row>
+    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B126" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D126" s="30" t="s">
         <v>850</v>
       </c>
-      <c r="E121" s="30" t="s">
+      <c r="E126" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="F121" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G121" s="30" t="s">
+      <c r="F126" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G126" s="30" t="s">
         <v>792</v>
       </c>
-      <c r="H121" s="31">
-        <v>0</v>
-      </c>
-      <c r="I121" s="31"/>
-    </row>
-    <row r="122" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B122" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D122" s="30" t="s">
+      <c r="H126" s="31">
+        <v>0</v>
+      </c>
+      <c r="I126" s="31"/>
+    </row>
+    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B127" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D127" s="30" t="s">
         <v>800</v>
       </c>
-      <c r="E122" s="30" t="s">
+      <c r="E127" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="F122" s="30" t="s">
+      <c r="F127" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="G122" s="30" t="s">
+      <c r="G127" s="30" t="s">
         <v>796</v>
       </c>
-      <c r="H122" s="31">
+      <c r="H127" s="31">
         <v>1</v>
       </c>
-      <c r="I122" s="31"/>
-    </row>
-    <row r="123" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H123" s="31"/>
-      <c r="I123" s="31"/>
-    </row>
-    <row r="124" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H124" s="31"/>
-      <c r="I124" s="31"/>
-    </row>
-    <row r="125" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H125" s="31"/>
-      <c r="I125" s="31"/>
-    </row>
-    <row r="126" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H126" s="31"/>
-      <c r="I126" s="31"/>
-    </row>
-    <row r="127" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H127" s="31"/>
       <c r="I127" s="31"/>
     </row>
-    <row r="128" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H128" s="31"/>
       <c r="I128" s="31"/>
     </row>
@@ -10283,8 +10407,28 @@
       <c r="H203" s="31"/>
       <c r="I203" s="31"/>
     </row>
+    <row r="204" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H204" s="31"/>
+      <c r="I204" s="31"/>
+    </row>
+    <row r="205" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H205" s="31"/>
+      <c r="I205" s="31"/>
+    </row>
+    <row r="206" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H206" s="31"/>
+      <c r="I206" s="31"/>
+    </row>
+    <row r="207" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H207" s="31"/>
+      <c r="I207" s="31"/>
+    </row>
+    <row r="208" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H208" s="31"/>
+      <c r="I208" s="31"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:Z130"/>
+  <autoFilter ref="A2:Z135"/>
   <mergeCells count="1">
     <mergeCell ref="T1:Y1"/>
   </mergeCells>

</xml_diff>

<commit_message>
Added Ventilation measure to office_ee.xlsx
Didn't have to alter measure. I matched reduce infiltration which
didn't' have any special machine readable attributes. Just has the
inputs.

I'm going to make new roof and wall R value measures that can provide
relative change vs. target R value.
</commit_message>
<xml_diff>
--- a/projects/office_ee.xlsx
+++ b/projects/office_ee.xlsx
@@ -16,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$135</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$138</definedName>
     <definedName name="AnalysisType">Lookups!$A$17:$A$23</definedName>
     <definedName name="instance_defs">Lookups!$A$2:$D$9</definedName>
     <definedName name="instance_types">Lookups!$A$2:$A$9</definedName>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2710" uniqueCount="864">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2725" uniqueCount="865">
   <si>
     <t>type</t>
   </si>
@@ -2633,6 +2633,9 @@
   </si>
   <si>
     <t>End Day</t>
+  </si>
+  <si>
+    <t>Design Specification Outdoor Air Reduction (%)</t>
   </si>
 </sst>
 </file>
@@ -7312,11 +7315,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y208"/>
+  <dimension ref="A1:Y211"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E89" sqref="E89"/>
+      <pane ySplit="3" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9227,92 +9230,114 @@
       <c r="N85" s="3"/>
       <c r="P85" s="40"/>
     </row>
-    <row r="86" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="49" t="b">
+    <row r="86" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="38" t="b">
         <v>1</v>
       </c>
-      <c r="B86" s="49" t="s">
+      <c r="B86" s="38" t="s">
+        <v>327</v>
+      </c>
+      <c r="C86" s="38" t="s">
+        <v>328</v>
+      </c>
+      <c r="D86" s="38" t="s">
+        <v>328</v>
+      </c>
+      <c r="E86" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="G86" s="39"/>
+      <c r="H86" s="39"/>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A87" s="30"/>
+      <c r="B87" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C87" s="30"/>
+      <c r="D87" s="30" t="s">
+        <v>373</v>
+      </c>
+      <c r="E87" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F87" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="G87" s="30"/>
+      <c r="H87" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="I87" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="J87" s="3"/>
+      <c r="K87" s="3"/>
+      <c r="L87" s="3"/>
+      <c r="M87" s="3"/>
+      <c r="N87" s="3"/>
+      <c r="P87" s="40"/>
+    </row>
+    <row r="88" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D88" s="43" t="s">
+        <v>864</v>
+      </c>
+      <c r="E88" s="43" t="s">
+        <v>330</v>
+      </c>
+      <c r="F88" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="H88" s="43">
+        <v>30</v>
+      </c>
+      <c r="I88" s="46"/>
+      <c r="J88" s="45">
+        <v>-100</v>
+      </c>
+      <c r="K88" s="45">
+        <v>100</v>
+      </c>
+      <c r="L88" s="45">
+        <v>0</v>
+      </c>
+      <c r="M88" s="45">
+        <f>(K88-J88)/6</f>
+        <v>33.333333333333336</v>
+      </c>
+      <c r="N88" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q88" s="43" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="B89" s="49" t="s">
         <v>855</v>
       </c>
-      <c r="C86" s="49" t="s">
+      <c r="C89" s="49" t="s">
         <v>854</v>
       </c>
-      <c r="D86" s="49" t="s">
+      <c r="D89" s="49" t="s">
         <v>854</v>
       </c>
-      <c r="E86" s="49" t="s">
+      <c r="E89" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="J86" s="50"/>
-      <c r="K86" s="51"/>
-      <c r="L86" s="51"/>
-      <c r="M86" s="51"/>
-      <c r="N86" s="51"/>
-      <c r="O86" s="51"/>
-      <c r="Q86" s="52"/>
-    </row>
-    <row r="87" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="18"/>
-      <c r="B87" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D87" s="30" t="s">
-        <v>860</v>
-      </c>
-      <c r="E87" s="30" t="s">
-        <v>856</v>
-      </c>
-      <c r="F87" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G87" s="30" t="s">
-        <v>852</v>
-      </c>
-      <c r="H87" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="18"/>
-      <c r="B88" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D88" s="30" t="s">
-        <v>861</v>
-      </c>
-      <c r="E88" s="30" t="s">
-        <v>857</v>
-      </c>
-      <c r="F88" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G88" s="30" t="s">
-        <v>853</v>
-      </c>
-      <c r="H88" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="18"/>
-      <c r="B89" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D89" s="30" t="s">
-        <v>862</v>
-      </c>
-      <c r="E89" s="30" t="s">
-        <v>858</v>
-      </c>
-      <c r="F89" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G89" s="30" t="s">
-        <v>852</v>
-      </c>
-      <c r="H89" s="30">
-        <v>12</v>
-      </c>
+      <c r="J89" s="50"/>
+      <c r="K89" s="51"/>
+      <c r="L89" s="51"/>
+      <c r="M89" s="51"/>
+      <c r="N89" s="51"/>
+      <c r="O89" s="51"/>
+      <c r="Q89" s="52"/>
     </row>
     <row r="90" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="18"/>
@@ -9320,204 +9345,207 @@
         <v>21</v>
       </c>
       <c r="D90" s="30" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
       <c r="E90" s="30" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
       <c r="F90" s="30" t="s">
         <v>65</v>
       </c>
       <c r="G90" s="30" t="s">
+        <v>852</v>
+      </c>
+      <c r="H90" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="18"/>
+      <c r="B91" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D91" s="30" t="s">
+        <v>861</v>
+      </c>
+      <c r="E91" s="30" t="s">
+        <v>857</v>
+      </c>
+      <c r="F91" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G91" s="30" t="s">
         <v>853</v>
       </c>
-      <c r="H90" s="30">
+      <c r="H91" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="18"/>
+      <c r="B92" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D92" s="30" t="s">
+        <v>862</v>
+      </c>
+      <c r="E92" s="30" t="s">
+        <v>858</v>
+      </c>
+      <c r="F92" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G92" s="30" t="s">
+        <v>852</v>
+      </c>
+      <c r="H92" s="30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="18"/>
+      <c r="B93" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D93" s="30" t="s">
+        <v>863</v>
+      </c>
+      <c r="E93" s="30" t="s">
+        <v>859</v>
+      </c>
+      <c r="F93" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G93" s="30" t="s">
+        <v>853</v>
+      </c>
+      <c r="H93" s="30">
         <v>31</v>
       </c>
     </row>
-    <row r="91" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="49" t="b">
+    <row r="94" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="49" t="b">
         <v>1</v>
       </c>
-      <c r="B91" s="49" t="s">
+      <c r="B94" s="49" t="s">
         <v>804</v>
       </c>
-      <c r="C91" s="49" t="s">
+      <c r="C94" s="49" t="s">
         <v>803</v>
       </c>
-      <c r="D91" s="49" t="s">
+      <c r="D94" s="49" t="s">
         <v>803</v>
       </c>
-      <c r="E91" s="49" t="s">
+      <c r="E94" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="J91" s="50"/>
-      <c r="K91" s="51"/>
-      <c r="L91" s="51"/>
-      <c r="M91" s="51"/>
-      <c r="N91" s="51"/>
-      <c r="O91" s="51"/>
-      <c r="Q91" s="52"/>
-    </row>
-    <row r="92" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="49" t="b">
+      <c r="J94" s="50"/>
+      <c r="K94" s="51"/>
+      <c r="L94" s="51"/>
+      <c r="M94" s="51"/>
+      <c r="N94" s="51"/>
+      <c r="O94" s="51"/>
+      <c r="Q94" s="52"/>
+    </row>
+    <row r="95" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="49" t="b">
         <v>1</v>
       </c>
-      <c r="B92" s="49" t="s">
+      <c r="B95" s="49" t="s">
         <v>832</v>
       </c>
-      <c r="C92" s="49" t="s">
+      <c r="C95" s="49" t="s">
         <v>831</v>
       </c>
-      <c r="D92" s="49" t="s">
+      <c r="D95" s="49" t="s">
         <v>831</v>
       </c>
-      <c r="E92" s="49" t="s">
+      <c r="E95" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="J92" s="50"/>
-      <c r="K92" s="51"/>
-      <c r="L92" s="51"/>
-      <c r="M92" s="51"/>
-      <c r="N92" s="51"/>
-      <c r="O92" s="51"/>
-      <c r="Q92" s="52"/>
-    </row>
-    <row r="93" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="22" t="b">
+      <c r="J95" s="50"/>
+      <c r="K95" s="51"/>
+      <c r="L95" s="51"/>
+      <c r="M95" s="51"/>
+      <c r="N95" s="51"/>
+      <c r="O95" s="51"/>
+      <c r="Q95" s="52"/>
+    </row>
+    <row r="96" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="B93" s="22" t="s">
+      <c r="B96" s="22" t="s">
         <v>801</v>
       </c>
-      <c r="C93" s="22" t="s">
+      <c r="C96" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="D93" s="22" t="s">
+      <c r="D96" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="E93" s="22" t="s">
+      <c r="E96" s="22" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="94" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="18"/>
-      <c r="B94" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D94" s="30" t="s">
+    <row r="97" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="18"/>
+      <c r="B97" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D97" s="30" t="s">
         <v>373</v>
       </c>
-      <c r="E94" s="30" t="s">
+      <c r="E97" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="F94" s="30" t="s">
+      <c r="F97" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="H94" s="30" t="s">
+      <c r="H97" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="I94" s="30" t="s">
+      <c r="I97" s="30" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="95" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="43" t="s">
+    <row r="98" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B98" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="D95" s="43" t="s">
+      <c r="D98" s="43" t="s">
         <v>802</v>
       </c>
-      <c r="E95" s="43" t="s">
+      <c r="E98" s="43" t="s">
         <v>288</v>
       </c>
-      <c r="F95" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="G95" s="43" t="s">
+      <c r="F98" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="G98" s="43" t="s">
         <v>792</v>
       </c>
-      <c r="H95" s="43">
-        <v>0</v>
-      </c>
-      <c r="J95" s="43">
-        <v>0</v>
-      </c>
-      <c r="K95" s="43">
+      <c r="H98" s="43">
+        <v>0</v>
+      </c>
+      <c r="J98" s="43">
+        <v>0</v>
+      </c>
+      <c r="K98" s="43">
         <v>40</v>
       </c>
-      <c r="L95" s="43">
+      <c r="L98" s="43">
         <v>-1</v>
       </c>
-      <c r="M95" s="45">
-        <f>(K95-J95)/6</f>
+      <c r="M98" s="45">
+        <f>(K98-J98)/6</f>
         <v>6.666666666666667</v>
       </c>
-      <c r="N95" s="45">
+      <c r="N98" s="45">
         <v>2.5</v>
       </c>
-      <c r="Q95" s="43" t="s">
+      <c r="Q98" s="43" t="s">
         <v>777</v>
-      </c>
-    </row>
-    <row r="96" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B96" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D96" s="30" t="s">
-        <v>793</v>
-      </c>
-      <c r="E96" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="F96" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G96" s="30" t="s">
-        <v>792</v>
-      </c>
-      <c r="H96" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D97" s="30" t="s">
-        <v>794</v>
-      </c>
-      <c r="E97" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="F97" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G97" s="30" t="s">
-        <v>792</v>
-      </c>
-      <c r="H97" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D98" s="30" t="s">
-        <v>795</v>
-      </c>
-      <c r="E98" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="F98" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G98" s="30" t="s">
-        <v>796</v>
-      </c>
-      <c r="H98" s="30">
-        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -9525,15 +9553,18 @@
         <v>21</v>
       </c>
       <c r="D99" s="30" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="E99" s="30" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F99" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="H99" s="30" t="b">
+        <v>64</v>
+      </c>
+      <c r="G99" s="30" t="s">
+        <v>792</v>
+      </c>
+      <c r="H99" s="30">
         <v>0</v>
       </c>
     </row>
@@ -9542,19 +9573,19 @@
         <v>21</v>
       </c>
       <c r="D100" s="30" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="E100" s="30" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F100" s="30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G100" s="30" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="H100" s="30">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -9562,16 +9593,16 @@
         <v>21</v>
       </c>
       <c r="D101" s="30" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="E101" s="30" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F101" s="30" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G101" s="30" t="s">
-        <v>792</v>
+        <v>796</v>
       </c>
       <c r="H101" s="30">
         <v>0</v>
@@ -9582,136 +9613,136 @@
         <v>21</v>
       </c>
       <c r="D102" s="30" t="s">
+        <v>797</v>
+      </c>
+      <c r="E102" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="F102" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="H102" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B103" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D103" s="30" t="s">
+        <v>798</v>
+      </c>
+      <c r="E103" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F103" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G103" s="30" t="s">
+        <v>796</v>
+      </c>
+      <c r="H103" s="30">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B104" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D104" s="30" t="s">
+        <v>799</v>
+      </c>
+      <c r="E104" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F104" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G104" s="30" t="s">
+        <v>792</v>
+      </c>
+      <c r="H104" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B105" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D105" s="30" t="s">
         <v>800</v>
       </c>
-      <c r="E102" s="30" t="s">
+      <c r="E105" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="F102" s="30" t="s">
+      <c r="F105" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="G102" s="30" t="s">
+      <c r="G105" s="30" t="s">
         <v>796</v>
       </c>
-      <c r="H102" s="30">
+      <c r="H105" s="30">
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="49" t="b">
+    <row r="106" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="49" t="b">
         <v>1</v>
       </c>
-      <c r="B103" s="49" t="s">
+      <c r="B106" s="49" t="s">
         <v>209</v>
       </c>
-      <c r="C103" s="49" t="s">
+      <c r="C106" s="49" t="s">
         <v>210</v>
       </c>
-      <c r="D103" s="49" t="s">
+      <c r="D106" s="49" t="s">
         <v>210</v>
       </c>
-      <c r="E103" s="49" t="s">
+      <c r="E106" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="J103" s="50"/>
-      <c r="K103" s="51"/>
-      <c r="L103" s="51"/>
-      <c r="M103" s="51"/>
-      <c r="N103" s="51"/>
-      <c r="O103" s="51"/>
-      <c r="Q103" s="52"/>
-    </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B104" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D104" s="31" t="s">
-        <v>835</v>
-      </c>
-      <c r="E104" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="F104" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H104" s="31" t="s">
-        <v>417</v>
-      </c>
-      <c r="I104" s="30" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B105" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D105" s="31" t="s">
-        <v>836</v>
-      </c>
-      <c r="E105" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="F105" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="H105" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="I105" s="31"/>
-    </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B106" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D106" s="31" t="s">
-        <v>837</v>
-      </c>
-      <c r="E106" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="F106" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="H106" s="31">
-        <v>0</v>
-      </c>
-      <c r="I106" s="31"/>
+      <c r="J106" s="50"/>
+      <c r="K106" s="51"/>
+      <c r="L106" s="51"/>
+      <c r="M106" s="51"/>
+      <c r="N106" s="51"/>
+      <c r="O106" s="51"/>
+      <c r="Q106" s="52"/>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B107" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D107" s="31" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
       <c r="E107" s="31" t="s">
-        <v>50</v>
+        <v>126</v>
       </c>
       <c r="F107" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="H107" s="31">
-        <v>0</v>
-      </c>
-      <c r="I107" s="31"/>
+        <v>62</v>
+      </c>
+      <c r="H107" s="31" t="s">
+        <v>417</v>
+      </c>
+      <c r="I107" s="30" t="s">
+        <v>418</v>
+      </c>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B108" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D108" s="31" t="s">
-        <v>795</v>
+        <v>836</v>
       </c>
       <c r="E108" s="31" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="F108" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G108" s="30" t="s">
-        <v>796</v>
-      </c>
-      <c r="H108" s="31">
+        <v>63</v>
+      </c>
+      <c r="H108" s="31" t="b">
         <v>0</v>
       </c>
       <c r="I108" s="31"/>
@@ -9721,16 +9752,15 @@
         <v>21</v>
       </c>
       <c r="D109" s="31" t="s">
-        <v>797</v>
+        <v>837</v>
       </c>
       <c r="E109" s="31" t="s">
-        <v>54</v>
+        <v>128</v>
       </c>
       <c r="F109" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="G109" s="30"/>
-      <c r="H109" s="31" t="b">
+        <v>64</v>
+      </c>
+      <c r="H109" s="31">
         <v>0</v>
       </c>
       <c r="I109" s="31"/>
@@ -9739,20 +9769,17 @@
       <c r="B110" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D110" s="30" t="s">
-        <v>798</v>
-      </c>
-      <c r="E110" s="30" t="s">
-        <v>56</v>
+      <c r="D110" s="31" t="s">
+        <v>838</v>
+      </c>
+      <c r="E110" s="31" t="s">
+        <v>50</v>
       </c>
       <c r="F110" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G110" s="30" t="s">
-        <v>796</v>
+        <v>64</v>
       </c>
       <c r="H110" s="31">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I110" s="31"/>
     </row>
@@ -9760,17 +9787,17 @@
       <c r="B111" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D111" s="30" t="s">
-        <v>851</v>
-      </c>
-      <c r="E111" s="30" t="s">
-        <v>58</v>
+      <c r="D111" s="31" t="s">
+        <v>795</v>
+      </c>
+      <c r="E111" s="31" t="s">
+        <v>52</v>
       </c>
       <c r="F111" s="30" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G111" s="30" t="s">
-        <v>792</v>
+        <v>796</v>
       </c>
       <c r="H111" s="31">
         <v>0</v>
@@ -9781,159 +9808,157 @@
       <c r="B112" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D112" s="30" t="s">
-        <v>800</v>
-      </c>
-      <c r="E112" s="30" t="s">
-        <v>60</v>
+      <c r="D112" s="31" t="s">
+        <v>797</v>
+      </c>
+      <c r="E112" s="31" t="s">
+        <v>54</v>
       </c>
       <c r="F112" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="G112" s="30"/>
+      <c r="H112" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I112" s="31"/>
+    </row>
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B113" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D113" s="30" t="s">
+        <v>798</v>
+      </c>
+      <c r="E113" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F113" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="G112" s="30" t="s">
+      <c r="G113" s="30" t="s">
         <v>796</v>
       </c>
-      <c r="H112" s="31">
-        <v>1</v>
-      </c>
-      <c r="I112" s="31"/>
-    </row>
-    <row r="113" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B113" s="49" t="s">
-        <v>216</v>
-      </c>
-      <c r="C113" s="49" t="s">
-        <v>217</v>
-      </c>
-      <c r="D113" s="49" t="s">
-        <v>217</v>
-      </c>
-      <c r="E113" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="J113" s="50"/>
-      <c r="K113" s="51"/>
-      <c r="L113" s="51"/>
-      <c r="M113" s="51"/>
-      <c r="N113" s="51"/>
-      <c r="O113" s="51"/>
-      <c r="Q113" s="52"/>
+      <c r="H113" s="31">
+        <v>15</v>
+      </c>
+      <c r="I113" s="31"/>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B114" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D114" s="31" t="s">
-        <v>835</v>
-      </c>
-      <c r="E114" s="31" t="s">
-        <v>126</v>
+      <c r="D114" s="30" t="s">
+        <v>851</v>
+      </c>
+      <c r="E114" s="30" t="s">
+        <v>58</v>
       </c>
       <c r="F114" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H114" s="31" t="s">
-        <v>417</v>
-      </c>
-      <c r="I114" s="30" t="s">
-        <v>418</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="G114" s="30" t="s">
+        <v>792</v>
+      </c>
+      <c r="H114" s="31">
+        <v>0</v>
+      </c>
+      <c r="I114" s="31"/>
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B115" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D115" s="31" t="s">
-        <v>841</v>
-      </c>
-      <c r="E115" s="31" t="s">
-        <v>219</v>
+      <c r="D115" s="30" t="s">
+        <v>800</v>
+      </c>
+      <c r="E115" s="30" t="s">
+        <v>60</v>
       </c>
       <c r="F115" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H115" s="31" t="s">
-        <v>839</v>
-      </c>
-      <c r="I115" s="30" t="s">
-        <v>840</v>
-      </c>
-    </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B116" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D116" s="31" t="s">
-        <v>842</v>
-      </c>
-      <c r="E116" s="31" t="s">
-        <v>221</v>
-      </c>
-      <c r="F116" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G116" s="31" t="s">
-        <v>843</v>
-      </c>
-      <c r="H116" s="31">
-        <v>69</v>
-      </c>
-      <c r="I116" s="31"/>
+        <v>65</v>
+      </c>
+      <c r="G115" s="30" t="s">
+        <v>796</v>
+      </c>
+      <c r="H115" s="31">
+        <v>1</v>
+      </c>
+      <c r="I115" s="31"/>
+    </row>
+    <row r="116" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="B116" s="49" t="s">
+        <v>216</v>
+      </c>
+      <c r="C116" s="49" t="s">
+        <v>217</v>
+      </c>
+      <c r="D116" s="49" t="s">
+        <v>217</v>
+      </c>
+      <c r="E116" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="J116" s="50"/>
+      <c r="K116" s="51"/>
+      <c r="L116" s="51"/>
+      <c r="M116" s="51"/>
+      <c r="N116" s="51"/>
+      <c r="O116" s="51"/>
+      <c r="Q116" s="52"/>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B117" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D117" s="31" t="s">
-        <v>845</v>
+        <v>835</v>
       </c>
       <c r="E117" s="31" t="s">
-        <v>223</v>
+        <v>126</v>
       </c>
       <c r="F117" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G117" s="31" t="s">
-        <v>844</v>
-      </c>
-      <c r="H117" s="31">
-        <v>28</v>
-      </c>
-      <c r="I117" s="31"/>
+        <v>62</v>
+      </c>
+      <c r="H117" s="31" t="s">
+        <v>417</v>
+      </c>
+      <c r="I117" s="30" t="s">
+        <v>418</v>
+      </c>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B118" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D118" s="31" t="s">
-        <v>846</v>
+        <v>841</v>
       </c>
       <c r="E118" s="31" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="F118" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G118" s="31" t="s">
-        <v>843</v>
-      </c>
-      <c r="H118" s="31">
-        <v>55</v>
-      </c>
-      <c r="I118" s="31"/>
+        <v>62</v>
+      </c>
+      <c r="H118" s="31" t="s">
+        <v>839</v>
+      </c>
+      <c r="I118" s="30" t="s">
+        <v>840</v>
+      </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B119" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D119" s="31" t="s">
-        <v>847</v>
+        <v>842</v>
       </c>
       <c r="E119" s="31" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="F119" s="30" t="s">
         <v>64</v>
@@ -9942,7 +9967,7 @@
         <v>843</v>
       </c>
       <c r="H119" s="31">
-        <v>-148</v>
+        <v>69</v>
       </c>
       <c r="I119" s="31"/>
     </row>
@@ -9951,16 +9976,19 @@
         <v>21</v>
       </c>
       <c r="D120" s="31" t="s">
-        <v>836</v>
+        <v>845</v>
       </c>
       <c r="E120" s="31" t="s">
-        <v>91</v>
+        <v>223</v>
       </c>
       <c r="F120" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="H120" s="31" t="b">
-        <v>0</v>
+        <v>64</v>
+      </c>
+      <c r="G120" s="31" t="s">
+        <v>844</v>
+      </c>
+      <c r="H120" s="31">
+        <v>28</v>
       </c>
       <c r="I120" s="31"/>
     </row>
@@ -9969,16 +9997,19 @@
         <v>21</v>
       </c>
       <c r="D121" s="31" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="E121" s="31" t="s">
-        <v>128</v>
+        <v>225</v>
       </c>
       <c r="F121" s="30" t="s">
         <v>64</v>
       </c>
+      <c r="G121" s="31" t="s">
+        <v>843</v>
+      </c>
       <c r="H121" s="31">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="I121" s="31"/>
     </row>
@@ -9987,16 +10018,19 @@
         <v>21</v>
       </c>
       <c r="D122" s="31" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="E122" s="31" t="s">
-        <v>50</v>
+        <v>227</v>
       </c>
       <c r="F122" s="30" t="s">
         <v>64</v>
       </c>
+      <c r="G122" s="31" t="s">
+        <v>843</v>
+      </c>
       <c r="H122" s="31">
-        <v>0</v>
+        <v>-148</v>
       </c>
       <c r="I122" s="31"/>
     </row>
@@ -10005,18 +10039,15 @@
         <v>21</v>
       </c>
       <c r="D123" s="31" t="s">
-        <v>795</v>
+        <v>836</v>
       </c>
       <c r="E123" s="31" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="F123" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G123" s="30" t="s">
-        <v>796</v>
-      </c>
-      <c r="H123" s="31">
+        <v>63</v>
+      </c>
+      <c r="H123" s="31" t="b">
         <v>0</v>
       </c>
       <c r="I123" s="31"/>
@@ -10026,16 +10057,15 @@
         <v>21</v>
       </c>
       <c r="D124" s="31" t="s">
-        <v>797</v>
+        <v>848</v>
       </c>
       <c r="E124" s="31" t="s">
-        <v>54</v>
+        <v>128</v>
       </c>
       <c r="F124" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="G124" s="30"/>
-      <c r="H124" s="31" t="b">
+        <v>64</v>
+      </c>
+      <c r="H124" s="31">
         <v>0</v>
       </c>
       <c r="I124" s="31"/>
@@ -10044,20 +10074,17 @@
       <c r="B125" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D125" s="30" t="s">
-        <v>798</v>
-      </c>
-      <c r="E125" s="30" t="s">
-        <v>56</v>
+      <c r="D125" s="31" t="s">
+        <v>849</v>
+      </c>
+      <c r="E125" s="31" t="s">
+        <v>50</v>
       </c>
       <c r="F125" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G125" s="30" t="s">
-        <v>796</v>
+        <v>64</v>
       </c>
       <c r="H125" s="31">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I125" s="31"/>
     </row>
@@ -10065,17 +10092,17 @@
       <c r="B126" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D126" s="30" t="s">
-        <v>850</v>
-      </c>
-      <c r="E126" s="30" t="s">
-        <v>58</v>
+      <c r="D126" s="31" t="s">
+        <v>795</v>
+      </c>
+      <c r="E126" s="31" t="s">
+        <v>52</v>
       </c>
       <c r="F126" s="30" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G126" s="30" t="s">
-        <v>792</v>
+        <v>796</v>
       </c>
       <c r="H126" s="31">
         <v>0</v>
@@ -10086,88 +10113,137 @@
       <c r="B127" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D127" s="30" t="s">
+      <c r="D127" s="31" t="s">
+        <v>797</v>
+      </c>
+      <c r="E127" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="F127" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="G127" s="30"/>
+      <c r="H127" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I127" s="31"/>
+    </row>
+    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B128" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D128" s="30" t="s">
+        <v>798</v>
+      </c>
+      <c r="E128" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F128" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G128" s="30" t="s">
+        <v>796</v>
+      </c>
+      <c r="H128" s="31">
+        <v>15</v>
+      </c>
+      <c r="I128" s="31"/>
+    </row>
+    <row r="129" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B129" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D129" s="30" t="s">
+        <v>850</v>
+      </c>
+      <c r="E129" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F129" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G129" s="30" t="s">
+        <v>792</v>
+      </c>
+      <c r="H129" s="31">
+        <v>0</v>
+      </c>
+      <c r="I129" s="31"/>
+    </row>
+    <row r="130" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B130" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D130" s="30" t="s">
         <v>800</v>
       </c>
-      <c r="E127" s="30" t="s">
+      <c r="E130" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="F127" s="30" t="s">
+      <c r="F130" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="G127" s="30" t="s">
+      <c r="G130" s="30" t="s">
         <v>796</v>
       </c>
-      <c r="H127" s="31">
+      <c r="H130" s="31">
         <v>1</v>
       </c>
-      <c r="I127" s="31"/>
-    </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H128" s="31"/>
-      <c r="I128" s="31"/>
-    </row>
-    <row r="129" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H129" s="31"/>
-      <c r="I129" s="31"/>
-    </row>
-    <row r="130" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H130" s="31"/>
       <c r="I130" s="31"/>
     </row>
-    <row r="131" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H131" s="31"/>
       <c r="I131" s="31"/>
     </row>
-    <row r="132" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H132" s="31"/>
       <c r="I132" s="31"/>
     </row>
-    <row r="133" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H133" s="31"/>
       <c r="I133" s="31"/>
     </row>
-    <row r="134" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H134" s="31"/>
       <c r="I134" s="31"/>
     </row>
-    <row r="135" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H135" s="31"/>
       <c r="I135" s="31"/>
     </row>
-    <row r="136" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H136" s="31"/>
       <c r="I136" s="31"/>
     </row>
-    <row r="137" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H137" s="31"/>
       <c r="I137" s="31"/>
     </row>
-    <row r="138" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H138" s="31"/>
       <c r="I138" s="31"/>
     </row>
-    <row r="139" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H139" s="31"/>
       <c r="I139" s="31"/>
     </row>
-    <row r="140" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H140" s="31"/>
       <c r="I140" s="31"/>
     </row>
-    <row r="141" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H141" s="31"/>
       <c r="I141" s="31"/>
     </row>
-    <row r="142" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H142" s="31"/>
       <c r="I142" s="31"/>
     </row>
-    <row r="143" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H143" s="31"/>
       <c r="I143" s="31"/>
     </row>
-    <row r="144" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H144" s="31"/>
       <c r="I144" s="31"/>
     </row>
@@ -10427,8 +10503,20 @@
       <c r="H208" s="31"/>
       <c r="I208" s="31"/>
     </row>
+    <row r="209" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H209" s="31"/>
+      <c r="I209" s="31"/>
+    </row>
+    <row r="210" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H210" s="31"/>
+      <c r="I210" s="31"/>
+    </row>
+    <row r="211" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H211" s="31"/>
+      <c r="I211" s="31"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:Z135"/>
+  <autoFilter ref="A2:Z138"/>
   <mergeCells count="1">
     <mergeCell ref="T1:Y1"/>
   </mergeCells>

</xml_diff>

<commit_message>
Adding Roof and Wall cal measure to office_ee.xlsx
</commit_message>
<xml_diff>
--- a/projects/office_ee.xlsx
+++ b/projects/office_ee.xlsx
@@ -16,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$138</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$142</definedName>
     <definedName name="AnalysisType">Lookups!$A$17:$A$23</definedName>
     <definedName name="instance_defs">Lookups!$A$2:$D$9</definedName>
     <definedName name="instance_types">Lookups!$A$2:$A$9</definedName>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2725" uniqueCount="865">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2743" uniqueCount="871">
   <si>
     <t>type</t>
   </si>
@@ -2636,6 +2636,24 @@
   </si>
   <si>
     <t>Design Specification Outdoor Air Reduction (%)</t>
+  </si>
+  <si>
+    <t>IncreaseInsulationRValueForRoofsByPercentage</t>
+  </si>
+  <si>
+    <t>IncreaseInsulationRValueForExteriorWallsByPercentage</t>
+  </si>
+  <si>
+    <t>Increase Insulation R value For Roofs By Percentage</t>
+  </si>
+  <si>
+    <t>Increase Insulation R value For Exterior Walls By Percentage</t>
+  </si>
+  <si>
+    <t>Percentage Increase of R-value for Roof Insulation</t>
+  </si>
+  <si>
+    <t>Percentage Increase of R-value for Exterior Wall Insulation</t>
   </si>
 </sst>
 </file>
@@ -7315,11 +7333,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y211"/>
+  <dimension ref="A1:Y215"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E87" sqref="E87"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9315,177 +9333,203 @@
         <v>777</v>
       </c>
     </row>
-    <row r="89" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="49" t="b">
+    <row r="89" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="38" t="b">
         <v>1</v>
       </c>
-      <c r="B89" s="49" t="s">
+      <c r="B89" s="38" t="s">
+        <v>867</v>
+      </c>
+      <c r="C89" s="38" t="s">
+        <v>865</v>
+      </c>
+      <c r="D89" s="38" t="s">
+        <v>865</v>
+      </c>
+      <c r="E89" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="G89" s="39"/>
+      <c r="H89" s="39"/>
+    </row>
+    <row r="90" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B90" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D90" s="43" t="s">
+        <v>869</v>
+      </c>
+      <c r="E90" s="43" t="s">
+        <v>258</v>
+      </c>
+      <c r="F90" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="H90" s="43">
+        <v>30</v>
+      </c>
+      <c r="I90" s="46"/>
+      <c r="J90" s="45">
+        <v>-100</v>
+      </c>
+      <c r="K90" s="45">
+        <v>100</v>
+      </c>
+      <c r="L90" s="45">
+        <v>0</v>
+      </c>
+      <c r="M90" s="45">
+        <f>(K90-J90)/6</f>
+        <v>33.333333333333336</v>
+      </c>
+      <c r="N90" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q90" s="43" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="B91" s="38" t="s">
+        <v>868</v>
+      </c>
+      <c r="C91" s="38" t="s">
+        <v>866</v>
+      </c>
+      <c r="D91" s="38" t="s">
+        <v>866</v>
+      </c>
+      <c r="E91" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="G91" s="39"/>
+      <c r="H91" s="39"/>
+    </row>
+    <row r="92" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B92" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D92" s="43" t="s">
+        <v>870</v>
+      </c>
+      <c r="E92" s="43" t="s">
+        <v>258</v>
+      </c>
+      <c r="F92" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="H92" s="43">
+        <v>30</v>
+      </c>
+      <c r="I92" s="46"/>
+      <c r="J92" s="45">
+        <v>-100</v>
+      </c>
+      <c r="K92" s="45">
+        <v>100</v>
+      </c>
+      <c r="L92" s="45">
+        <v>0</v>
+      </c>
+      <c r="M92" s="45">
+        <f>(K92-J92)/6</f>
+        <v>33.333333333333336</v>
+      </c>
+      <c r="N92" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q92" s="43" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="B93" s="49" t="s">
         <v>855</v>
       </c>
-      <c r="C89" s="49" t="s">
+      <c r="C93" s="49" t="s">
         <v>854</v>
       </c>
-      <c r="D89" s="49" t="s">
+      <c r="D93" s="49" t="s">
         <v>854</v>
       </c>
-      <c r="E89" s="49" t="s">
+      <c r="E93" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="J89" s="50"/>
-      <c r="K89" s="51"/>
-      <c r="L89" s="51"/>
-      <c r="M89" s="51"/>
-      <c r="N89" s="51"/>
-      <c r="O89" s="51"/>
-      <c r="Q89" s="52"/>
-    </row>
-    <row r="90" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="18"/>
-      <c r="B90" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D90" s="30" t="s">
+      <c r="J93" s="50"/>
+      <c r="K93" s="51"/>
+      <c r="L93" s="51"/>
+      <c r="M93" s="51"/>
+      <c r="N93" s="51"/>
+      <c r="O93" s="51"/>
+      <c r="Q93" s="52"/>
+    </row>
+    <row r="94" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="18"/>
+      <c r="B94" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D94" s="30" t="s">
         <v>860</v>
       </c>
-      <c r="E90" s="30" t="s">
+      <c r="E94" s="30" t="s">
         <v>856</v>
       </c>
-      <c r="F90" s="30" t="s">
+      <c r="F94" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="G90" s="30" t="s">
+      <c r="G94" s="30" t="s">
         <v>852</v>
       </c>
-      <c r="H90" s="30">
+      <c r="H94" s="30">
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="18"/>
-      <c r="B91" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D91" s="30" t="s">
+    <row r="95" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="18"/>
+      <c r="B95" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D95" s="30" t="s">
         <v>861</v>
       </c>
-      <c r="E91" s="30" t="s">
+      <c r="E95" s="30" t="s">
         <v>857</v>
       </c>
-      <c r="F91" s="30" t="s">
+      <c r="F95" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="G91" s="30" t="s">
+      <c r="G95" s="30" t="s">
         <v>853</v>
       </c>
-      <c r="H91" s="30">
+      <c r="H95" s="30">
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="18"/>
-      <c r="B92" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D92" s="30" t="s">
+    <row r="96" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="18"/>
+      <c r="B96" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D96" s="30" t="s">
         <v>862</v>
       </c>
-      <c r="E92" s="30" t="s">
+      <c r="E96" s="30" t="s">
         <v>858</v>
       </c>
-      <c r="F92" s="30" t="s">
+      <c r="F96" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="G92" s="30" t="s">
+      <c r="G96" s="30" t="s">
         <v>852</v>
       </c>
-      <c r="H92" s="30">
+      <c r="H96" s="30">
         <v>12</v>
-      </c>
-    </row>
-    <row r="93" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="18"/>
-      <c r="B93" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D93" s="30" t="s">
-        <v>863</v>
-      </c>
-      <c r="E93" s="30" t="s">
-        <v>859</v>
-      </c>
-      <c r="F93" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G93" s="30" t="s">
-        <v>853</v>
-      </c>
-      <c r="H93" s="30">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="94" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B94" s="49" t="s">
-        <v>804</v>
-      </c>
-      <c r="C94" s="49" t="s">
-        <v>803</v>
-      </c>
-      <c r="D94" s="49" t="s">
-        <v>803</v>
-      </c>
-      <c r="E94" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="J94" s="50"/>
-      <c r="K94" s="51"/>
-      <c r="L94" s="51"/>
-      <c r="M94" s="51"/>
-      <c r="N94" s="51"/>
-      <c r="O94" s="51"/>
-      <c r="Q94" s="52"/>
-    </row>
-    <row r="95" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B95" s="49" t="s">
-        <v>832</v>
-      </c>
-      <c r="C95" s="49" t="s">
-        <v>831</v>
-      </c>
-      <c r="D95" s="49" t="s">
-        <v>831</v>
-      </c>
-      <c r="E95" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="J95" s="50"/>
-      <c r="K95" s="51"/>
-      <c r="L95" s="51"/>
-      <c r="M95" s="51"/>
-      <c r="N95" s="51"/>
-      <c r="O95" s="51"/>
-      <c r="Q95" s="52"/>
-    </row>
-    <row r="96" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="B96" s="22" t="s">
-        <v>801</v>
-      </c>
-      <c r="C96" s="22" t="s">
-        <v>286</v>
-      </c>
-      <c r="D96" s="22" t="s">
-        <v>286</v>
-      </c>
-      <c r="E96" s="22" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="97" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -9494,135 +9538,144 @@
         <v>21</v>
       </c>
       <c r="D97" s="30" t="s">
+        <v>863</v>
+      </c>
+      <c r="E97" s="30" t="s">
+        <v>859</v>
+      </c>
+      <c r="F97" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G97" s="30" t="s">
+        <v>853</v>
+      </c>
+      <c r="H97" s="30">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="B98" s="49" t="s">
+        <v>804</v>
+      </c>
+      <c r="C98" s="49" t="s">
+        <v>803</v>
+      </c>
+      <c r="D98" s="49" t="s">
+        <v>803</v>
+      </c>
+      <c r="E98" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="J98" s="50"/>
+      <c r="K98" s="51"/>
+      <c r="L98" s="51"/>
+      <c r="M98" s="51"/>
+      <c r="N98" s="51"/>
+      <c r="O98" s="51"/>
+      <c r="Q98" s="52"/>
+    </row>
+    <row r="99" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="B99" s="49" t="s">
+        <v>832</v>
+      </c>
+      <c r="C99" s="49" t="s">
+        <v>831</v>
+      </c>
+      <c r="D99" s="49" t="s">
+        <v>831</v>
+      </c>
+      <c r="E99" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="J99" s="50"/>
+      <c r="K99" s="51"/>
+      <c r="L99" s="51"/>
+      <c r="M99" s="51"/>
+      <c r="N99" s="51"/>
+      <c r="O99" s="51"/>
+      <c r="Q99" s="52"/>
+    </row>
+    <row r="100" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="B100" s="22" t="s">
+        <v>801</v>
+      </c>
+      <c r="C100" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="D100" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="E100" s="22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="18"/>
+      <c r="B101" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D101" s="30" t="s">
         <v>373</v>
       </c>
-      <c r="E97" s="30" t="s">
+      <c r="E101" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="F97" s="30" t="s">
+      <c r="F101" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="H97" s="30" t="s">
+      <c r="H101" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="I97" s="30" t="s">
+      <c r="I101" s="30" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="98" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="43" t="s">
+    <row r="102" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B102" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="D98" s="43" t="s">
+      <c r="D102" s="43" t="s">
         <v>802</v>
       </c>
-      <c r="E98" s="43" t="s">
+      <c r="E102" s="43" t="s">
         <v>288</v>
       </c>
-      <c r="F98" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="G98" s="43" t="s">
+      <c r="F102" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="G102" s="43" t="s">
         <v>792</v>
       </c>
-      <c r="H98" s="43">
-        <v>0</v>
-      </c>
-      <c r="J98" s="43">
-        <v>0</v>
-      </c>
-      <c r="K98" s="43">
+      <c r="H102" s="43">
+        <v>0</v>
+      </c>
+      <c r="J102" s="43">
+        <v>0</v>
+      </c>
+      <c r="K102" s="43">
         <v>40</v>
       </c>
-      <c r="L98" s="43">
+      <c r="L102" s="43">
         <v>-1</v>
       </c>
-      <c r="M98" s="45">
-        <f>(K98-J98)/6</f>
+      <c r="M102" s="45">
+        <f>(K102-J102)/6</f>
         <v>6.666666666666667</v>
       </c>
-      <c r="N98" s="45">
+      <c r="N102" s="45">
         <v>2.5</v>
       </c>
-      <c r="Q98" s="43" t="s">
+      <c r="Q102" s="43" t="s">
         <v>777</v>
-      </c>
-    </row>
-    <row r="99" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D99" s="30" t="s">
-        <v>793</v>
-      </c>
-      <c r="E99" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="F99" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G99" s="30" t="s">
-        <v>792</v>
-      </c>
-      <c r="H99" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D100" s="30" t="s">
-        <v>794</v>
-      </c>
-      <c r="E100" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="F100" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G100" s="30" t="s">
-        <v>792</v>
-      </c>
-      <c r="H100" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D101" s="30" t="s">
-        <v>795</v>
-      </c>
-      <c r="E101" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="F101" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G101" s="30" t="s">
-        <v>796</v>
-      </c>
-      <c r="H101" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D102" s="30" t="s">
-        <v>797</v>
-      </c>
-      <c r="E102" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="F102" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="H102" s="30" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -9630,19 +9683,19 @@
         <v>21</v>
       </c>
       <c r="D103" s="30" t="s">
-        <v>798</v>
+        <v>793</v>
       </c>
       <c r="E103" s="30" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="F103" s="30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G103" s="30" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="H103" s="30">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -9650,10 +9703,10 @@
         <v>21</v>
       </c>
       <c r="D104" s="30" t="s">
-        <v>799</v>
+        <v>794</v>
       </c>
       <c r="E104" s="30" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="F104" s="30" t="s">
         <v>64</v>
@@ -9670,10 +9723,10 @@
         <v>21</v>
       </c>
       <c r="D105" s="30" t="s">
-        <v>800</v>
+        <v>795</v>
       </c>
       <c r="E105" s="30" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="F105" s="30" t="s">
         <v>65</v>
@@ -9682,142 +9735,143 @@
         <v>796</v>
       </c>
       <c r="H105" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B106" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D106" s="30" t="s">
+        <v>797</v>
+      </c>
+      <c r="E106" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="F106" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="H106" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B107" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D107" s="30" t="s">
+        <v>798</v>
+      </c>
+      <c r="E107" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F107" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G107" s="30" t="s">
+        <v>796</v>
+      </c>
+      <c r="H107" s="30">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="108" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B108" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D108" s="30" t="s">
+        <v>799</v>
+      </c>
+      <c r="E108" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F108" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G108" s="30" t="s">
+        <v>792</v>
+      </c>
+      <c r="H108" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B109" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D109" s="30" t="s">
+        <v>800</v>
+      </c>
+      <c r="E109" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="F109" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G109" s="30" t="s">
+        <v>796</v>
+      </c>
+      <c r="H109" s="30">
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="49" t="b">
+    <row r="110" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="49" t="b">
         <v>1</v>
       </c>
-      <c r="B106" s="49" t="s">
+      <c r="B110" s="49" t="s">
         <v>209</v>
       </c>
-      <c r="C106" s="49" t="s">
+      <c r="C110" s="49" t="s">
         <v>210</v>
       </c>
-      <c r="D106" s="49" t="s">
+      <c r="D110" s="49" t="s">
         <v>210</v>
       </c>
-      <c r="E106" s="49" t="s">
+      <c r="E110" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="J106" s="50"/>
-      <c r="K106" s="51"/>
-      <c r="L106" s="51"/>
-      <c r="M106" s="51"/>
-      <c r="N106" s="51"/>
-      <c r="O106" s="51"/>
-      <c r="Q106" s="52"/>
-    </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B107" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D107" s="31" t="s">
-        <v>835</v>
-      </c>
-      <c r="E107" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="F107" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H107" s="31" t="s">
-        <v>417</v>
-      </c>
-      <c r="I107" s="30" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B108" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D108" s="31" t="s">
-        <v>836</v>
-      </c>
-      <c r="E108" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="F108" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="H108" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="I108" s="31"/>
-    </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B109" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D109" s="31" t="s">
-        <v>837</v>
-      </c>
-      <c r="E109" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="F109" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="H109" s="31">
-        <v>0</v>
-      </c>
-      <c r="I109" s="31"/>
-    </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B110" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D110" s="31" t="s">
-        <v>838</v>
-      </c>
-      <c r="E110" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="F110" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="H110" s="31">
-        <v>0</v>
-      </c>
-      <c r="I110" s="31"/>
+      <c r="J110" s="50"/>
+      <c r="K110" s="51"/>
+      <c r="L110" s="51"/>
+      <c r="M110" s="51"/>
+      <c r="N110" s="51"/>
+      <c r="O110" s="51"/>
+      <c r="Q110" s="52"/>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B111" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D111" s="31" t="s">
-        <v>795</v>
+        <v>835</v>
       </c>
       <c r="E111" s="31" t="s">
-        <v>52</v>
+        <v>126</v>
       </c>
       <c r="F111" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G111" s="30" t="s">
-        <v>796</v>
-      </c>
-      <c r="H111" s="31">
-        <v>0</v>
-      </c>
-      <c r="I111" s="31"/>
+        <v>62</v>
+      </c>
+      <c r="H111" s="31" t="s">
+        <v>417</v>
+      </c>
+      <c r="I111" s="30" t="s">
+        <v>418</v>
+      </c>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B112" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D112" s="31" t="s">
-        <v>797</v>
+        <v>836</v>
       </c>
       <c r="E112" s="31" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="F112" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="G112" s="30"/>
       <c r="H112" s="31" t="b">
         <v>0</v>
       </c>
@@ -9827,20 +9881,17 @@
       <c r="B113" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D113" s="30" t="s">
-        <v>798</v>
-      </c>
-      <c r="E113" s="30" t="s">
-        <v>56</v>
+      <c r="D113" s="31" t="s">
+        <v>837</v>
+      </c>
+      <c r="E113" s="31" t="s">
+        <v>128</v>
       </c>
       <c r="F113" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G113" s="30" t="s">
-        <v>796</v>
+        <v>64</v>
       </c>
       <c r="H113" s="31">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I113" s="31"/>
     </row>
@@ -9848,17 +9899,14 @@
       <c r="B114" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D114" s="30" t="s">
-        <v>851</v>
-      </c>
-      <c r="E114" s="30" t="s">
-        <v>58</v>
+      <c r="D114" s="31" t="s">
+        <v>838</v>
+      </c>
+      <c r="E114" s="31" t="s">
+        <v>50</v>
       </c>
       <c r="F114" s="30" t="s">
         <v>64</v>
-      </c>
-      <c r="G114" s="30" t="s">
-        <v>792</v>
       </c>
       <c r="H114" s="31">
         <v>0</v>
@@ -9869,11 +9917,11 @@
       <c r="B115" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D115" s="30" t="s">
-        <v>800</v>
-      </c>
-      <c r="E115" s="30" t="s">
-        <v>60</v>
+      <c r="D115" s="31" t="s">
+        <v>795</v>
+      </c>
+      <c r="E115" s="31" t="s">
+        <v>52</v>
       </c>
       <c r="F115" s="30" t="s">
         <v>65</v>
@@ -9882,173 +9930,174 @@
         <v>796</v>
       </c>
       <c r="H115" s="31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I115" s="31"/>
     </row>
-    <row r="116" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B116" s="49" t="s">
-        <v>216</v>
-      </c>
-      <c r="C116" s="49" t="s">
-        <v>217</v>
-      </c>
-      <c r="D116" s="49" t="s">
-        <v>217</v>
-      </c>
-      <c r="E116" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="J116" s="50"/>
-      <c r="K116" s="51"/>
-      <c r="L116" s="51"/>
-      <c r="M116" s="51"/>
-      <c r="N116" s="51"/>
-      <c r="O116" s="51"/>
-      <c r="Q116" s="52"/>
+    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B116" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D116" s="31" t="s">
+        <v>797</v>
+      </c>
+      <c r="E116" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="F116" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="G116" s="30"/>
+      <c r="H116" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I116" s="31"/>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B117" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D117" s="31" t="s">
-        <v>835</v>
-      </c>
-      <c r="E117" s="31" t="s">
-        <v>126</v>
+      <c r="D117" s="30" t="s">
+        <v>798</v>
+      </c>
+      <c r="E117" s="30" t="s">
+        <v>56</v>
       </c>
       <c r="F117" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H117" s="31" t="s">
-        <v>417</v>
-      </c>
-      <c r="I117" s="30" t="s">
-        <v>418</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="G117" s="30" t="s">
+        <v>796</v>
+      </c>
+      <c r="H117" s="31">
+        <v>15</v>
+      </c>
+      <c r="I117" s="31"/>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B118" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D118" s="31" t="s">
-        <v>841</v>
-      </c>
-      <c r="E118" s="31" t="s">
-        <v>219</v>
+      <c r="D118" s="30" t="s">
+        <v>851</v>
+      </c>
+      <c r="E118" s="30" t="s">
+        <v>58</v>
       </c>
       <c r="F118" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H118" s="31" t="s">
-        <v>839</v>
-      </c>
-      <c r="I118" s="30" t="s">
-        <v>840</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="G118" s="30" t="s">
+        <v>792</v>
+      </c>
+      <c r="H118" s="31">
+        <v>0</v>
+      </c>
+      <c r="I118" s="31"/>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B119" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D119" s="31" t="s">
-        <v>842</v>
-      </c>
-      <c r="E119" s="31" t="s">
-        <v>221</v>
+      <c r="D119" s="30" t="s">
+        <v>800</v>
+      </c>
+      <c r="E119" s="30" t="s">
+        <v>60</v>
       </c>
       <c r="F119" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G119" s="31" t="s">
-        <v>843</v>
+        <v>65</v>
+      </c>
+      <c r="G119" s="30" t="s">
+        <v>796</v>
       </c>
       <c r="H119" s="31">
-        <v>69</v>
+        <v>1</v>
       </c>
       <c r="I119" s="31"/>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B120" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D120" s="31" t="s">
-        <v>845</v>
-      </c>
-      <c r="E120" s="31" t="s">
-        <v>223</v>
-      </c>
-      <c r="F120" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G120" s="31" t="s">
-        <v>844</v>
-      </c>
-      <c r="H120" s="31">
-        <v>28</v>
-      </c>
-      <c r="I120" s="31"/>
+    <row r="120" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="B120" s="49" t="s">
+        <v>216</v>
+      </c>
+      <c r="C120" s="49" t="s">
+        <v>217</v>
+      </c>
+      <c r="D120" s="49" t="s">
+        <v>217</v>
+      </c>
+      <c r="E120" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="J120" s="50"/>
+      <c r="K120" s="51"/>
+      <c r="L120" s="51"/>
+      <c r="M120" s="51"/>
+      <c r="N120" s="51"/>
+      <c r="O120" s="51"/>
+      <c r="Q120" s="52"/>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B121" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D121" s="31" t="s">
-        <v>846</v>
+        <v>835</v>
       </c>
       <c r="E121" s="31" t="s">
-        <v>225</v>
+        <v>126</v>
       </c>
       <c r="F121" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G121" s="31" t="s">
-        <v>843</v>
-      </c>
-      <c r="H121" s="31">
-        <v>55</v>
-      </c>
-      <c r="I121" s="31"/>
+        <v>62</v>
+      </c>
+      <c r="H121" s="31" t="s">
+        <v>417</v>
+      </c>
+      <c r="I121" s="30" t="s">
+        <v>418</v>
+      </c>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B122" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D122" s="31" t="s">
-        <v>847</v>
+        <v>841</v>
       </c>
       <c r="E122" s="31" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="F122" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G122" s="31" t="s">
-        <v>843</v>
-      </c>
-      <c r="H122" s="31">
-        <v>-148</v>
-      </c>
-      <c r="I122" s="31"/>
+        <v>62</v>
+      </c>
+      <c r="H122" s="31" t="s">
+        <v>839</v>
+      </c>
+      <c r="I122" s="30" t="s">
+        <v>840</v>
+      </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B123" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D123" s="31" t="s">
-        <v>836</v>
+        <v>842</v>
       </c>
       <c r="E123" s="31" t="s">
-        <v>91</v>
+        <v>221</v>
       </c>
       <c r="F123" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="H123" s="31" t="b">
-        <v>0</v>
+        <v>64</v>
+      </c>
+      <c r="G123" s="31" t="s">
+        <v>843</v>
+      </c>
+      <c r="H123" s="31">
+        <v>69</v>
       </c>
       <c r="I123" s="31"/>
     </row>
@@ -10057,16 +10106,19 @@
         <v>21</v>
       </c>
       <c r="D124" s="31" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="E124" s="31" t="s">
-        <v>128</v>
+        <v>223</v>
       </c>
       <c r="F124" s="30" t="s">
         <v>64</v>
       </c>
+      <c r="G124" s="31" t="s">
+        <v>844</v>
+      </c>
       <c r="H124" s="31">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="I124" s="31"/>
     </row>
@@ -10075,16 +10127,19 @@
         <v>21</v>
       </c>
       <c r="D125" s="31" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="E125" s="31" t="s">
-        <v>50</v>
+        <v>225</v>
       </c>
       <c r="F125" s="30" t="s">
         <v>64</v>
       </c>
+      <c r="G125" s="31" t="s">
+        <v>843</v>
+      </c>
       <c r="H125" s="31">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="I125" s="31"/>
     </row>
@@ -10093,19 +10148,19 @@
         <v>21</v>
       </c>
       <c r="D126" s="31" t="s">
-        <v>795</v>
+        <v>847</v>
       </c>
       <c r="E126" s="31" t="s">
-        <v>52</v>
+        <v>227</v>
       </c>
       <c r="F126" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G126" s="30" t="s">
-        <v>796</v>
+        <v>64</v>
+      </c>
+      <c r="G126" s="31" t="s">
+        <v>843</v>
       </c>
       <c r="H126" s="31">
-        <v>0</v>
+        <v>-148</v>
       </c>
       <c r="I126" s="31"/>
     </row>
@@ -10114,15 +10169,14 @@
         <v>21</v>
       </c>
       <c r="D127" s="31" t="s">
-        <v>797</v>
+        <v>836</v>
       </c>
       <c r="E127" s="31" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="F127" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="G127" s="30"/>
       <c r="H127" s="31" t="b">
         <v>0</v>
       </c>
@@ -10132,20 +10186,17 @@
       <c r="B128" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D128" s="30" t="s">
-        <v>798</v>
-      </c>
-      <c r="E128" s="30" t="s">
-        <v>56</v>
+      <c r="D128" s="31" t="s">
+        <v>848</v>
+      </c>
+      <c r="E128" s="31" t="s">
+        <v>128</v>
       </c>
       <c r="F128" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G128" s="30" t="s">
-        <v>796</v>
+        <v>64</v>
       </c>
       <c r="H128" s="31">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I128" s="31"/>
     </row>
@@ -10153,17 +10204,14 @@
       <c r="B129" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D129" s="30" t="s">
-        <v>850</v>
-      </c>
-      <c r="E129" s="30" t="s">
-        <v>58</v>
+      <c r="D129" s="31" t="s">
+        <v>849</v>
+      </c>
+      <c r="E129" s="31" t="s">
+        <v>50</v>
       </c>
       <c r="F129" s="30" t="s">
         <v>64</v>
-      </c>
-      <c r="G129" s="30" t="s">
-        <v>792</v>
       </c>
       <c r="H129" s="31">
         <v>0</v>
@@ -10174,11 +10222,11 @@
       <c r="B130" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D130" s="30" t="s">
-        <v>800</v>
-      </c>
-      <c r="E130" s="30" t="s">
-        <v>60</v>
+      <c r="D130" s="31" t="s">
+        <v>795</v>
+      </c>
+      <c r="E130" s="31" t="s">
+        <v>52</v>
       </c>
       <c r="F130" s="30" t="s">
         <v>65</v>
@@ -10187,24 +10235,90 @@
         <v>796</v>
       </c>
       <c r="H130" s="31">
+        <v>0</v>
+      </c>
+      <c r="I130" s="31"/>
+    </row>
+    <row r="131" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B131" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D131" s="31" t="s">
+        <v>797</v>
+      </c>
+      <c r="E131" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="F131" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="G131" s="30"/>
+      <c r="H131" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I131" s="31"/>
+    </row>
+    <row r="132" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B132" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D132" s="30" t="s">
+        <v>798</v>
+      </c>
+      <c r="E132" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F132" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G132" s="30" t="s">
+        <v>796</v>
+      </c>
+      <c r="H132" s="31">
+        <v>15</v>
+      </c>
+      <c r="I132" s="31"/>
+    </row>
+    <row r="133" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B133" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D133" s="30" t="s">
+        <v>850</v>
+      </c>
+      <c r="E133" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F133" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G133" s="30" t="s">
+        <v>792</v>
+      </c>
+      <c r="H133" s="31">
+        <v>0</v>
+      </c>
+      <c r="I133" s="31"/>
+    </row>
+    <row r="134" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B134" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D134" s="30" t="s">
+        <v>800</v>
+      </c>
+      <c r="E134" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="F134" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G134" s="30" t="s">
+        <v>796</v>
+      </c>
+      <c r="H134" s="31">
         <v>1</v>
       </c>
-      <c r="I130" s="31"/>
-    </row>
-    <row r="131" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H131" s="31"/>
-      <c r="I131" s="31"/>
-    </row>
-    <row r="132" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H132" s="31"/>
-      <c r="I132" s="31"/>
-    </row>
-    <row r="133" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H133" s="31"/>
-      <c r="I133" s="31"/>
-    </row>
-    <row r="134" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H134" s="31"/>
       <c r="I134" s="31"/>
     </row>
     <row r="135" spans="2:9" x14ac:dyDescent="0.25">
@@ -10515,8 +10629,24 @@
       <c r="H211" s="31"/>
       <c r="I211" s="31"/>
     </row>
+    <row r="212" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H212" s="31"/>
+      <c r="I212" s="31"/>
+    </row>
+    <row r="213" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H213" s="31"/>
+      <c r="I213" s="31"/>
+    </row>
+    <row r="214" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H214" s="31"/>
+      <c r="I214" s="31"/>
+    </row>
+    <row r="215" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H215" s="31"/>
+      <c r="I215" s="31"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:Z138"/>
+  <autoFilter ref="A2:Z142"/>
   <mergeCells count="1">
     <mergeCell ref="T1:Y1"/>
   </mergeCells>

</xml_diff>

<commit_message>
Adding Building Rotation to repo and office_ee.xlsx
I added this to model 0 in the workflow prior to running WWR measures.
</commit_message>
<xml_diff>
--- a/projects/office_ee.xlsx
+++ b/projects/office_ee.xlsx
@@ -16,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$142</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$144</definedName>
     <definedName name="AnalysisType">Lookups!$A$17:$A$23</definedName>
     <definedName name="instance_defs">Lookups!$A$2:$D$9</definedName>
     <definedName name="instance_types">Lookups!$A$2:$A$9</definedName>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2743" uniqueCount="871">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2752" uniqueCount="874">
   <si>
     <t>type</t>
   </si>
@@ -2654,6 +2654,15 @@
   </si>
   <si>
     <t>Percentage Increase of R-value for Exterior Wall Insulation</t>
+  </si>
+  <si>
+    <t>Rotate Building</t>
+  </si>
+  <si>
+    <t>Number of Degrees to Rotate Building positive value is clockwise</t>
+  </si>
+  <si>
+    <t>degrees</t>
   </si>
 </sst>
 </file>
@@ -7333,11 +7342,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y215"/>
+  <dimension ref="A1:Y217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D93" sqref="D93"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8069,13 +8078,13 @@
         <v>1</v>
       </c>
       <c r="B36" s="38" t="s">
-        <v>680</v>
+        <v>871</v>
       </c>
       <c r="C36" s="38" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D36" s="38" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E36" s="38" t="s">
         <v>68</v>
@@ -8088,72 +8097,56 @@
         <v>21</v>
       </c>
       <c r="D37" s="31" t="s">
-        <v>683</v>
+        <v>872</v>
       </c>
       <c r="E37" s="31" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F37" s="31" t="s">
         <v>619</v>
       </c>
+      <c r="G37" s="31" t="s">
+        <v>873</v>
+      </c>
       <c r="H37" s="31">
-        <v>0.4</v>
-      </c>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-      <c r="N37" s="3"/>
-      <c r="P37" s="40"/>
-      <c r="Q37" s="2"/>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B38" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D38" s="31" t="s">
-        <v>667</v>
-      </c>
-      <c r="E38" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="F38" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="G38" s="31" t="s">
-        <v>668</v>
-      </c>
-      <c r="H38" s="31">
-        <v>30</v>
-      </c>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3"/>
-      <c r="P38" s="40"/>
-      <c r="Q38" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="I37" s="31"/>
+    </row>
+    <row r="38" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="B38" s="38" t="s">
+        <v>680</v>
+      </c>
+      <c r="C38" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="D38" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="E38" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="G38" s="39"/>
+      <c r="H38" s="39"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B39" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D39" s="31" t="s">
-        <v>672</v>
+        <v>683</v>
       </c>
       <c r="E39" s="31" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F39" s="31" t="s">
-        <v>618</v>
-      </c>
-      <c r="G39" s="31" t="s">
-        <v>668</v>
-      </c>
-      <c r="H39" s="31" t="s">
-        <v>669</v>
+        <v>619</v>
+      </c>
+      <c r="H39" s="31">
+        <v>0.4</v>
       </c>
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
@@ -8164,40 +8157,52 @@
       <c r="P39" s="40"/>
       <c r="Q39" s="2"/>
     </row>
-    <row r="40" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="B40" s="38" t="s">
-        <v>687</v>
-      </c>
-      <c r="C40" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="D40" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="E40" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="G40" s="39"/>
-      <c r="H40" s="39"/>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B40" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="31" t="s">
+        <v>667</v>
+      </c>
+      <c r="E40" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="F40" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="G40" s="31" t="s">
+        <v>668</v>
+      </c>
+      <c r="H40" s="31">
+        <v>30</v>
+      </c>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
+      <c r="P40" s="40"/>
+      <c r="Q40" s="2"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B41" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D41" s="31" t="s">
-        <v>684</v>
+        <v>672</v>
       </c>
       <c r="E41" s="31" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F41" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="H41" s="31">
-        <v>0.4</v>
+        <v>618</v>
+      </c>
+      <c r="G41" s="31" t="s">
+        <v>668</v>
+      </c>
+      <c r="H41" s="31" t="s">
+        <v>669</v>
       </c>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
@@ -8208,52 +8213,40 @@
       <c r="P41" s="40"/>
       <c r="Q41" s="2"/>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B42" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D42" s="31" t="s">
-        <v>667</v>
-      </c>
-      <c r="E42" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="F42" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="G42" s="31" t="s">
-        <v>668</v>
-      </c>
-      <c r="H42" s="31">
-        <v>30</v>
-      </c>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-      <c r="N42" s="3"/>
-      <c r="P42" s="40"/>
-      <c r="Q42" s="2"/>
+    <row r="42" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="B42" s="38" t="s">
+        <v>687</v>
+      </c>
+      <c r="C42" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="D42" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="E42" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="G42" s="39"/>
+      <c r="H42" s="39"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B43" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D43" s="31" t="s">
-        <v>673</v>
+        <v>684</v>
       </c>
       <c r="E43" s="31" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F43" s="31" t="s">
-        <v>618</v>
-      </c>
-      <c r="G43" s="31" t="s">
-        <v>668</v>
-      </c>
-      <c r="H43" s="31" t="s">
-        <v>82</v>
+        <v>619</v>
+      </c>
+      <c r="H43" s="31">
+        <v>0.4</v>
       </c>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
@@ -8264,40 +8257,52 @@
       <c r="P43" s="40"/>
       <c r="Q43" s="2"/>
     </row>
-    <row r="44" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="B44" s="38" t="s">
-        <v>688</v>
-      </c>
-      <c r="C44" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="D44" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="E44" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="G44" s="39"/>
-      <c r="H44" s="39"/>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B44" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" s="31" t="s">
+        <v>667</v>
+      </c>
+      <c r="E44" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="F44" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="G44" s="31" t="s">
+        <v>668</v>
+      </c>
+      <c r="H44" s="31">
+        <v>30</v>
+      </c>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="3"/>
+      <c r="P44" s="40"/>
+      <c r="Q44" s="2"/>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B45" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D45" s="31" t="s">
-        <v>685</v>
+        <v>673</v>
       </c>
       <c r="E45" s="31" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F45" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="H45" s="31">
-        <v>0.4</v>
+        <v>618</v>
+      </c>
+      <c r="G45" s="31" t="s">
+        <v>668</v>
+      </c>
+      <c r="H45" s="31" t="s">
+        <v>82</v>
       </c>
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
@@ -8308,52 +8313,40 @@
       <c r="P45" s="40"/>
       <c r="Q45" s="2"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B46" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D46" s="31" t="s">
-        <v>667</v>
-      </c>
-      <c r="E46" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="F46" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="G46" s="31" t="s">
-        <v>668</v>
-      </c>
-      <c r="H46" s="31">
-        <v>30</v>
-      </c>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
-      <c r="K46" s="3"/>
-      <c r="L46" s="3"/>
-      <c r="M46" s="3"/>
-      <c r="N46" s="3"/>
-      <c r="P46" s="40"/>
-      <c r="Q46" s="2"/>
+    <row r="46" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="B46" s="38" t="s">
+        <v>688</v>
+      </c>
+      <c r="C46" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="D46" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="E46" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="G46" s="39"/>
+      <c r="H46" s="39"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B47" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D47" s="31" t="s">
-        <v>674</v>
+        <v>685</v>
       </c>
       <c r="E47" s="31" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F47" s="31" t="s">
-        <v>618</v>
-      </c>
-      <c r="G47" s="31" t="s">
-        <v>668</v>
-      </c>
-      <c r="H47" s="31" t="s">
-        <v>670</v>
+        <v>619</v>
+      </c>
+      <c r="H47" s="31">
+        <v>0.4</v>
       </c>
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
@@ -8364,40 +8357,52 @@
       <c r="P47" s="40"/>
       <c r="Q47" s="2"/>
     </row>
-    <row r="48" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="B48" s="38" t="s">
-        <v>681</v>
-      </c>
-      <c r="C48" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="D48" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="E48" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="G48" s="39"/>
-      <c r="H48" s="39"/>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B48" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48" s="31" t="s">
+        <v>667</v>
+      </c>
+      <c r="E48" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="F48" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="G48" s="31" t="s">
+        <v>668</v>
+      </c>
+      <c r="H48" s="31">
+        <v>30</v>
+      </c>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
+      <c r="M48" s="3"/>
+      <c r="N48" s="3"/>
+      <c r="P48" s="40"/>
+      <c r="Q48" s="2"/>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B49" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D49" s="31" t="s">
-        <v>686</v>
+        <v>674</v>
       </c>
       <c r="E49" s="31" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F49" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="H49" s="31">
-        <v>0.4</v>
+        <v>618</v>
+      </c>
+      <c r="G49" s="31" t="s">
+        <v>668</v>
+      </c>
+      <c r="H49" s="31" t="s">
+        <v>670</v>
       </c>
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
@@ -8408,52 +8413,40 @@
       <c r="P49" s="40"/>
       <c r="Q49" s="2"/>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B50" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D50" s="31" t="s">
-        <v>667</v>
-      </c>
-      <c r="E50" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="F50" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="G50" s="31" t="s">
-        <v>668</v>
-      </c>
-      <c r="H50" s="31">
-        <v>30</v>
-      </c>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
-      <c r="K50" s="3"/>
-      <c r="L50" s="3"/>
-      <c r="M50" s="3"/>
-      <c r="N50" s="3"/>
-      <c r="P50" s="40"/>
-      <c r="Q50" s="2"/>
+    <row r="50" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="B50" s="38" t="s">
+        <v>681</v>
+      </c>
+      <c r="C50" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="D50" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="E50" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="G50" s="39"/>
+      <c r="H50" s="39"/>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B51" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D51" s="31" t="s">
-        <v>675</v>
+        <v>686</v>
       </c>
       <c r="E51" s="31" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F51" s="31" t="s">
-        <v>618</v>
-      </c>
-      <c r="G51" s="31" t="s">
-        <v>668</v>
-      </c>
-      <c r="H51" s="31" t="s">
-        <v>671</v>
+        <v>619</v>
+      </c>
+      <c r="H51" s="31">
+        <v>0.4</v>
       </c>
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
@@ -8464,76 +8457,96 @@
       <c r="P51" s="40"/>
       <c r="Q51" s="2"/>
     </row>
-    <row r="52" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="B52" s="38" t="s">
-        <v>691</v>
-      </c>
-      <c r="C52" s="38" t="s">
-        <v>690</v>
-      </c>
-      <c r="D52" s="38" t="s">
-        <v>690</v>
-      </c>
-      <c r="E52" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="G52" s="39"/>
-      <c r="H52" s="39"/>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B52" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D52" s="31" t="s">
+        <v>667</v>
+      </c>
+      <c r="E52" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="F52" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="G52" s="31" t="s">
+        <v>668</v>
+      </c>
+      <c r="H52" s="31">
+        <v>30</v>
+      </c>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3"/>
+      <c r="N52" s="3"/>
+      <c r="P52" s="40"/>
+      <c r="Q52" s="2"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B53" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D53" s="31" t="s">
-        <v>693</v>
+        <v>675</v>
       </c>
       <c r="E53" s="31" t="s">
-        <v>692</v>
+        <v>81</v>
       </c>
       <c r="F53" s="31" t="s">
         <v>618</v>
       </c>
+      <c r="G53" s="31" t="s">
+        <v>668</v>
+      </c>
       <c r="H53" s="31" t="s">
-        <v>702</v>
-      </c>
-      <c r="I53" s="31"/>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B54" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D54" s="31" t="s">
-        <v>695</v>
-      </c>
-      <c r="E54" s="31" t="s">
-        <v>694</v>
-      </c>
-      <c r="F54" s="31" t="s">
-        <v>618</v>
-      </c>
-      <c r="H54" s="31" t="s">
-        <v>703</v>
-      </c>
-      <c r="I54" s="31"/>
+        <v>671</v>
+      </c>
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="3"/>
+      <c r="L53" s="3"/>
+      <c r="M53" s="3"/>
+      <c r="N53" s="3"/>
+      <c r="P53" s="40"/>
+      <c r="Q53" s="2"/>
+    </row>
+    <row r="54" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="B54" s="38" t="s">
+        <v>691</v>
+      </c>
+      <c r="C54" s="38" t="s">
+        <v>690</v>
+      </c>
+      <c r="D54" s="38" t="s">
+        <v>690</v>
+      </c>
+      <c r="E54" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="G54" s="39"/>
+      <c r="H54" s="39"/>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B55" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D55" s="31" t="s">
-        <v>698</v>
+        <v>693</v>
       </c>
       <c r="E55" s="31" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="F55" s="31" t="s">
         <v>618</v>
       </c>
-      <c r="H55" s="41" t="s">
-        <v>701</v>
+      <c r="H55" s="31" t="s">
+        <v>702</v>
       </c>
       <c r="I55" s="31"/>
     </row>
@@ -8542,529 +8555,498 @@
         <v>21</v>
       </c>
       <c r="D56" s="31" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="E56" s="31" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="F56" s="31" t="s">
         <v>618</v>
       </c>
-      <c r="H56" s="41" t="s">
+      <c r="H56" s="31" t="s">
+        <v>703</v>
+      </c>
+      <c r="I56" s="31"/>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B57" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D57" s="31" t="s">
+        <v>698</v>
+      </c>
+      <c r="E57" s="31" t="s">
+        <v>696</v>
+      </c>
+      <c r="F57" s="31" t="s">
+        <v>618</v>
+      </c>
+      <c r="H57" s="41" t="s">
+        <v>701</v>
+      </c>
+      <c r="I57" s="31"/>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B58" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D58" s="31" t="s">
+        <v>699</v>
+      </c>
+      <c r="E58" s="31" t="s">
+        <v>697</v>
+      </c>
+      <c r="F58" s="31" t="s">
+        <v>618</v>
+      </c>
+      <c r="H58" s="41" t="s">
         <v>700</v>
       </c>
-      <c r="I56" s="31"/>
-    </row>
-    <row r="57" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="38" t="b">
+      <c r="I58" s="31"/>
+    </row>
+    <row r="59" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="38" t="b">
         <v>1</v>
       </c>
-      <c r="B57" s="38" t="s">
+      <c r="B59" s="38" t="s">
         <v>705</v>
       </c>
-      <c r="C57" s="38" t="s">
+      <c r="C59" s="38" t="s">
         <v>704</v>
       </c>
-      <c r="D57" s="38" t="s">
+      <c r="D59" s="38" t="s">
         <v>704</v>
       </c>
-      <c r="E57" s="38" t="s">
+      <c r="E59" s="38" t="s">
         <v>233</v>
       </c>
-      <c r="G57" s="39"/>
-      <c r="H57" s="39"/>
-    </row>
-    <row r="58" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="38" t="b">
+      <c r="G59" s="39"/>
+      <c r="H59" s="39"/>
+    </row>
+    <row r="60" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="38" t="b">
         <v>1</v>
       </c>
-      <c r="B58" s="38" t="s">
+      <c r="B60" s="38" t="s">
         <v>775</v>
       </c>
-      <c r="C58" s="38" t="s">
+      <c r="C60" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="D58" s="38" t="s">
+      <c r="D60" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="E58" s="38" t="s">
+      <c r="E60" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="G58" s="39"/>
-      <c r="H58" s="39"/>
-    </row>
-    <row r="59" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="D59" s="43" t="s">
+      <c r="G60" s="39"/>
+      <c r="H60" s="39"/>
+    </row>
+    <row r="61" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D61" s="43" t="s">
         <v>776</v>
       </c>
-      <c r="E59" s="43" t="s">
+      <c r="E61" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="F59" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="H59" s="43">
+      <c r="F61" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="H61" s="43">
         <v>0.44400000000000001</v>
       </c>
-      <c r="J59" s="43">
+      <c r="J61" s="43">
         <v>0.3</v>
       </c>
-      <c r="K59" s="43">
+      <c r="K61" s="43">
         <v>0.5</v>
       </c>
-      <c r="L59" s="43">
+      <c r="L61" s="43">
         <v>0.4</v>
       </c>
-      <c r="M59" s="43">
-        <f>(K59+J59)/6</f>
+      <c r="M61" s="43">
+        <f>(K61+J61)/6</f>
         <v>0.13333333333333333</v>
       </c>
-      <c r="N59" s="43">
+      <c r="N61" s="43">
         <v>0.01</v>
       </c>
-      <c r="Q59" s="43" t="s">
+      <c r="Q61" s="43" t="s">
         <v>777</v>
       </c>
     </row>
-    <row r="60" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D60" s="30" t="s">
+    <row r="62" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D62" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="E60" s="30" t="s">
+      <c r="E62" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="F60" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="H60" s="30">
+      <c r="F62" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="H62" s="30">
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D61" s="30" t="s">
+    <row r="63" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D63" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="E61" s="30" t="s">
+      <c r="E63" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="F61" s="30" t="s">
+      <c r="F63" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="H61" s="30" t="s">
+      <c r="H63" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="I61" s="30" t="s">
+      <c r="I63" s="30" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="62" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="38" t="b">
+    <row r="64" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="38" t="b">
         <v>1</v>
       </c>
-      <c r="B62" s="38" t="s">
+      <c r="B64" s="38" t="s">
         <v>778</v>
       </c>
-      <c r="C62" s="38" t="s">
+      <c r="C64" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="D62" s="38" t="s">
+      <c r="D64" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="E62" s="38" t="s">
+      <c r="E64" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="G62" s="39"/>
-      <c r="H62" s="39"/>
-    </row>
-    <row r="63" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="D63" s="43" t="s">
+      <c r="G64" s="39"/>
+      <c r="H64" s="39"/>
+    </row>
+    <row r="65" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D65" s="43" t="s">
         <v>779</v>
       </c>
-      <c r="E63" s="43" t="s">
+      <c r="E65" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="F63" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="H63" s="43">
+      <c r="F65" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="H65" s="43">
         <v>0.2</v>
       </c>
-      <c r="J63" s="43">
+      <c r="J65" s="43">
         <v>0.3</v>
       </c>
-      <c r="K63" s="43">
+      <c r="K65" s="43">
         <v>0.5</v>
       </c>
-      <c r="L63" s="43">
+      <c r="L65" s="43">
         <v>0.4</v>
       </c>
-      <c r="M63" s="43">
-        <f>(K63+J63)/6</f>
+      <c r="M65" s="43">
+        <f>(K65+J65)/6</f>
         <v>0.13333333333333333</v>
       </c>
-      <c r="N63" s="43">
+      <c r="N65" s="43">
         <v>0.01</v>
       </c>
-      <c r="Q63" s="43" t="s">
+      <c r="Q65" s="43" t="s">
         <v>777</v>
       </c>
     </row>
-    <row r="64" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D64" s="30" t="s">
+    <row r="66" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D66" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="E64" s="30" t="s">
+      <c r="E66" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="F64" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="H64" s="30">
+      <c r="F66" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="H66" s="30">
         <v>30</v>
       </c>
     </row>
-    <row r="65" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D65" s="30" t="s">
+    <row r="67" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D67" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="E65" s="30" t="s">
+      <c r="E67" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="F65" s="30" t="s">
+      <c r="F67" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="H65" s="30" t="s">
+      <c r="H67" s="30" t="s">
         <v>670</v>
       </c>
-      <c r="I65" s="30" t="s">
+      <c r="I67" s="30" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="38" t="b">
+    <row r="68" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="38" t="b">
         <v>1</v>
       </c>
-      <c r="B66" s="38" t="s">
+      <c r="B68" s="38" t="s">
         <v>780</v>
       </c>
-      <c r="C66" s="38" t="s">
+      <c r="C68" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="D66" s="38" t="s">
+      <c r="D68" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="E66" s="38" t="s">
+      <c r="E68" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="G66" s="39"/>
-      <c r="H66" s="39"/>
-    </row>
-    <row r="67" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="D67" s="43" t="s">
+      <c r="G68" s="39"/>
+      <c r="H68" s="39"/>
+    </row>
+    <row r="69" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D69" s="43" t="s">
         <v>781</v>
       </c>
-      <c r="E67" s="43" t="s">
+      <c r="E69" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="F67" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="H67" s="43">
+      <c r="F69" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="H69" s="43">
         <v>0.3</v>
       </c>
-      <c r="J67" s="43">
+      <c r="J69" s="43">
         <v>0.3</v>
       </c>
-      <c r="K67" s="43">
+      <c r="K69" s="43">
         <v>0.5</v>
       </c>
-      <c r="L67" s="43">
+      <c r="L69" s="43">
         <v>0.4</v>
       </c>
-      <c r="M67" s="43">
-        <f>(K67+J67)/6</f>
+      <c r="M69" s="43">
+        <f>(K69+J69)/6</f>
         <v>0.13333333333333333</v>
       </c>
-      <c r="N67" s="43">
+      <c r="N69" s="43">
         <v>0.01</v>
       </c>
-      <c r="Q67" s="43" t="s">
+      <c r="Q69" s="43" t="s">
         <v>777</v>
       </c>
     </row>
-    <row r="68" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D68" s="30" t="s">
+    <row r="70" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D70" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="E68" s="30" t="s">
+      <c r="E70" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="F68" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="H68" s="30">
+      <c r="F70" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="H70" s="30">
         <v>30</v>
       </c>
-    </row>
-    <row r="69" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D69" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="E69" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="F69" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H69" s="30" t="s">
-        <v>671</v>
-      </c>
-      <c r="I69" s="30" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="70" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="B70" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="C70" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="D70" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="E70" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="G70" s="39"/>
-      <c r="H70" s="39"/>
     </row>
     <row r="71" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B71" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D71" s="30" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="E71" s="30" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="F71" s="30" t="s">
         <v>62</v>
       </c>
       <c r="H71" s="30" t="s">
-        <v>66</v>
+        <v>671</v>
       </c>
       <c r="I71" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="O71" s="31"/>
-    </row>
-    <row r="72" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="D72" s="44" t="s">
-        <v>782</v>
-      </c>
-      <c r="E72" s="43" t="s">
-        <v>70</v>
-      </c>
-      <c r="F72" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="H72" s="43">
-        <v>-20</v>
-      </c>
-      <c r="J72" s="45">
-        <v>-100</v>
-      </c>
-      <c r="K72" s="45">
-        <v>100</v>
-      </c>
-      <c r="L72" s="45">
-        <v>0</v>
-      </c>
-      <c r="M72" s="45">
-        <f>(K72-J72)/6</f>
-        <v>33.333333333333336</v>
-      </c>
-      <c r="N72" s="45">
-        <v>2.5</v>
-      </c>
-      <c r="Q72" s="43" t="s">
-        <v>777</v>
-      </c>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="B72" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="C72" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="D72" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="E72" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="G72" s="39"/>
+      <c r="H72" s="39"/>
     </row>
     <row r="73" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D73" s="30" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="E73" s="30" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F73" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="H73" s="30">
-        <v>0</v>
+        <v>62</v>
+      </c>
+      <c r="H73" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="I73" s="30" t="s">
+        <v>83</v>
       </c>
       <c r="O73" s="31"/>
     </row>
-    <row r="74" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D74" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="E74" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="F74" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="H74" s="30">
-        <v>0</v>
-      </c>
-      <c r="O74" s="31"/>
+    <row r="74" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D74" s="44" t="s">
+        <v>782</v>
+      </c>
+      <c r="E74" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="F74" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="H74" s="43">
+        <v>-20</v>
+      </c>
+      <c r="J74" s="45">
+        <v>-100</v>
+      </c>
+      <c r="K74" s="45">
+        <v>100</v>
+      </c>
+      <c r="L74" s="45">
+        <v>0</v>
+      </c>
+      <c r="M74" s="45">
+        <f>(K74-J74)/6</f>
+        <v>33.333333333333336</v>
+      </c>
+      <c r="N74" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q74" s="43" t="s">
+        <v>777</v>
+      </c>
     </row>
     <row r="75" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B75" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D75" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="E75" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="F75" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="H75" s="30">
+        <v>0</v>
+      </c>
+      <c r="O75" s="31"/>
+    </row>
+    <row r="76" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D76" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="E76" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F76" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="H76" s="30">
+        <v>0</v>
+      </c>
+      <c r="O76" s="31"/>
+    </row>
+    <row r="77" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B77" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D77" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="E75" s="30" t="s">
+      <c r="E77" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="F75" s="30" t="s">
+      <c r="F77" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="H75" s="30">
+      <c r="H77" s="30">
         <v>1</v>
       </c>
-      <c r="O75" s="31"/>
-    </row>
-    <row r="76" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="38" t="b">
+      <c r="O77" s="31"/>
+    </row>
+    <row r="78" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="38" t="b">
         <v>1</v>
       </c>
-      <c r="B76" s="38" t="s">
+      <c r="B78" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="C76" s="38" t="s">
+      <c r="C78" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="D76" s="38" t="s">
+      <c r="D78" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="E76" s="38" t="s">
+      <c r="E78" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="G76" s="39"/>
-      <c r="H76" s="39"/>
-    </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A77" s="30"/>
-      <c r="B77" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C77" s="30"/>
-      <c r="D77" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="E77" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="F77" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="G77" s="30"/>
-      <c r="H77" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="I77" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="J77" s="3"/>
-      <c r="K77" s="3"/>
-      <c r="L77" s="3"/>
-      <c r="M77" s="3"/>
-      <c r="N77" s="3"/>
-      <c r="P77" s="40"/>
-    </row>
-    <row r="78" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="D78" s="43" t="s">
-        <v>783</v>
-      </c>
-      <c r="E78" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="F78" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="H78" s="43">
-        <v>30</v>
-      </c>
-      <c r="I78" s="46"/>
-      <c r="J78" s="45">
-        <v>-40</v>
-      </c>
-      <c r="K78" s="45">
-        <v>40</v>
-      </c>
-      <c r="L78" s="45">
-        <v>-1</v>
-      </c>
-      <c r="M78" s="45">
-        <f>(K78-J78)/6</f>
-        <v>13.333333333333334</v>
-      </c>
-      <c r="N78" s="45">
-        <v>2.5</v>
-      </c>
-      <c r="P78" s="47"/>
-      <c r="Q78" s="43" t="s">
-        <v>24</v>
-      </c>
+      <c r="G78" s="39"/>
+      <c r="H78" s="39"/>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" s="30"/>
@@ -9072,18 +9054,21 @@
         <v>21</v>
       </c>
       <c r="C79" s="30"/>
-      <c r="D79" s="48" t="s">
-        <v>47</v>
+      <c r="D79" s="30" t="s">
+        <v>44</v>
       </c>
       <c r="E79" s="30" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F79" s="30" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G79" s="30"/>
-      <c r="H79" s="30">
-        <v>0</v>
+      <c r="H79" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="I79" s="30" t="s">
+        <v>83</v>
       </c>
       <c r="J79" s="3"/>
       <c r="K79" s="3"/>
@@ -9092,31 +9077,43 @@
       <c r="N79" s="3"/>
       <c r="P79" s="40"/>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A80" s="30"/>
-      <c r="B80" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C80" s="30"/>
-      <c r="D80" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="E80" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="F80" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G80" s="30"/>
-      <c r="H80" s="30">
-        <v>0</v>
-      </c>
-      <c r="J80" s="3"/>
-      <c r="K80" s="3"/>
-      <c r="L80" s="3"/>
-      <c r="M80" s="3"/>
-      <c r="N80" s="3"/>
-      <c r="P80" s="40"/>
+    <row r="80" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D80" s="43" t="s">
+        <v>783</v>
+      </c>
+      <c r="E80" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="F80" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="H80" s="43">
+        <v>30</v>
+      </c>
+      <c r="I80" s="46"/>
+      <c r="J80" s="45">
+        <v>-40</v>
+      </c>
+      <c r="K80" s="45">
+        <v>40</v>
+      </c>
+      <c r="L80" s="45">
+        <v>-1</v>
+      </c>
+      <c r="M80" s="45">
+        <f>(K80-J80)/6</f>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="N80" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="P80" s="47"/>
+      <c r="Q80" s="43" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" s="30"/>
@@ -9124,14 +9121,14 @@
         <v>21</v>
       </c>
       <c r="C81" s="30"/>
-      <c r="D81" s="30" t="s">
-        <v>51</v>
+      <c r="D81" s="48" t="s">
+        <v>47</v>
       </c>
       <c r="E81" s="30" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F81" s="30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G81" s="30"/>
       <c r="H81" s="30">
@@ -9151,17 +9148,17 @@
       </c>
       <c r="C82" s="30"/>
       <c r="D82" s="30" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E82" s="30" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F82" s="30" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G82" s="30"/>
-      <c r="H82" s="30" t="b">
-        <v>1</v>
+      <c r="H82" s="30">
+        <v>0</v>
       </c>
       <c r="J82" s="3"/>
       <c r="K82" s="3"/>
@@ -9177,17 +9174,17 @@
       </c>
       <c r="C83" s="30"/>
       <c r="D83" s="30" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E83" s="30" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F83" s="30" t="s">
         <v>65</v>
       </c>
       <c r="G83" s="30"/>
       <c r="H83" s="30">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="J83" s="3"/>
       <c r="K83" s="3"/>
@@ -9203,17 +9200,17 @@
       </c>
       <c r="C84" s="30"/>
       <c r="D84" s="30" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E84" s="30" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F84" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G84" s="30"/>
-      <c r="H84" s="30">
-        <v>0</v>
+      <c r="H84" s="30" t="b">
+        <v>1</v>
       </c>
       <c r="J84" s="3"/>
       <c r="K84" s="3"/>
@@ -9229,17 +9226,17 @@
       </c>
       <c r="C85" s="30"/>
       <c r="D85" s="30" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E85" s="30" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F85" s="30" t="s">
         <v>65</v>
       </c>
       <c r="G85" s="30"/>
       <c r="H85" s="30">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="J85" s="3"/>
       <c r="K85" s="3"/>
@@ -9248,24 +9245,31 @@
       <c r="N85" s="3"/>
       <c r="P85" s="40"/>
     </row>
-    <row r="86" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="B86" s="38" t="s">
-        <v>327</v>
-      </c>
-      <c r="C86" s="38" t="s">
-        <v>328</v>
-      </c>
-      <c r="D86" s="38" t="s">
-        <v>328</v>
-      </c>
-      <c r="E86" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="G86" s="39"/>
-      <c r="H86" s="39"/>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A86" s="30"/>
+      <c r="B86" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C86" s="30"/>
+      <c r="D86" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="E86" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F86" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G86" s="30"/>
+      <c r="H86" s="30">
+        <v>0</v>
+      </c>
+      <c r="J86" s="3"/>
+      <c r="K86" s="3"/>
+      <c r="L86" s="3"/>
+      <c r="M86" s="3"/>
+      <c r="N86" s="3"/>
+      <c r="P86" s="40"/>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" s="30"/>
@@ -9274,20 +9278,17 @@
       </c>
       <c r="C87" s="30"/>
       <c r="D87" s="30" t="s">
-        <v>373</v>
+        <v>59</v>
       </c>
       <c r="E87" s="30" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="F87" s="30" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="G87" s="30"/>
-      <c r="H87" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="I87" s="30" t="s">
-        <v>83</v>
+      <c r="H87" s="30">
+        <v>1</v>
       </c>
       <c r="J87" s="3"/>
       <c r="K87" s="3"/>
@@ -9296,71 +9297,63 @@
       <c r="N87" s="3"/>
       <c r="P87" s="40"/>
     </row>
-    <row r="88" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="D88" s="43" t="s">
-        <v>864</v>
-      </c>
-      <c r="E88" s="43" t="s">
-        <v>330</v>
-      </c>
-      <c r="F88" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="H88" s="43">
-        <v>30</v>
-      </c>
-      <c r="I88" s="46"/>
-      <c r="J88" s="45">
-        <v>-100</v>
-      </c>
-      <c r="K88" s="45">
-        <v>100</v>
-      </c>
-      <c r="L88" s="45">
-        <v>0</v>
-      </c>
-      <c r="M88" s="45">
-        <f>(K88-J88)/6</f>
-        <v>33.333333333333336</v>
-      </c>
-      <c r="N88" s="45">
-        <v>2.5</v>
-      </c>
-      <c r="Q88" s="43" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="89" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="38" t="b">
+    <row r="88" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="38" t="b">
         <v>1</v>
       </c>
-      <c r="B89" s="38" t="s">
-        <v>867</v>
-      </c>
-      <c r="C89" s="38" t="s">
-        <v>865</v>
-      </c>
-      <c r="D89" s="38" t="s">
-        <v>865</v>
-      </c>
-      <c r="E89" s="38" t="s">
+      <c r="B88" s="38" t="s">
+        <v>327</v>
+      </c>
+      <c r="C88" s="38" t="s">
+        <v>328</v>
+      </c>
+      <c r="D88" s="38" t="s">
+        <v>328</v>
+      </c>
+      <c r="E88" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="G89" s="39"/>
-      <c r="H89" s="39"/>
+      <c r="G88" s="39"/>
+      <c r="H88" s="39"/>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A89" s="30"/>
+      <c r="B89" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C89" s="30"/>
+      <c r="D89" s="30" t="s">
+        <v>373</v>
+      </c>
+      <c r="E89" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F89" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="G89" s="30"/>
+      <c r="H89" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="I89" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="J89" s="3"/>
+      <c r="K89" s="3"/>
+      <c r="L89" s="3"/>
+      <c r="M89" s="3"/>
+      <c r="N89" s="3"/>
+      <c r="P89" s="40"/>
     </row>
     <row r="90" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B90" s="43" t="s">
         <v>21</v>
       </c>
       <c r="D90" s="43" t="s">
-        <v>869</v>
+        <v>864</v>
       </c>
       <c r="E90" s="43" t="s">
-        <v>258</v>
+        <v>330</v>
       </c>
       <c r="F90" s="43" t="s">
         <v>64</v>
@@ -9394,13 +9387,13 @@
         <v>1</v>
       </c>
       <c r="B91" s="38" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="C91" s="38" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="D91" s="38" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="E91" s="38" t="s">
         <v>68</v>
@@ -9413,7 +9406,7 @@
         <v>21</v>
       </c>
       <c r="D92" s="43" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="E92" s="43" t="s">
         <v>258</v>
@@ -9445,71 +9438,85 @@
         <v>777</v>
       </c>
     </row>
-    <row r="93" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="49" t="b">
+    <row r="93" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="38" t="b">
         <v>1</v>
       </c>
-      <c r="B93" s="49" t="s">
+      <c r="B93" s="38" t="s">
+        <v>868</v>
+      </c>
+      <c r="C93" s="38" t="s">
+        <v>866</v>
+      </c>
+      <c r="D93" s="38" t="s">
+        <v>866</v>
+      </c>
+      <c r="E93" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="G93" s="39"/>
+      <c r="H93" s="39"/>
+    </row>
+    <row r="94" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B94" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D94" s="43" t="s">
+        <v>870</v>
+      </c>
+      <c r="E94" s="43" t="s">
+        <v>258</v>
+      </c>
+      <c r="F94" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="H94" s="43">
+        <v>30</v>
+      </c>
+      <c r="I94" s="46"/>
+      <c r="J94" s="45">
+        <v>-100</v>
+      </c>
+      <c r="K94" s="45">
+        <v>100</v>
+      </c>
+      <c r="L94" s="45">
+        <v>0</v>
+      </c>
+      <c r="M94" s="45">
+        <f>(K94-J94)/6</f>
+        <v>33.333333333333336</v>
+      </c>
+      <c r="N94" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q94" s="43" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="B95" s="49" t="s">
         <v>855</v>
       </c>
-      <c r="C93" s="49" t="s">
+      <c r="C95" s="49" t="s">
         <v>854</v>
       </c>
-      <c r="D93" s="49" t="s">
+      <c r="D95" s="49" t="s">
         <v>854</v>
       </c>
-      <c r="E93" s="49" t="s">
+      <c r="E95" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="J93" s="50"/>
-      <c r="K93" s="51"/>
-      <c r="L93" s="51"/>
-      <c r="M93" s="51"/>
-      <c r="N93" s="51"/>
-      <c r="O93" s="51"/>
-      <c r="Q93" s="52"/>
-    </row>
-    <row r="94" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="18"/>
-      <c r="B94" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D94" s="30" t="s">
-        <v>860</v>
-      </c>
-      <c r="E94" s="30" t="s">
-        <v>856</v>
-      </c>
-      <c r="F94" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G94" s="30" t="s">
-        <v>852</v>
-      </c>
-      <c r="H94" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="18"/>
-      <c r="B95" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D95" s="30" t="s">
-        <v>861</v>
-      </c>
-      <c r="E95" s="30" t="s">
-        <v>857</v>
-      </c>
-      <c r="F95" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G95" s="30" t="s">
-        <v>853</v>
-      </c>
-      <c r="H95" s="30">
-        <v>1</v>
-      </c>
+      <c r="J95" s="50"/>
+      <c r="K95" s="51"/>
+      <c r="L95" s="51"/>
+      <c r="M95" s="51"/>
+      <c r="N95" s="51"/>
+      <c r="O95" s="51"/>
+      <c r="Q95" s="52"/>
     </row>
     <row r="96" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="18"/>
@@ -9517,10 +9524,10 @@
         <v>21</v>
       </c>
       <c r="D96" s="30" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="E96" s="30" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="F96" s="30" t="s">
         <v>65</v>
@@ -9529,7 +9536,7 @@
         <v>852</v>
       </c>
       <c r="H96" s="30">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -9538,10 +9545,10 @@
         <v>21</v>
       </c>
       <c r="D97" s="30" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="E97" s="30" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="F97" s="30" t="s">
         <v>65</v>
@@ -9550,172 +9557,174 @@
         <v>853</v>
       </c>
       <c r="H97" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="18"/>
+      <c r="B98" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D98" s="30" t="s">
+        <v>862</v>
+      </c>
+      <c r="E98" s="30" t="s">
+        <v>858</v>
+      </c>
+      <c r="F98" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G98" s="30" t="s">
+        <v>852</v>
+      </c>
+      <c r="H98" s="30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="18"/>
+      <c r="B99" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D99" s="30" t="s">
+        <v>863</v>
+      </c>
+      <c r="E99" s="30" t="s">
+        <v>859</v>
+      </c>
+      <c r="F99" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G99" s="30" t="s">
+        <v>853</v>
+      </c>
+      <c r="H99" s="30">
         <v>31</v>
       </c>
     </row>
-    <row r="98" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="49" t="b">
+    <row r="100" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="49" t="b">
         <v>1</v>
       </c>
-      <c r="B98" s="49" t="s">
+      <c r="B100" s="49" t="s">
         <v>804</v>
       </c>
-      <c r="C98" s="49" t="s">
+      <c r="C100" s="49" t="s">
         <v>803</v>
       </c>
-      <c r="D98" s="49" t="s">
+      <c r="D100" s="49" t="s">
         <v>803</v>
       </c>
-      <c r="E98" s="49" t="s">
+      <c r="E100" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="J98" s="50"/>
-      <c r="K98" s="51"/>
-      <c r="L98" s="51"/>
-      <c r="M98" s="51"/>
-      <c r="N98" s="51"/>
-      <c r="O98" s="51"/>
-      <c r="Q98" s="52"/>
-    </row>
-    <row r="99" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="49" t="b">
+      <c r="J100" s="50"/>
+      <c r="K100" s="51"/>
+      <c r="L100" s="51"/>
+      <c r="M100" s="51"/>
+      <c r="N100" s="51"/>
+      <c r="O100" s="51"/>
+      <c r="Q100" s="52"/>
+    </row>
+    <row r="101" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="49" t="b">
         <v>1</v>
       </c>
-      <c r="B99" s="49" t="s">
+      <c r="B101" s="49" t="s">
         <v>832</v>
       </c>
-      <c r="C99" s="49" t="s">
+      <c r="C101" s="49" t="s">
         <v>831</v>
       </c>
-      <c r="D99" s="49" t="s">
+      <c r="D101" s="49" t="s">
         <v>831</v>
       </c>
-      <c r="E99" s="49" t="s">
+      <c r="E101" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="J99" s="50"/>
-      <c r="K99" s="51"/>
-      <c r="L99" s="51"/>
-      <c r="M99" s="51"/>
-      <c r="N99" s="51"/>
-      <c r="O99" s="51"/>
-      <c r="Q99" s="52"/>
-    </row>
-    <row r="100" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="22" t="b">
+      <c r="J101" s="50"/>
+      <c r="K101" s="51"/>
+      <c r="L101" s="51"/>
+      <c r="M101" s="51"/>
+      <c r="N101" s="51"/>
+      <c r="O101" s="51"/>
+      <c r="Q101" s="52"/>
+    </row>
+    <row r="102" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="B100" s="22" t="s">
+      <c r="B102" s="22" t="s">
         <v>801</v>
       </c>
-      <c r="C100" s="22" t="s">
+      <c r="C102" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="D100" s="22" t="s">
+      <c r="D102" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="E100" s="22" t="s">
+      <c r="E102" s="22" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="101" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="18"/>
-      <c r="B101" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D101" s="30" t="s">
+    <row r="103" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="18"/>
+      <c r="B103" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D103" s="30" t="s">
         <v>373</v>
       </c>
-      <c r="E101" s="30" t="s">
+      <c r="E103" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="F101" s="30" t="s">
+      <c r="F103" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="H101" s="30" t="s">
+      <c r="H103" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="I101" s="30" t="s">
+      <c r="I103" s="30" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="102" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="43" t="s">
+    <row r="104" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B104" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="D102" s="43" t="s">
+      <c r="D104" s="43" t="s">
         <v>802</v>
       </c>
-      <c r="E102" s="43" t="s">
+      <c r="E104" s="43" t="s">
         <v>288</v>
       </c>
-      <c r="F102" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="G102" s="43" t="s">
+      <c r="F104" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="G104" s="43" t="s">
         <v>792</v>
       </c>
-      <c r="H102" s="43">
-        <v>0</v>
-      </c>
-      <c r="J102" s="43">
-        <v>0</v>
-      </c>
-      <c r="K102" s="43">
+      <c r="H104" s="43">
+        <v>0</v>
+      </c>
+      <c r="J104" s="43">
+        <v>0</v>
+      </c>
+      <c r="K104" s="43">
         <v>40</v>
       </c>
-      <c r="L102" s="43">
+      <c r="L104" s="43">
         <v>-1</v>
       </c>
-      <c r="M102" s="45">
-        <f>(K102-J102)/6</f>
+      <c r="M104" s="45">
+        <f>(K104-J104)/6</f>
         <v>6.666666666666667</v>
       </c>
-      <c r="N102" s="45">
+      <c r="N104" s="45">
         <v>2.5</v>
       </c>
-      <c r="Q102" s="43" t="s">
+      <c r="Q104" s="43" t="s">
         <v>777</v>
-      </c>
-    </row>
-    <row r="103" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B103" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D103" s="30" t="s">
-        <v>793</v>
-      </c>
-      <c r="E103" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="F103" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G103" s="30" t="s">
-        <v>792</v>
-      </c>
-      <c r="H103" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D104" s="30" t="s">
-        <v>794</v>
-      </c>
-      <c r="E104" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="F104" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G104" s="30" t="s">
-        <v>792</v>
-      </c>
-      <c r="H104" s="30">
-        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -9723,16 +9732,16 @@
         <v>21</v>
       </c>
       <c r="D105" s="30" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="E105" s="30" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F105" s="30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G105" s="30" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="H105" s="30">
         <v>0</v>
@@ -9743,15 +9752,18 @@
         <v>21</v>
       </c>
       <c r="D106" s="30" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="E106" s="30" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F106" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="H106" s="30" t="b">
+        <v>64</v>
+      </c>
+      <c r="G106" s="30" t="s">
+        <v>792</v>
+      </c>
+      <c r="H106" s="30">
         <v>0</v>
       </c>
     </row>
@@ -9760,10 +9772,10 @@
         <v>21</v>
       </c>
       <c r="D107" s="30" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="E107" s="30" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F107" s="30" t="s">
         <v>65</v>
@@ -9772,7 +9784,7 @@
         <v>796</v>
       </c>
       <c r="H107" s="30">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -9780,18 +9792,15 @@
         <v>21</v>
       </c>
       <c r="D108" s="30" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="E108" s="30" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F108" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G108" s="30" t="s">
-        <v>792</v>
-      </c>
-      <c r="H108" s="30">
+        <v>63</v>
+      </c>
+      <c r="H108" s="30" t="b">
         <v>0</v>
       </c>
     </row>
@@ -9800,10 +9809,10 @@
         <v>21</v>
       </c>
       <c r="D109" s="30" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="E109" s="30" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F109" s="30" t="s">
         <v>65</v>
@@ -9812,103 +9821,107 @@
         <v>796</v>
       </c>
       <c r="H109" s="30">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="110" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B110" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D110" s="30" t="s">
+        <v>799</v>
+      </c>
+      <c r="E110" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F110" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G110" s="30" t="s">
+        <v>792</v>
+      </c>
+      <c r="H110" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B111" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D111" s="30" t="s">
+        <v>800</v>
+      </c>
+      <c r="E111" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="F111" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G111" s="30" t="s">
+        <v>796</v>
+      </c>
+      <c r="H111" s="30">
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="49" t="b">
+    <row r="112" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="49" t="b">
         <v>1</v>
       </c>
-      <c r="B110" s="49" t="s">
+      <c r="B112" s="49" t="s">
         <v>209</v>
       </c>
-      <c r="C110" s="49" t="s">
+      <c r="C112" s="49" t="s">
         <v>210</v>
       </c>
-      <c r="D110" s="49" t="s">
+      <c r="D112" s="49" t="s">
         <v>210</v>
       </c>
-      <c r="E110" s="49" t="s">
+      <c r="E112" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="J110" s="50"/>
-      <c r="K110" s="51"/>
-      <c r="L110" s="51"/>
-      <c r="M110" s="51"/>
-      <c r="N110" s="51"/>
-      <c r="O110" s="51"/>
-      <c r="Q110" s="52"/>
-    </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B111" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D111" s="31" t="s">
-        <v>835</v>
-      </c>
-      <c r="E111" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="F111" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H111" s="31" t="s">
-        <v>417</v>
-      </c>
-      <c r="I111" s="30" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B112" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D112" s="31" t="s">
-        <v>836</v>
-      </c>
-      <c r="E112" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="F112" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="H112" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="I112" s="31"/>
+      <c r="J112" s="50"/>
+      <c r="K112" s="51"/>
+      <c r="L112" s="51"/>
+      <c r="M112" s="51"/>
+      <c r="N112" s="51"/>
+      <c r="O112" s="51"/>
+      <c r="Q112" s="52"/>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B113" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D113" s="31" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="E113" s="31" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F113" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="H113" s="31">
-        <v>0</v>
-      </c>
-      <c r="I113" s="31"/>
+        <v>62</v>
+      </c>
+      <c r="H113" s="31" t="s">
+        <v>417</v>
+      </c>
+      <c r="I113" s="30" t="s">
+        <v>418</v>
+      </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B114" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D114" s="31" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="E114" s="31" t="s">
-        <v>50</v>
+        <v>91</v>
       </c>
       <c r="F114" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="H114" s="31">
+        <v>63</v>
+      </c>
+      <c r="H114" s="31" t="b">
         <v>0</v>
       </c>
       <c r="I114" s="31"/>
@@ -9918,16 +9931,13 @@
         <v>21</v>
       </c>
       <c r="D115" s="31" t="s">
-        <v>795</v>
+        <v>837</v>
       </c>
       <c r="E115" s="31" t="s">
-        <v>52</v>
+        <v>128</v>
       </c>
       <c r="F115" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G115" s="30" t="s">
-        <v>796</v>
+        <v>64</v>
       </c>
       <c r="H115" s="31">
         <v>0</v>
@@ -9939,16 +9949,15 @@
         <v>21</v>
       </c>
       <c r="D116" s="31" t="s">
-        <v>797</v>
+        <v>838</v>
       </c>
       <c r="E116" s="31" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F116" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="G116" s="30"/>
-      <c r="H116" s="31" t="b">
+        <v>64</v>
+      </c>
+      <c r="H116" s="31">
         <v>0</v>
       </c>
       <c r="I116" s="31"/>
@@ -9957,11 +9966,11 @@
       <c r="B117" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D117" s="30" t="s">
-        <v>798</v>
-      </c>
-      <c r="E117" s="30" t="s">
-        <v>56</v>
+      <c r="D117" s="31" t="s">
+        <v>795</v>
+      </c>
+      <c r="E117" s="31" t="s">
+        <v>52</v>
       </c>
       <c r="F117" s="30" t="s">
         <v>65</v>
@@ -9970,7 +9979,7 @@
         <v>796</v>
       </c>
       <c r="H117" s="31">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I117" s="31"/>
     </row>
@@ -9978,19 +9987,17 @@
       <c r="B118" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D118" s="30" t="s">
-        <v>851</v>
-      </c>
-      <c r="E118" s="30" t="s">
-        <v>58</v>
+      <c r="D118" s="31" t="s">
+        <v>797</v>
+      </c>
+      <c r="E118" s="31" t="s">
+        <v>54</v>
       </c>
       <c r="F118" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G118" s="30" t="s">
-        <v>792</v>
-      </c>
-      <c r="H118" s="31">
+        <v>63</v>
+      </c>
+      <c r="G118" s="30"/>
+      <c r="H118" s="31" t="b">
         <v>0</v>
       </c>
       <c r="I118" s="31"/>
@@ -10000,10 +10007,10 @@
         <v>21</v>
       </c>
       <c r="D119" s="30" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="E119" s="30" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F119" s="30" t="s">
         <v>65</v>
@@ -10012,125 +10019,125 @@
         <v>796</v>
       </c>
       <c r="H119" s="31">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="I119" s="31"/>
     </row>
-    <row r="120" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B120" s="49" t="s">
-        <v>216</v>
-      </c>
-      <c r="C120" s="49" t="s">
-        <v>217</v>
-      </c>
-      <c r="D120" s="49" t="s">
-        <v>217</v>
-      </c>
-      <c r="E120" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="J120" s="50"/>
-      <c r="K120" s="51"/>
-      <c r="L120" s="51"/>
-      <c r="M120" s="51"/>
-      <c r="N120" s="51"/>
-      <c r="O120" s="51"/>
-      <c r="Q120" s="52"/>
+    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B120" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D120" s="30" t="s">
+        <v>851</v>
+      </c>
+      <c r="E120" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F120" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G120" s="30" t="s">
+        <v>792</v>
+      </c>
+      <c r="H120" s="31">
+        <v>0</v>
+      </c>
+      <c r="I120" s="31"/>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B121" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D121" s="31" t="s">
-        <v>835</v>
-      </c>
-      <c r="E121" s="31" t="s">
-        <v>126</v>
+      <c r="D121" s="30" t="s">
+        <v>800</v>
+      </c>
+      <c r="E121" s="30" t="s">
+        <v>60</v>
       </c>
       <c r="F121" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H121" s="31" t="s">
-        <v>417</v>
-      </c>
-      <c r="I121" s="30" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B122" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D122" s="31" t="s">
-        <v>841</v>
-      </c>
-      <c r="E122" s="31" t="s">
-        <v>219</v>
-      </c>
-      <c r="F122" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H122" s="31" t="s">
-        <v>839</v>
-      </c>
-      <c r="I122" s="30" t="s">
-        <v>840</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="G121" s="30" t="s">
+        <v>796</v>
+      </c>
+      <c r="H121" s="31">
+        <v>1</v>
+      </c>
+      <c r="I121" s="31"/>
+    </row>
+    <row r="122" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="B122" s="49" t="s">
+        <v>216</v>
+      </c>
+      <c r="C122" s="49" t="s">
+        <v>217</v>
+      </c>
+      <c r="D122" s="49" t="s">
+        <v>217</v>
+      </c>
+      <c r="E122" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="J122" s="50"/>
+      <c r="K122" s="51"/>
+      <c r="L122" s="51"/>
+      <c r="M122" s="51"/>
+      <c r="N122" s="51"/>
+      <c r="O122" s="51"/>
+      <c r="Q122" s="52"/>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B123" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D123" s="31" t="s">
-        <v>842</v>
+        <v>835</v>
       </c>
       <c r="E123" s="31" t="s">
-        <v>221</v>
+        <v>126</v>
       </c>
       <c r="F123" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G123" s="31" t="s">
-        <v>843</v>
-      </c>
-      <c r="H123" s="31">
-        <v>69</v>
-      </c>
-      <c r="I123" s="31"/>
+        <v>62</v>
+      </c>
+      <c r="H123" s="31" t="s">
+        <v>417</v>
+      </c>
+      <c r="I123" s="30" t="s">
+        <v>418</v>
+      </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B124" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D124" s="31" t="s">
-        <v>845</v>
+        <v>841</v>
       </c>
       <c r="E124" s="31" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="F124" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G124" s="31" t="s">
-        <v>844</v>
-      </c>
-      <c r="H124" s="31">
-        <v>28</v>
-      </c>
-      <c r="I124" s="31"/>
+        <v>62</v>
+      </c>
+      <c r="H124" s="31" t="s">
+        <v>839</v>
+      </c>
+      <c r="I124" s="30" t="s">
+        <v>840</v>
+      </c>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B125" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D125" s="31" t="s">
-        <v>846</v>
+        <v>842</v>
       </c>
       <c r="E125" s="31" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="F125" s="30" t="s">
         <v>64</v>
@@ -10139,7 +10146,7 @@
         <v>843</v>
       </c>
       <c r="H125" s="31">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="I125" s="31"/>
     </row>
@@ -10148,19 +10155,19 @@
         <v>21</v>
       </c>
       <c r="D126" s="31" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="E126" s="31" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="F126" s="30" t="s">
         <v>64</v>
       </c>
       <c r="G126" s="31" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="H126" s="31">
-        <v>-148</v>
+        <v>28</v>
       </c>
       <c r="I126" s="31"/>
     </row>
@@ -10169,16 +10176,19 @@
         <v>21</v>
       </c>
       <c r="D127" s="31" t="s">
-        <v>836</v>
+        <v>846</v>
       </c>
       <c r="E127" s="31" t="s">
-        <v>91</v>
+        <v>225</v>
       </c>
       <c r="F127" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="H127" s="31" t="b">
-        <v>0</v>
+        <v>64</v>
+      </c>
+      <c r="G127" s="31" t="s">
+        <v>843</v>
+      </c>
+      <c r="H127" s="31">
+        <v>55</v>
       </c>
       <c r="I127" s="31"/>
     </row>
@@ -10187,16 +10197,19 @@
         <v>21</v>
       </c>
       <c r="D128" s="31" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="E128" s="31" t="s">
-        <v>128</v>
+        <v>227</v>
       </c>
       <c r="F128" s="30" t="s">
         <v>64</v>
       </c>
+      <c r="G128" s="31" t="s">
+        <v>843</v>
+      </c>
       <c r="H128" s="31">
-        <v>0</v>
+        <v>-148</v>
       </c>
       <c r="I128" s="31"/>
     </row>
@@ -10205,15 +10218,15 @@
         <v>21</v>
       </c>
       <c r="D129" s="31" t="s">
-        <v>849</v>
+        <v>836</v>
       </c>
       <c r="E129" s="31" t="s">
-        <v>50</v>
+        <v>91</v>
       </c>
       <c r="F129" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="H129" s="31">
+        <v>63</v>
+      </c>
+      <c r="H129" s="31" t="b">
         <v>0</v>
       </c>
       <c r="I129" s="31"/>
@@ -10223,16 +10236,13 @@
         <v>21</v>
       </c>
       <c r="D130" s="31" t="s">
-        <v>795</v>
+        <v>848</v>
       </c>
       <c r="E130" s="31" t="s">
-        <v>52</v>
+        <v>128</v>
       </c>
       <c r="F130" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G130" s="30" t="s">
-        <v>796</v>
+        <v>64</v>
       </c>
       <c r="H130" s="31">
         <v>0</v>
@@ -10244,16 +10254,15 @@
         <v>21</v>
       </c>
       <c r="D131" s="31" t="s">
-        <v>797</v>
+        <v>849</v>
       </c>
       <c r="E131" s="31" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F131" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="G131" s="30"/>
-      <c r="H131" s="31" t="b">
+        <v>64</v>
+      </c>
+      <c r="H131" s="31">
         <v>0</v>
       </c>
       <c r="I131" s="31"/>
@@ -10262,11 +10271,11 @@
       <c r="B132" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D132" s="30" t="s">
-        <v>798</v>
-      </c>
-      <c r="E132" s="30" t="s">
-        <v>56</v>
+      <c r="D132" s="31" t="s">
+        <v>795</v>
+      </c>
+      <c r="E132" s="31" t="s">
+        <v>52</v>
       </c>
       <c r="F132" s="30" t="s">
         <v>65</v>
@@ -10275,7 +10284,7 @@
         <v>796</v>
       </c>
       <c r="H132" s="31">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I132" s="31"/>
     </row>
@@ -10283,19 +10292,17 @@
       <c r="B133" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D133" s="30" t="s">
-        <v>850</v>
-      </c>
-      <c r="E133" s="30" t="s">
-        <v>58</v>
+      <c r="D133" s="31" t="s">
+        <v>797</v>
+      </c>
+      <c r="E133" s="31" t="s">
+        <v>54</v>
       </c>
       <c r="F133" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G133" s="30" t="s">
-        <v>792</v>
-      </c>
-      <c r="H133" s="31">
+        <v>63</v>
+      </c>
+      <c r="G133" s="30"/>
+      <c r="H133" s="31" t="b">
         <v>0</v>
       </c>
       <c r="I133" s="31"/>
@@ -10305,10 +10312,10 @@
         <v>21</v>
       </c>
       <c r="D134" s="30" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="E134" s="30" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F134" s="30" t="s">
         <v>65</v>
@@ -10317,16 +10324,50 @@
         <v>796</v>
       </c>
       <c r="H134" s="31">
+        <v>15</v>
+      </c>
+      <c r="I134" s="31"/>
+    </row>
+    <row r="135" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B135" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D135" s="30" t="s">
+        <v>850</v>
+      </c>
+      <c r="E135" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F135" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G135" s="30" t="s">
+        <v>792</v>
+      </c>
+      <c r="H135" s="31">
+        <v>0</v>
+      </c>
+      <c r="I135" s="31"/>
+    </row>
+    <row r="136" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B136" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D136" s="30" t="s">
+        <v>800</v>
+      </c>
+      <c r="E136" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="F136" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G136" s="30" t="s">
+        <v>796</v>
+      </c>
+      <c r="H136" s="31">
         <v>1</v>
       </c>
-      <c r="I134" s="31"/>
-    </row>
-    <row r="135" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H135" s="31"/>
-      <c r="I135" s="31"/>
-    </row>
-    <row r="136" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H136" s="31"/>
       <c r="I136" s="31"/>
     </row>
     <row r="137" spans="2:9" x14ac:dyDescent="0.25">
@@ -10645,8 +10686,16 @@
       <c r="H215" s="31"/>
       <c r="I215" s="31"/>
     </row>
+    <row r="216" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H216" s="31"/>
+      <c r="I216" s="31"/>
+    </row>
+    <row r="217" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H217" s="31"/>
+      <c r="I217" s="31"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:Z142"/>
+  <autoFilter ref="A2:Z144"/>
   <mergeCells count="1">
     <mergeCell ref="T1:Y1"/>
   </mergeCells>

</xml_diff>

<commit_message>
Added Adjust thermostat to cali for office_ee
Has argument for heating and cooling that takes delta change in degrees
fahrenheit.
</commit_message>
<xml_diff>
--- a/projects/office_ee.xlsx
+++ b/projects/office_ee.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23265" windowHeight="13185" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15090" windowHeight="7905" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -16,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$144</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$148</definedName>
     <definedName name="AnalysisType">Lookups!$A$17:$A$23</definedName>
     <definedName name="instance_defs">Lookups!$A$2:$D$9</definedName>
     <definedName name="instance_types">Lookups!$A$2:$A$9</definedName>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2752" uniqueCount="874">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2772" uniqueCount="879">
   <si>
     <t>type</t>
   </si>
@@ -2663,6 +2663,21 @@
   </si>
   <si>
     <t>degrees</t>
+  </si>
+  <si>
+    <t>AdjustThermostatSetpointsByDegrees</t>
+  </si>
+  <si>
+    <t>deg F</t>
+  </si>
+  <si>
+    <t>Alter Design Day Thermostats</t>
+  </si>
+  <si>
+    <t>Degrees Fahrenheit to Adjust Cooling Setpoint By</t>
+  </si>
+  <si>
+    <t>Degrees Fahrenheit to Adjust heating Setpoint By</t>
   </si>
 </sst>
 </file>
@@ -7342,11 +7357,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y217"/>
+  <dimension ref="A1:Y221"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I37" sqref="I37"/>
+      <pane ySplit="3" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O102" sqref="O102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9494,177 +9509,212 @@
         <v>777</v>
       </c>
     </row>
-    <row r="95" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="49" t="b">
+    <row r="95" spans="1:17" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="38" t="b">
         <v>1</v>
       </c>
-      <c r="B95" s="49" t="s">
+      <c r="B95" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="C95" s="38" t="s">
+        <v>874</v>
+      </c>
+      <c r="D95" s="38" t="s">
+        <v>874</v>
+      </c>
+      <c r="E95" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="G95" s="39"/>
+      <c r="H95" s="39"/>
+    </row>
+    <row r="96" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B96" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D96" s="43" t="s">
+        <v>877</v>
+      </c>
+      <c r="E96" s="43" t="s">
+        <v>190</v>
+      </c>
+      <c r="F96" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="G96" s="43" t="s">
+        <v>875</v>
+      </c>
+      <c r="H96" s="43">
+        <v>1</v>
+      </c>
+      <c r="I96" s="46"/>
+      <c r="J96" s="45">
+        <v>-5</v>
+      </c>
+      <c r="K96" s="45">
+        <v>5</v>
+      </c>
+      <c r="L96" s="45">
+        <v>0</v>
+      </c>
+      <c r="M96" s="45">
+        <f>(K96-J96)/6</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="N96" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q96" s="43" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B97" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D97" s="43" t="s">
+        <v>878</v>
+      </c>
+      <c r="E97" s="43" t="s">
+        <v>192</v>
+      </c>
+      <c r="F97" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="G97" s="43" t="s">
+        <v>875</v>
+      </c>
+      <c r="H97" s="43">
+        <v>-1</v>
+      </c>
+      <c r="I97" s="46"/>
+      <c r="J97" s="45">
+        <v>-5</v>
+      </c>
+      <c r="K97" s="45">
+        <v>5</v>
+      </c>
+      <c r="L97" s="45">
+        <v>0</v>
+      </c>
+      <c r="M97" s="45">
+        <f>(K97-J97)/6</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="N97" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q97" s="43" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B98" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D98" s="31" t="s">
+        <v>876</v>
+      </c>
+      <c r="E98" s="31" t="s">
+        <v>194</v>
+      </c>
+      <c r="F98" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="H98" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="J98" s="3"/>
+      <c r="K98" s="3"/>
+      <c r="L98" s="3"/>
+      <c r="M98" s="3"/>
+      <c r="N98" s="3"/>
+    </row>
+    <row r="99" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="B99" s="49" t="s">
         <v>855</v>
       </c>
-      <c r="C95" s="49" t="s">
+      <c r="C99" s="49" t="s">
         <v>854</v>
       </c>
-      <c r="D95" s="49" t="s">
+      <c r="D99" s="49" t="s">
         <v>854</v>
       </c>
-      <c r="E95" s="49" t="s">
+      <c r="E99" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="J95" s="50"/>
-      <c r="K95" s="51"/>
-      <c r="L95" s="51"/>
-      <c r="M95" s="51"/>
-      <c r="N95" s="51"/>
-      <c r="O95" s="51"/>
-      <c r="Q95" s="52"/>
-    </row>
-    <row r="96" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="18"/>
-      <c r="B96" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D96" s="30" t="s">
+      <c r="J99" s="50"/>
+      <c r="K99" s="51"/>
+      <c r="L99" s="51"/>
+      <c r="M99" s="51"/>
+      <c r="N99" s="51"/>
+      <c r="O99" s="51"/>
+      <c r="Q99" s="52"/>
+    </row>
+    <row r="100" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="18"/>
+      <c r="B100" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D100" s="30" t="s">
         <v>860</v>
       </c>
-      <c r="E96" s="30" t="s">
+      <c r="E100" s="30" t="s">
         <v>856</v>
       </c>
-      <c r="F96" s="30" t="s">
+      <c r="F100" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="G96" s="30" t="s">
+      <c r="G100" s="30" t="s">
         <v>852</v>
       </c>
-      <c r="H96" s="30">
+      <c r="H100" s="30">
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="18"/>
-      <c r="B97" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D97" s="30" t="s">
+    <row r="101" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="18"/>
+      <c r="B101" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D101" s="30" t="s">
         <v>861</v>
       </c>
-      <c r="E97" s="30" t="s">
+      <c r="E101" s="30" t="s">
         <v>857</v>
       </c>
-      <c r="F97" s="30" t="s">
+      <c r="F101" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="G97" s="30" t="s">
+      <c r="G101" s="30" t="s">
         <v>853</v>
       </c>
-      <c r="H97" s="30">
+      <c r="H101" s="30">
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="18"/>
-      <c r="B98" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D98" s="30" t="s">
+    <row r="102" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="18"/>
+      <c r="B102" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D102" s="30" t="s">
         <v>862</v>
       </c>
-      <c r="E98" s="30" t="s">
+      <c r="E102" s="30" t="s">
         <v>858</v>
       </c>
-      <c r="F98" s="30" t="s">
+      <c r="F102" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="G98" s="30" t="s">
+      <c r="G102" s="30" t="s">
         <v>852</v>
       </c>
-      <c r="H98" s="30">
+      <c r="H102" s="30">
         <v>12</v>
-      </c>
-    </row>
-    <row r="99" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="18"/>
-      <c r="B99" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D99" s="30" t="s">
-        <v>863</v>
-      </c>
-      <c r="E99" s="30" t="s">
-        <v>859</v>
-      </c>
-      <c r="F99" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G99" s="30" t="s">
-        <v>853</v>
-      </c>
-      <c r="H99" s="30">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="100" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B100" s="49" t="s">
-        <v>804</v>
-      </c>
-      <c r="C100" s="49" t="s">
-        <v>803</v>
-      </c>
-      <c r="D100" s="49" t="s">
-        <v>803</v>
-      </c>
-      <c r="E100" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="J100" s="50"/>
-      <c r="K100" s="51"/>
-      <c r="L100" s="51"/>
-      <c r="M100" s="51"/>
-      <c r="N100" s="51"/>
-      <c r="O100" s="51"/>
-      <c r="Q100" s="52"/>
-    </row>
-    <row r="101" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B101" s="49" t="s">
-        <v>832</v>
-      </c>
-      <c r="C101" s="49" t="s">
-        <v>831</v>
-      </c>
-      <c r="D101" s="49" t="s">
-        <v>831</v>
-      </c>
-      <c r="E101" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="J101" s="50"/>
-      <c r="K101" s="51"/>
-      <c r="L101" s="51"/>
-      <c r="M101" s="51"/>
-      <c r="N101" s="51"/>
-      <c r="O101" s="51"/>
-      <c r="Q101" s="52"/>
-    </row>
-    <row r="102" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="B102" s="22" t="s">
-        <v>801</v>
-      </c>
-      <c r="C102" s="22" t="s">
-        <v>286</v>
-      </c>
-      <c r="D102" s="22" t="s">
-        <v>286</v>
-      </c>
-      <c r="E102" s="22" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="103" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -9673,135 +9723,144 @@
         <v>21</v>
       </c>
       <c r="D103" s="30" t="s">
+        <v>863</v>
+      </c>
+      <c r="E103" s="30" t="s">
+        <v>859</v>
+      </c>
+      <c r="F103" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G103" s="30" t="s">
+        <v>853</v>
+      </c>
+      <c r="H103" s="30">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="B104" s="49" t="s">
+        <v>804</v>
+      </c>
+      <c r="C104" s="49" t="s">
+        <v>803</v>
+      </c>
+      <c r="D104" s="49" t="s">
+        <v>803</v>
+      </c>
+      <c r="E104" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="J104" s="50"/>
+      <c r="K104" s="51"/>
+      <c r="L104" s="51"/>
+      <c r="M104" s="51"/>
+      <c r="N104" s="51"/>
+      <c r="O104" s="51"/>
+      <c r="Q104" s="52"/>
+    </row>
+    <row r="105" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="B105" s="49" t="s">
+        <v>832</v>
+      </c>
+      <c r="C105" s="49" t="s">
+        <v>831</v>
+      </c>
+      <c r="D105" s="49" t="s">
+        <v>831</v>
+      </c>
+      <c r="E105" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="J105" s="50"/>
+      <c r="K105" s="51"/>
+      <c r="L105" s="51"/>
+      <c r="M105" s="51"/>
+      <c r="N105" s="51"/>
+      <c r="O105" s="51"/>
+      <c r="Q105" s="52"/>
+    </row>
+    <row r="106" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="B106" s="22" t="s">
+        <v>801</v>
+      </c>
+      <c r="C106" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="D106" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="E106" s="22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="18"/>
+      <c r="B107" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D107" s="30" t="s">
         <v>373</v>
       </c>
-      <c r="E103" s="30" t="s">
+      <c r="E107" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="F103" s="30" t="s">
+      <c r="F107" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="H103" s="30" t="s">
+      <c r="H107" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="I103" s="30" t="s">
+      <c r="I107" s="30" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="104" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="43" t="s">
+    <row r="108" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B108" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="D104" s="43" t="s">
+      <c r="D108" s="43" t="s">
         <v>802</v>
       </c>
-      <c r="E104" s="43" t="s">
+      <c r="E108" s="43" t="s">
         <v>288</v>
       </c>
-      <c r="F104" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="G104" s="43" t="s">
+      <c r="F108" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="G108" s="43" t="s">
         <v>792</v>
       </c>
-      <c r="H104" s="43">
-        <v>0</v>
-      </c>
-      <c r="J104" s="43">
-        <v>0</v>
-      </c>
-      <c r="K104" s="43">
+      <c r="H108" s="43">
+        <v>0</v>
+      </c>
+      <c r="J108" s="43">
+        <v>0</v>
+      </c>
+      <c r="K108" s="43">
         <v>40</v>
       </c>
-      <c r="L104" s="43">
+      <c r="L108" s="43">
         <v>-1</v>
       </c>
-      <c r="M104" s="45">
-        <f>(K104-J104)/6</f>
+      <c r="M108" s="45">
+        <f>(K108-J108)/6</f>
         <v>6.666666666666667</v>
       </c>
-      <c r="N104" s="45">
+      <c r="N108" s="45">
         <v>2.5</v>
       </c>
-      <c r="Q104" s="43" t="s">
+      <c r="Q108" s="43" t="s">
         <v>777</v>
-      </c>
-    </row>
-    <row r="105" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B105" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D105" s="30" t="s">
-        <v>793</v>
-      </c>
-      <c r="E105" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="F105" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G105" s="30" t="s">
-        <v>792</v>
-      </c>
-      <c r="H105" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B106" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D106" s="30" t="s">
-        <v>794</v>
-      </c>
-      <c r="E106" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="F106" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G106" s="30" t="s">
-        <v>792</v>
-      </c>
-      <c r="H106" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B107" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D107" s="30" t="s">
-        <v>795</v>
-      </c>
-      <c r="E107" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="F107" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G107" s="30" t="s">
-        <v>796</v>
-      </c>
-      <c r="H107" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B108" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D108" s="30" t="s">
-        <v>797</v>
-      </c>
-      <c r="E108" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="F108" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="H108" s="30" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -9809,19 +9868,19 @@
         <v>21</v>
       </c>
       <c r="D109" s="30" t="s">
-        <v>798</v>
+        <v>793</v>
       </c>
       <c r="E109" s="30" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="F109" s="30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G109" s="30" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="H109" s="30">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -9829,10 +9888,10 @@
         <v>21</v>
       </c>
       <c r="D110" s="30" t="s">
-        <v>799</v>
+        <v>794</v>
       </c>
       <c r="E110" s="30" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="F110" s="30" t="s">
         <v>64</v>
@@ -9849,10 +9908,10 @@
         <v>21</v>
       </c>
       <c r="D111" s="30" t="s">
-        <v>800</v>
+        <v>795</v>
       </c>
       <c r="E111" s="30" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="F111" s="30" t="s">
         <v>65</v>
@@ -9861,142 +9920,143 @@
         <v>796</v>
       </c>
       <c r="H111" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B112" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D112" s="30" t="s">
+        <v>797</v>
+      </c>
+      <c r="E112" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="F112" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="H112" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B113" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D113" s="30" t="s">
+        <v>798</v>
+      </c>
+      <c r="E113" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F113" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G113" s="30" t="s">
+        <v>796</v>
+      </c>
+      <c r="H113" s="30">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="114" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B114" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D114" s="30" t="s">
+        <v>799</v>
+      </c>
+      <c r="E114" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F114" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G114" s="30" t="s">
+        <v>792</v>
+      </c>
+      <c r="H114" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B115" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D115" s="30" t="s">
+        <v>800</v>
+      </c>
+      <c r="E115" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="F115" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G115" s="30" t="s">
+        <v>796</v>
+      </c>
+      <c r="H115" s="30">
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="49" t="b">
+    <row r="116" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="49" t="b">
         <v>1</v>
       </c>
-      <c r="B112" s="49" t="s">
+      <c r="B116" s="49" t="s">
         <v>209</v>
       </c>
-      <c r="C112" s="49" t="s">
+      <c r="C116" s="49" t="s">
         <v>210</v>
       </c>
-      <c r="D112" s="49" t="s">
+      <c r="D116" s="49" t="s">
         <v>210</v>
       </c>
-      <c r="E112" s="49" t="s">
+      <c r="E116" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="J112" s="50"/>
-      <c r="K112" s="51"/>
-      <c r="L112" s="51"/>
-      <c r="M112" s="51"/>
-      <c r="N112" s="51"/>
-      <c r="O112" s="51"/>
-      <c r="Q112" s="52"/>
-    </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B113" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D113" s="31" t="s">
-        <v>835</v>
-      </c>
-      <c r="E113" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="F113" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H113" s="31" t="s">
-        <v>417</v>
-      </c>
-      <c r="I113" s="30" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B114" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D114" s="31" t="s">
-        <v>836</v>
-      </c>
-      <c r="E114" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="F114" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="H114" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="I114" s="31"/>
-    </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B115" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D115" s="31" t="s">
-        <v>837</v>
-      </c>
-      <c r="E115" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="F115" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="H115" s="31">
-        <v>0</v>
-      </c>
-      <c r="I115" s="31"/>
-    </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B116" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D116" s="31" t="s">
-        <v>838</v>
-      </c>
-      <c r="E116" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="F116" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="H116" s="31">
-        <v>0</v>
-      </c>
-      <c r="I116" s="31"/>
+      <c r="J116" s="50"/>
+      <c r="K116" s="51"/>
+      <c r="L116" s="51"/>
+      <c r="M116" s="51"/>
+      <c r="N116" s="51"/>
+      <c r="O116" s="51"/>
+      <c r="Q116" s="52"/>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B117" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D117" s="31" t="s">
-        <v>795</v>
+        <v>835</v>
       </c>
       <c r="E117" s="31" t="s">
-        <v>52</v>
+        <v>126</v>
       </c>
       <c r="F117" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G117" s="30" t="s">
-        <v>796</v>
-      </c>
-      <c r="H117" s="31">
-        <v>0</v>
-      </c>
-      <c r="I117" s="31"/>
+        <v>62</v>
+      </c>
+      <c r="H117" s="31" t="s">
+        <v>417</v>
+      </c>
+      <c r="I117" s="30" t="s">
+        <v>418</v>
+      </c>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B118" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D118" s="31" t="s">
-        <v>797</v>
+        <v>836</v>
       </c>
       <c r="E118" s="31" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="F118" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="G118" s="30"/>
       <c r="H118" s="31" t="b">
         <v>0</v>
       </c>
@@ -10006,20 +10066,17 @@
       <c r="B119" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D119" s="30" t="s">
-        <v>798</v>
-      </c>
-      <c r="E119" s="30" t="s">
-        <v>56</v>
+      <c r="D119" s="31" t="s">
+        <v>837</v>
+      </c>
+      <c r="E119" s="31" t="s">
+        <v>128</v>
       </c>
       <c r="F119" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G119" s="30" t="s">
-        <v>796</v>
+        <v>64</v>
       </c>
       <c r="H119" s="31">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I119" s="31"/>
     </row>
@@ -10027,17 +10084,14 @@
       <c r="B120" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D120" s="30" t="s">
-        <v>851</v>
-      </c>
-      <c r="E120" s="30" t="s">
-        <v>58</v>
+      <c r="D120" s="31" t="s">
+        <v>838</v>
+      </c>
+      <c r="E120" s="31" t="s">
+        <v>50</v>
       </c>
       <c r="F120" s="30" t="s">
         <v>64</v>
-      </c>
-      <c r="G120" s="30" t="s">
-        <v>792</v>
       </c>
       <c r="H120" s="31">
         <v>0</v>
@@ -10048,11 +10102,11 @@
       <c r="B121" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D121" s="30" t="s">
-        <v>800</v>
-      </c>
-      <c r="E121" s="30" t="s">
-        <v>60</v>
+      <c r="D121" s="31" t="s">
+        <v>795</v>
+      </c>
+      <c r="E121" s="31" t="s">
+        <v>52</v>
       </c>
       <c r="F121" s="30" t="s">
         <v>65</v>
@@ -10061,173 +10115,174 @@
         <v>796</v>
       </c>
       <c r="H121" s="31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I121" s="31"/>
     </row>
-    <row r="122" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B122" s="49" t="s">
-        <v>216</v>
-      </c>
-      <c r="C122" s="49" t="s">
-        <v>217</v>
-      </c>
-      <c r="D122" s="49" t="s">
-        <v>217</v>
-      </c>
-      <c r="E122" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="J122" s="50"/>
-      <c r="K122" s="51"/>
-      <c r="L122" s="51"/>
-      <c r="M122" s="51"/>
-      <c r="N122" s="51"/>
-      <c r="O122" s="51"/>
-      <c r="Q122" s="52"/>
+    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B122" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D122" s="31" t="s">
+        <v>797</v>
+      </c>
+      <c r="E122" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="F122" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="G122" s="30"/>
+      <c r="H122" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I122" s="31"/>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B123" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D123" s="31" t="s">
-        <v>835</v>
-      </c>
-      <c r="E123" s="31" t="s">
-        <v>126</v>
+      <c r="D123" s="30" t="s">
+        <v>798</v>
+      </c>
+      <c r="E123" s="30" t="s">
+        <v>56</v>
       </c>
       <c r="F123" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H123" s="31" t="s">
-        <v>417</v>
-      </c>
-      <c r="I123" s="30" t="s">
-        <v>418</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="G123" s="30" t="s">
+        <v>796</v>
+      </c>
+      <c r="H123" s="31">
+        <v>15</v>
+      </c>
+      <c r="I123" s="31"/>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B124" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D124" s="31" t="s">
-        <v>841</v>
-      </c>
-      <c r="E124" s="31" t="s">
-        <v>219</v>
+      <c r="D124" s="30" t="s">
+        <v>851</v>
+      </c>
+      <c r="E124" s="30" t="s">
+        <v>58</v>
       </c>
       <c r="F124" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H124" s="31" t="s">
-        <v>839</v>
-      </c>
-      <c r="I124" s="30" t="s">
-        <v>840</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="G124" s="30" t="s">
+        <v>792</v>
+      </c>
+      <c r="H124" s="31">
+        <v>0</v>
+      </c>
+      <c r="I124" s="31"/>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B125" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D125" s="31" t="s">
-        <v>842</v>
-      </c>
-      <c r="E125" s="31" t="s">
-        <v>221</v>
+      <c r="D125" s="30" t="s">
+        <v>800</v>
+      </c>
+      <c r="E125" s="30" t="s">
+        <v>60</v>
       </c>
       <c r="F125" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G125" s="31" t="s">
-        <v>843</v>
+        <v>65</v>
+      </c>
+      <c r="G125" s="30" t="s">
+        <v>796</v>
       </c>
       <c r="H125" s="31">
-        <v>69</v>
+        <v>1</v>
       </c>
       <c r="I125" s="31"/>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B126" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D126" s="31" t="s">
-        <v>845</v>
-      </c>
-      <c r="E126" s="31" t="s">
-        <v>223</v>
-      </c>
-      <c r="F126" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G126" s="31" t="s">
-        <v>844</v>
-      </c>
-      <c r="H126" s="31">
-        <v>28</v>
-      </c>
-      <c r="I126" s="31"/>
+    <row r="126" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="B126" s="49" t="s">
+        <v>216</v>
+      </c>
+      <c r="C126" s="49" t="s">
+        <v>217</v>
+      </c>
+      <c r="D126" s="49" t="s">
+        <v>217</v>
+      </c>
+      <c r="E126" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="J126" s="50"/>
+      <c r="K126" s="51"/>
+      <c r="L126" s="51"/>
+      <c r="M126" s="51"/>
+      <c r="N126" s="51"/>
+      <c r="O126" s="51"/>
+      <c r="Q126" s="52"/>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B127" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D127" s="31" t="s">
-        <v>846</v>
+        <v>835</v>
       </c>
       <c r="E127" s="31" t="s">
-        <v>225</v>
+        <v>126</v>
       </c>
       <c r="F127" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G127" s="31" t="s">
-        <v>843</v>
-      </c>
-      <c r="H127" s="31">
-        <v>55</v>
-      </c>
-      <c r="I127" s="31"/>
+        <v>62</v>
+      </c>
+      <c r="H127" s="31" t="s">
+        <v>417</v>
+      </c>
+      <c r="I127" s="30" t="s">
+        <v>418</v>
+      </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B128" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D128" s="31" t="s">
-        <v>847</v>
+        <v>841</v>
       </c>
       <c r="E128" s="31" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="F128" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G128" s="31" t="s">
-        <v>843</v>
-      </c>
-      <c r="H128" s="31">
-        <v>-148</v>
-      </c>
-      <c r="I128" s="31"/>
+        <v>62</v>
+      </c>
+      <c r="H128" s="31" t="s">
+        <v>839</v>
+      </c>
+      <c r="I128" s="30" t="s">
+        <v>840</v>
+      </c>
     </row>
     <row r="129" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B129" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D129" s="31" t="s">
-        <v>836</v>
+        <v>842</v>
       </c>
       <c r="E129" s="31" t="s">
-        <v>91</v>
+        <v>221</v>
       </c>
       <c r="F129" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="H129" s="31" t="b">
-        <v>0</v>
+        <v>64</v>
+      </c>
+      <c r="G129" s="31" t="s">
+        <v>843</v>
+      </c>
+      <c r="H129" s="31">
+        <v>69</v>
       </c>
       <c r="I129" s="31"/>
     </row>
@@ -10236,16 +10291,19 @@
         <v>21</v>
       </c>
       <c r="D130" s="31" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="E130" s="31" t="s">
-        <v>128</v>
+        <v>223</v>
       </c>
       <c r="F130" s="30" t="s">
         <v>64</v>
       </c>
+      <c r="G130" s="31" t="s">
+        <v>844</v>
+      </c>
       <c r="H130" s="31">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="I130" s="31"/>
     </row>
@@ -10254,16 +10312,19 @@
         <v>21</v>
       </c>
       <c r="D131" s="31" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="E131" s="31" t="s">
-        <v>50</v>
+        <v>225</v>
       </c>
       <c r="F131" s="30" t="s">
         <v>64</v>
       </c>
+      <c r="G131" s="31" t="s">
+        <v>843</v>
+      </c>
       <c r="H131" s="31">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="I131" s="31"/>
     </row>
@@ -10272,19 +10333,19 @@
         <v>21</v>
       </c>
       <c r="D132" s="31" t="s">
-        <v>795</v>
+        <v>847</v>
       </c>
       <c r="E132" s="31" t="s">
-        <v>52</v>
+        <v>227</v>
       </c>
       <c r="F132" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G132" s="30" t="s">
-        <v>796</v>
+        <v>64</v>
+      </c>
+      <c r="G132" s="31" t="s">
+        <v>843</v>
       </c>
       <c r="H132" s="31">
-        <v>0</v>
+        <v>-148</v>
       </c>
       <c r="I132" s="31"/>
     </row>
@@ -10293,15 +10354,14 @@
         <v>21</v>
       </c>
       <c r="D133" s="31" t="s">
-        <v>797</v>
+        <v>836</v>
       </c>
       <c r="E133" s="31" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="F133" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="G133" s="30"/>
       <c r="H133" s="31" t="b">
         <v>0</v>
       </c>
@@ -10311,20 +10371,17 @@
       <c r="B134" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D134" s="30" t="s">
-        <v>798</v>
-      </c>
-      <c r="E134" s="30" t="s">
-        <v>56</v>
+      <c r="D134" s="31" t="s">
+        <v>848</v>
+      </c>
+      <c r="E134" s="31" t="s">
+        <v>128</v>
       </c>
       <c r="F134" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G134" s="30" t="s">
-        <v>796</v>
+        <v>64</v>
       </c>
       <c r="H134" s="31">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I134" s="31"/>
     </row>
@@ -10332,17 +10389,14 @@
       <c r="B135" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D135" s="30" t="s">
-        <v>850</v>
-      </c>
-      <c r="E135" s="30" t="s">
-        <v>58</v>
+      <c r="D135" s="31" t="s">
+        <v>849</v>
+      </c>
+      <c r="E135" s="31" t="s">
+        <v>50</v>
       </c>
       <c r="F135" s="30" t="s">
         <v>64</v>
-      </c>
-      <c r="G135" s="30" t="s">
-        <v>792</v>
       </c>
       <c r="H135" s="31">
         <v>0</v>
@@ -10353,11 +10407,11 @@
       <c r="B136" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D136" s="30" t="s">
-        <v>800</v>
-      </c>
-      <c r="E136" s="30" t="s">
-        <v>60</v>
+      <c r="D136" s="31" t="s">
+        <v>795</v>
+      </c>
+      <c r="E136" s="31" t="s">
+        <v>52</v>
       </c>
       <c r="F136" s="30" t="s">
         <v>65</v>
@@ -10366,24 +10420,90 @@
         <v>796</v>
       </c>
       <c r="H136" s="31">
+        <v>0</v>
+      </c>
+      <c r="I136" s="31"/>
+    </row>
+    <row r="137" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B137" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D137" s="31" t="s">
+        <v>797</v>
+      </c>
+      <c r="E137" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="F137" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="G137" s="30"/>
+      <c r="H137" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I137" s="31"/>
+    </row>
+    <row r="138" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B138" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D138" s="30" t="s">
+        <v>798</v>
+      </c>
+      <c r="E138" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F138" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G138" s="30" t="s">
+        <v>796</v>
+      </c>
+      <c r="H138" s="31">
+        <v>15</v>
+      </c>
+      <c r="I138" s="31"/>
+    </row>
+    <row r="139" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B139" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D139" s="30" t="s">
+        <v>850</v>
+      </c>
+      <c r="E139" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F139" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G139" s="30" t="s">
+        <v>792</v>
+      </c>
+      <c r="H139" s="31">
+        <v>0</v>
+      </c>
+      <c r="I139" s="31"/>
+    </row>
+    <row r="140" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B140" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D140" s="30" t="s">
+        <v>800</v>
+      </c>
+      <c r="E140" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="F140" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G140" s="30" t="s">
+        <v>796</v>
+      </c>
+      <c r="H140" s="31">
         <v>1</v>
       </c>
-      <c r="I136" s="31"/>
-    </row>
-    <row r="137" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H137" s="31"/>
-      <c r="I137" s="31"/>
-    </row>
-    <row r="138" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H138" s="31"/>
-      <c r="I138" s="31"/>
-    </row>
-    <row r="139" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H139" s="31"/>
-      <c r="I139" s="31"/>
-    </row>
-    <row r="140" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H140" s="31"/>
       <c r="I140" s="31"/>
     </row>
     <row r="141" spans="2:9" x14ac:dyDescent="0.25">
@@ -10694,8 +10814,24 @@
       <c r="H217" s="31"/>
       <c r="I217" s="31"/>
     </row>
+    <row r="218" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H218" s="31"/>
+      <c r="I218" s="31"/>
+    </row>
+    <row r="219" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H219" s="31"/>
+      <c r="I219" s="31"/>
+    </row>
+    <row r="220" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H220" s="31"/>
+      <c r="I220" s="31"/>
+    </row>
+    <row r="221" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H221" s="31"/>
+      <c r="I221" s="31"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:Z144"/>
+  <autoFilter ref="A2:Z148"/>
   <mergeCells count="1">
     <mergeCell ref="T1:Y1"/>
   </mergeCells>

</xml_diff>

<commit_message>
Updating EE measures to all have variable
Made update to measures and ee spreadsheet
</commit_message>
<xml_diff>
--- a/projects/office_ee.xlsx
+++ b/projects/office_ee.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="22840" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21840" windowHeight="13740" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -16,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$148</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$131</definedName>
     <definedName name="AnalysisType">Lookups!$A$17:$A$23</definedName>
     <definedName name="instance_defs">Lookups!$A$2:$D$9</definedName>
     <definedName name="instance_types">Lookups!$A$2:$A$9</definedName>
@@ -31,7 +31,7 @@
     <definedName name="TrueFalse">Lookups!$C$12:$C$13</definedName>
     <definedName name="Workflow">Lookups!$E$12:$E$13</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2772" uniqueCount="879">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2692" uniqueCount="875">
   <si>
     <t>type</t>
   </si>
@@ -2545,24 +2545,6 @@
     <t>Add Sys 3 - PSZ-AC Ngrid</t>
   </si>
   <si>
-    <t>Choose an Air Loop to Alter</t>
-  </si>
-  <si>
-    <t>Remove Baseline Costs From Effected AirLoopHVACOutdoorAirSystems</t>
-  </si>
-  <si>
-    <t>Material and Installation Costs per Air Loop to Enable Demand Controlled Ventilation</t>
-  </si>
-  <si>
-    <t>Demolition Costs per Air Loop to Enable Demand Controlled Ventilation</t>
-  </si>
-  <si>
-    <t>FixedEnthalpy</t>
-  </si>
-  <si>
-    <t>|FixedDryBulb,FixedEnthalpy,DifferentialDryBulb,DifferentialEnthalpy,FixedDewPointAndDryBulb,NoEconomizer|</t>
-  </si>
-  <si>
     <t>Economizer Control Type</t>
   </si>
   <si>
@@ -2572,30 +2554,9 @@
     <t>F</t>
   </si>
   <si>
-    <t>Btu/lb</t>
-  </si>
-  <si>
-    <t>Economizer Maximum Enthalpy</t>
-  </si>
-  <si>
-    <t>Economizer Maximum Limit Dewpoint Temperature</t>
-  </si>
-  <si>
     <t>Economizer Minimum Limit Dry-Bulb Temperature</t>
   </si>
   <si>
-    <t>Material and Installation Costs per Air Loop to Enable Economizer</t>
-  </si>
-  <si>
-    <t>Demolition Costs per Air Loop to Enable Economizer</t>
-  </si>
-  <si>
-    <t>O &amp; M Costs per Air Loop for Economizer</t>
-  </si>
-  <si>
-    <t>O &amp; M Costs per Air Loop for Demand Controlled Ventilation</t>
-  </si>
-  <si>
     <t>month</t>
   </si>
   <si>
@@ -2678,6 +2639,33 @@
   </si>
   <si>
     <t>DOE Ref 1980-2004</t>
+  </si>
+  <si>
+    <t>|EnableDCV,DisableDCV,NoChange|</t>
+  </si>
+  <si>
+    <t>EnableDCV</t>
+  </si>
+  <si>
+    <t>dcv_type</t>
+  </si>
+  <si>
+    <t>lpd_to_lamps</t>
+  </si>
+  <si>
+    <t>Replace LPD with Lamps</t>
+  </si>
+  <si>
+    <t>t12_to_t8_lamp_replacement</t>
+  </si>
+  <si>
+    <t>Replace T12s with T8s</t>
+  </si>
+  <si>
+    <t>FixedDryBulb</t>
+  </si>
+  <si>
+    <t>|FixedDryBulb,NoEconomizer,NoChange|</t>
   </si>
 </sst>
 </file>
@@ -2687,7 +2675,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4767,10 +4755,10 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1828">
     <cellStyle name="Comma" xfId="1749" builtinId="3"/>
@@ -6905,17 +6893,17 @@
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="81.83203125" customWidth="1"/>
+    <col min="1" max="1" width="81.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="28">
+    <row r="1" spans="1:1" ht="45">
       <c r="A1" s="36" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="28">
+    <row r="2" spans="1:1" ht="30">
       <c r="A2" s="36" t="s">
         <v>41</v>
       </c>
@@ -6939,14 +6927,14 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" style="26" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" style="1" customWidth="1"/>
-    <col min="4" max="4" width="33.1640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="61.6640625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.6640625" style="1"/>
+    <col min="4" max="4" width="33.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="61.7109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -6978,7 +6966,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28">
+    <row r="4" spans="1:5" ht="30">
       <c r="A4" s="1" t="s">
         <v>456</v>
       </c>
@@ -6989,7 +6977,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="42">
+    <row r="5" spans="1:5" ht="75">
       <c r="A5" s="1" t="s">
         <v>469</v>
       </c>
@@ -7000,7 +6988,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="46" customHeight="1">
+    <row r="6" spans="1:5" ht="45.95" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>470</v>
       </c>
@@ -7011,7 +6999,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" ht="30">
       <c r="A7" s="1" t="s">
         <v>442</v>
       </c>
@@ -7030,7 +7018,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28">
+    <row r="8" spans="1:5" ht="30">
       <c r="A8" s="1" t="s">
         <v>443</v>
       </c>
@@ -7115,7 +7103,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" ht="30">
       <c r="A16" s="1" t="s">
         <v>463</v>
       </c>
@@ -7148,7 +7136,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="20" spans="1:5" s="2" customFormat="1" ht="60">
       <c r="A20" s="11" t="s">
         <v>27</v>
       </c>
@@ -7173,7 +7161,7 @@
       <c r="B22" s="26"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="23" spans="1:5" s="2" customFormat="1" ht="60">
       <c r="A23" s="11" t="s">
         <v>450</v>
       </c>
@@ -7263,7 +7251,7 @@
       <c r="C35" s="26"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:5" s="2" customFormat="1" ht="28">
+    <row r="36" spans="1:5" s="2" customFormat="1" ht="45">
       <c r="A36" s="11" t="s">
         <v>33</v>
       </c>
@@ -7284,7 +7272,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="2" customFormat="1" ht="28">
+    <row r="39" spans="1:5" s="2" customFormat="1" ht="30">
       <c r="A39" s="11" t="s">
         <v>30</v>
       </c>
@@ -7313,7 +7301,7 @@
       </c>
       <c r="E40" s="2"/>
     </row>
-    <row r="42" spans="1:5" s="2" customFormat="1" ht="56">
+    <row r="42" spans="1:5" s="2" customFormat="1" ht="60">
       <c r="A42" s="11" t="s">
         <v>35</v>
       </c>
@@ -7367,39 +7355,39 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y221"/>
+  <dimension ref="A1:Y204"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I122" sqref="I122"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="31" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="31" customWidth="1"/>
     <col min="2" max="2" width="47" style="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47" style="31" customWidth="1"/>
-    <col min="4" max="4" width="39.1640625" style="31" customWidth="1"/>
-    <col min="5" max="5" width="24.1640625" style="31" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" style="31" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" style="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5" style="4" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="7.1640625" style="31" customWidth="1"/>
-    <col min="11" max="11" width="8.1640625" style="31" customWidth="1"/>
-    <col min="12" max="12" width="6.6640625" style="31" customWidth="1"/>
-    <col min="13" max="14" width="7.83203125" style="31" customWidth="1"/>
-    <col min="15" max="15" width="11.5" style="31"/>
-    <col min="16" max="16" width="11.5" style="31" customWidth="1"/>
+    <col min="4" max="4" width="39.140625" style="31" customWidth="1"/>
+    <col min="5" max="5" width="35.140625" style="31" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" style="31" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="31" customWidth="1"/>
+    <col min="11" max="11" width="8.140625" style="31" customWidth="1"/>
+    <col min="12" max="12" width="6.7109375" style="31" customWidth="1"/>
+    <col min="13" max="14" width="7.85546875" style="31" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="31"/>
+    <col min="16" max="16" width="11.42578125" style="31" customWidth="1"/>
     <col min="17" max="17" width="23" style="31" customWidth="1"/>
-    <col min="18" max="18" width="27.6640625" style="31" customWidth="1"/>
-    <col min="19" max="19" width="46.1640625" style="31" customWidth="1"/>
-    <col min="20" max="22" width="11.5" style="31"/>
-    <col min="23" max="23" width="13.33203125" style="31" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="11.5" style="31"/>
+    <col min="18" max="18" width="27.7109375" style="31" customWidth="1"/>
+    <col min="19" max="19" width="46.140625" style="31" customWidth="1"/>
+    <col min="20" max="22" width="11.42578125" style="31"/>
+    <col min="23" max="23" width="13.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="11.42578125" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="18">
+    <row r="1" spans="1:25" ht="18.75">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -7425,16 +7413,16 @@
       <c r="Q1" s="5"/>
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
-      <c r="T1" s="53" t="s">
+      <c r="T1" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="53"/>
-    </row>
-    <row r="2" spans="1:25" s="8" customFormat="1" ht="15">
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+    </row>
+    <row r="2" spans="1:25" s="8" customFormat="1" ht="15.75">
       <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
@@ -7450,7 +7438,7 @@
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
     </row>
-    <row r="3" spans="1:25" s="14" customFormat="1" ht="45">
+    <row r="3" spans="1:25" s="14" customFormat="1" ht="63">
       <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
@@ -7635,7 +7623,7 @@
         <v>618</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>878</v>
+        <v>865</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
@@ -7717,7 +7705,7 @@
       <c r="G13" s="39"/>
       <c r="H13" s="39"/>
     </row>
-    <row r="14" spans="1:25" s="30" customFormat="1" ht="17">
+    <row r="14" spans="1:25" s="30" customFormat="1" ht="18">
       <c r="B14" s="30" t="s">
         <v>21</v>
       </c>
@@ -7733,7 +7721,7 @@
       <c r="G14" s="30" t="s">
         <v>766</v>
       </c>
-      <c r="H14" s="54">
+      <c r="H14" s="53">
         <v>104666</v>
       </c>
     </row>
@@ -8108,7 +8096,7 @@
         <v>1</v>
       </c>
       <c r="B36" s="38" t="s">
-        <v>870</v>
+        <v>857</v>
       </c>
       <c r="C36" s="38" t="s">
         <v>74</v>
@@ -8127,7 +8115,7 @@
         <v>21</v>
       </c>
       <c r="D37" s="31" t="s">
-        <v>871</v>
+        <v>858</v>
       </c>
       <c r="E37" s="31" t="s">
         <v>75</v>
@@ -8136,7 +8124,7 @@
         <v>619</v>
       </c>
       <c r="G37" s="31" t="s">
-        <v>872</v>
+        <v>859</v>
       </c>
       <c r="H37" s="31">
         <v>10</v>
@@ -9380,7 +9368,7 @@
         <v>21</v>
       </c>
       <c r="D90" s="43" t="s">
-        <v>863</v>
+        <v>850</v>
       </c>
       <c r="E90" s="43" t="s">
         <v>330</v>
@@ -9417,13 +9405,13 @@
         <v>1</v>
       </c>
       <c r="B91" s="38" t="s">
-        <v>866</v>
+        <v>853</v>
       </c>
       <c r="C91" s="38" t="s">
-        <v>864</v>
+        <v>851</v>
       </c>
       <c r="D91" s="38" t="s">
-        <v>864</v>
+        <v>851</v>
       </c>
       <c r="E91" s="38" t="s">
         <v>68</v>
@@ -9436,7 +9424,7 @@
         <v>21</v>
       </c>
       <c r="D92" s="43" t="s">
-        <v>868</v>
+        <v>855</v>
       </c>
       <c r="E92" s="43" t="s">
         <v>258</v>
@@ -9473,13 +9461,13 @@
         <v>1</v>
       </c>
       <c r="B93" s="38" t="s">
-        <v>867</v>
+        <v>854</v>
       </c>
       <c r="C93" s="38" t="s">
-        <v>865</v>
+        <v>852</v>
       </c>
       <c r="D93" s="38" t="s">
-        <v>865</v>
+        <v>852</v>
       </c>
       <c r="E93" s="38" t="s">
         <v>68</v>
@@ -9492,7 +9480,7 @@
         <v>21</v>
       </c>
       <c r="D94" s="43" t="s">
-        <v>869</v>
+        <v>856</v>
       </c>
       <c r="E94" s="43" t="s">
         <v>258</v>
@@ -9532,10 +9520,10 @@
         <v>187</v>
       </c>
       <c r="C95" s="38" t="s">
-        <v>873</v>
+        <v>860</v>
       </c>
       <c r="D95" s="38" t="s">
-        <v>873</v>
+        <v>860</v>
       </c>
       <c r="E95" s="38" t="s">
         <v>68</v>
@@ -9548,7 +9536,7 @@
         <v>21</v>
       </c>
       <c r="D96" s="43" t="s">
-        <v>876</v>
+        <v>863</v>
       </c>
       <c r="E96" s="43" t="s">
         <v>190</v>
@@ -9557,7 +9545,7 @@
         <v>64</v>
       </c>
       <c r="G96" s="43" t="s">
-        <v>874</v>
+        <v>861</v>
       </c>
       <c r="H96" s="43">
         <v>1</v>
@@ -9588,7 +9576,7 @@
         <v>21</v>
       </c>
       <c r="D97" s="43" t="s">
-        <v>877</v>
+        <v>864</v>
       </c>
       <c r="E97" s="43" t="s">
         <v>192</v>
@@ -9597,7 +9585,7 @@
         <v>64</v>
       </c>
       <c r="G97" s="43" t="s">
-        <v>874</v>
+        <v>861</v>
       </c>
       <c r="H97" s="43">
         <v>-1</v>
@@ -9628,7 +9616,7 @@
         <v>21</v>
       </c>
       <c r="D98" s="31" t="s">
-        <v>875</v>
+        <v>862</v>
       </c>
       <c r="E98" s="31" t="s">
         <v>194</v>
@@ -9650,13 +9638,13 @@
         <v>1</v>
       </c>
       <c r="B99" s="49" t="s">
-        <v>854</v>
+        <v>841</v>
       </c>
       <c r="C99" s="49" t="s">
-        <v>853</v>
+        <v>840</v>
       </c>
       <c r="D99" s="49" t="s">
-        <v>853</v>
+        <v>840</v>
       </c>
       <c r="E99" s="49" t="s">
         <v>68</v>
@@ -9675,16 +9663,16 @@
         <v>21</v>
       </c>
       <c r="D100" s="30" t="s">
-        <v>859</v>
+        <v>846</v>
       </c>
       <c r="E100" s="30" t="s">
-        <v>855</v>
+        <v>842</v>
       </c>
       <c r="F100" s="30" t="s">
         <v>65</v>
       </c>
       <c r="G100" s="30" t="s">
-        <v>851</v>
+        <v>838</v>
       </c>
       <c r="H100" s="30">
         <v>1</v>
@@ -9696,16 +9684,16 @@
         <v>21</v>
       </c>
       <c r="D101" s="30" t="s">
-        <v>860</v>
+        <v>847</v>
       </c>
       <c r="E101" s="30" t="s">
-        <v>856</v>
+        <v>843</v>
       </c>
       <c r="F101" s="30" t="s">
         <v>65</v>
       </c>
       <c r="G101" s="30" t="s">
-        <v>852</v>
+        <v>839</v>
       </c>
       <c r="H101" s="30">
         <v>1</v>
@@ -9717,16 +9705,16 @@
         <v>21</v>
       </c>
       <c r="D102" s="30" t="s">
-        <v>861</v>
+        <v>848</v>
       </c>
       <c r="E102" s="30" t="s">
-        <v>857</v>
+        <v>844</v>
       </c>
       <c r="F102" s="30" t="s">
         <v>65</v>
       </c>
       <c r="G102" s="30" t="s">
-        <v>851</v>
+        <v>838</v>
       </c>
       <c r="H102" s="30">
         <v>12</v>
@@ -9738,16 +9726,16 @@
         <v>21</v>
       </c>
       <c r="D103" s="30" t="s">
-        <v>862</v>
+        <v>849</v>
       </c>
       <c r="E103" s="30" t="s">
-        <v>858</v>
+        <v>845</v>
       </c>
       <c r="F103" s="30" t="s">
         <v>65</v>
       </c>
       <c r="G103" s="30" t="s">
-        <v>852</v>
+        <v>839</v>
       </c>
       <c r="H103" s="30">
         <v>31</v>
@@ -9777,145 +9765,148 @@
       <c r="O104" s="51"/>
       <c r="Q104" s="52"/>
     </row>
-    <row r="105" spans="1:17" s="49" customFormat="1">
-      <c r="A105" s="49" t="b">
+    <row r="105" spans="1:17">
+      <c r="B105" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D105" s="31" t="s">
+        <v>870</v>
+      </c>
+      <c r="E105" s="31" t="s">
+        <v>869</v>
+      </c>
+      <c r="F105" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="H105" s="31" t="b">
         <v>1</v>
       </c>
-      <c r="B105" s="49" t="s">
+      <c r="I105" s="31"/>
+      <c r="J105" s="4"/>
+      <c r="K105" s="3"/>
+      <c r="L105" s="3"/>
+      <c r="M105" s="3"/>
+      <c r="N105" s="3"/>
+      <c r="O105" s="3"/>
+      <c r="Q105" s="40"/>
+    </row>
+    <row r="106" spans="1:17" s="49" customFormat="1">
+      <c r="A106" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="B106" s="49" t="s">
         <v>831</v>
       </c>
-      <c r="C105" s="49" t="s">
+      <c r="C106" s="49" t="s">
         <v>830</v>
       </c>
-      <c r="D105" s="49" t="s">
+      <c r="D106" s="49" t="s">
         <v>830</v>
       </c>
-      <c r="E105" s="49" t="s">
+      <c r="E106" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="J105" s="50"/>
-      <c r="K105" s="51"/>
-      <c r="L105" s="51"/>
-      <c r="M105" s="51"/>
-      <c r="N105" s="51"/>
-      <c r="O105" s="51"/>
-      <c r="Q105" s="52"/>
-    </row>
-    <row r="106" spans="1:17" s="22" customFormat="1">
-      <c r="A106" s="22" t="b">
+      <c r="J106" s="50"/>
+      <c r="K106" s="51"/>
+      <c r="L106" s="51"/>
+      <c r="M106" s="51"/>
+      <c r="N106" s="51"/>
+      <c r="O106" s="51"/>
+      <c r="Q106" s="52"/>
+    </row>
+    <row r="107" spans="1:17">
+      <c r="B107" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D107" s="31" t="s">
+        <v>872</v>
+      </c>
+      <c r="E107" s="31" t="s">
+        <v>871</v>
+      </c>
+      <c r="F107" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="H107" s="31" t="b">
         <v>1</v>
       </c>
-      <c r="B106" s="22" t="s">
+      <c r="I107" s="30"/>
+    </row>
+    <row r="108" spans="1:17" s="22" customFormat="1">
+      <c r="A108" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="B108" s="22" t="s">
         <v>800</v>
       </c>
-      <c r="C106" s="22" t="s">
+      <c r="C108" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="D106" s="22" t="s">
+      <c r="D108" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="E106" s="22" t="s">
+      <c r="E108" s="22" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="107" spans="1:17" s="30" customFormat="1">
-      <c r="A107" s="18"/>
-      <c r="B107" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D107" s="30" t="s">
+    <row r="109" spans="1:17" s="30" customFormat="1">
+      <c r="A109" s="18"/>
+      <c r="B109" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D109" s="30" t="s">
         <v>373</v>
       </c>
-      <c r="E107" s="30" t="s">
+      <c r="E109" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="F107" s="30" t="s">
+      <c r="F109" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="H107" s="30" t="s">
+      <c r="H109" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="I107" s="30" t="s">
+      <c r="I109" s="30" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="108" spans="1:17" s="43" customFormat="1">
-      <c r="B108" s="43" t="s">
+    <row r="110" spans="1:17" s="43" customFormat="1">
+      <c r="B110" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="D108" s="43" t="s">
+      <c r="D110" s="43" t="s">
         <v>801</v>
       </c>
-      <c r="E108" s="43" t="s">
+      <c r="E110" s="43" t="s">
         <v>288</v>
       </c>
-      <c r="F108" s="43" t="s">
+      <c r="F110" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="G108" s="43" t="s">
+      <c r="G110" s="43" t="s">
         <v>791</v>
       </c>
-      <c r="H108" s="43">
-        <v>0</v>
-      </c>
-      <c r="J108" s="43">
-        <v>0</v>
-      </c>
-      <c r="K108" s="43">
+      <c r="H110" s="43">
+        <v>0</v>
+      </c>
+      <c r="J110" s="43">
+        <v>0</v>
+      </c>
+      <c r="K110" s="43">
         <v>40</v>
       </c>
-      <c r="L108" s="43">
+      <c r="L110" s="43">
         <v>-1</v>
       </c>
-      <c r="M108" s="45">
-        <f>(K108-J108)/6</f>
+      <c r="M110" s="45">
+        <f>(K110-J110)/6</f>
         <v>6.666666666666667</v>
       </c>
-      <c r="N108" s="45">
+      <c r="N110" s="45">
         <v>2.5</v>
       </c>
-      <c r="Q108" s="43" t="s">
+      <c r="Q110" s="43" t="s">
         <v>776</v>
-      </c>
-    </row>
-    <row r="109" spans="1:17" s="30" customFormat="1">
-      <c r="B109" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D109" s="30" t="s">
-        <v>792</v>
-      </c>
-      <c r="E109" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="F109" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G109" s="30" t="s">
-        <v>791</v>
-      </c>
-      <c r="H109" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:17" s="30" customFormat="1">
-      <c r="B110" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D110" s="30" t="s">
-        <v>793</v>
-      </c>
-      <c r="E110" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="F110" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G110" s="30" t="s">
-        <v>791</v>
-      </c>
-      <c r="H110" s="30">
-        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:17" s="30" customFormat="1">
@@ -9923,16 +9914,16 @@
         <v>21</v>
       </c>
       <c r="D111" s="30" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="E111" s="30" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F111" s="30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G111" s="30" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="H111" s="30">
         <v>0</v>
@@ -9943,15 +9934,18 @@
         <v>21</v>
       </c>
       <c r="D112" s="30" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="E112" s="30" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F112" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="H112" s="30" t="b">
+        <v>64</v>
+      </c>
+      <c r="G112" s="30" t="s">
+        <v>791</v>
+      </c>
+      <c r="H112" s="30">
         <v>0</v>
       </c>
     </row>
@@ -9960,10 +9954,10 @@
         <v>21</v>
       </c>
       <c r="D113" s="30" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="E113" s="30" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F113" s="30" t="s">
         <v>65</v>
@@ -9972,7 +9966,7 @@
         <v>795</v>
       </c>
       <c r="H113" s="30">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:17" s="30" customFormat="1">
@@ -9980,18 +9974,15 @@
         <v>21</v>
       </c>
       <c r="D114" s="30" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="E114" s="30" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F114" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G114" s="30" t="s">
-        <v>791</v>
-      </c>
-      <c r="H114" s="30">
+        <v>63</v>
+      </c>
+      <c r="H114" s="30" t="b">
         <v>0</v>
       </c>
     </row>
@@ -10000,10 +9991,10 @@
         <v>21</v>
       </c>
       <c r="D115" s="30" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="E115" s="30" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F115" s="30" t="s">
         <v>65</v>
@@ -10012,144 +10003,155 @@
         <v>795</v>
       </c>
       <c r="H115" s="30">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="116" spans="1:17" s="30" customFormat="1">
+      <c r="B116" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D116" s="30" t="s">
+        <v>798</v>
+      </c>
+      <c r="E116" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F116" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G116" s="30" t="s">
+        <v>791</v>
+      </c>
+      <c r="H116" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:17" s="30" customFormat="1">
+      <c r="B117" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D117" s="30" t="s">
+        <v>799</v>
+      </c>
+      <c r="E117" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="F117" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G117" s="30" t="s">
+        <v>795</v>
+      </c>
+      <c r="H117" s="30">
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:17" s="49" customFormat="1">
-      <c r="A116" s="49" t="b">
+    <row r="118" spans="1:17" s="49" customFormat="1">
+      <c r="A118" s="49" t="b">
         <v>1</v>
       </c>
-      <c r="B116" s="49" t="s">
+      <c r="B118" s="49" t="s">
         <v>209</v>
       </c>
-      <c r="C116" s="49" t="s">
+      <c r="C118" s="49" t="s">
         <v>210</v>
       </c>
-      <c r="D116" s="49" t="s">
+      <c r="D118" s="49" t="s">
         <v>210</v>
       </c>
-      <c r="E116" s="49" t="s">
+      <c r="E118" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="J116" s="50"/>
-      <c r="K116" s="51"/>
-      <c r="L116" s="51"/>
-      <c r="M116" s="51"/>
-      <c r="N116" s="51"/>
-      <c r="O116" s="51"/>
-      <c r="Q116" s="52"/>
-    </row>
-    <row r="117" spans="1:17">
-      <c r="B117" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D117" s="31" t="s">
-        <v>834</v>
-      </c>
-      <c r="E117" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="F117" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H117" s="31" t="s">
-        <v>417</v>
-      </c>
-      <c r="I117" s="30" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="118" spans="1:17">
-      <c r="B118" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D118" s="31" t="s">
-        <v>835</v>
-      </c>
-      <c r="E118" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="F118" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="H118" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="I118" s="31"/>
+      <c r="J118" s="50"/>
+      <c r="K118" s="51"/>
+      <c r="L118" s="51"/>
+      <c r="M118" s="51"/>
+      <c r="N118" s="51"/>
+      <c r="O118" s="51"/>
+      <c r="Q118" s="52"/>
     </row>
     <row r="119" spans="1:17">
       <c r="B119" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D119" s="31" t="s">
-        <v>836</v>
+        <v>209</v>
       </c>
       <c r="E119" s="31" t="s">
-        <v>128</v>
+        <v>868</v>
       </c>
       <c r="F119" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="H119" s="31">
-        <v>0</v>
-      </c>
-      <c r="I119" s="31"/>
-    </row>
-    <row r="120" spans="1:17">
-      <c r="B120" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D120" s="31" t="s">
-        <v>837</v>
-      </c>
-      <c r="E120" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="F120" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="H120" s="31">
-        <v>0</v>
-      </c>
-      <c r="I120" s="31"/>
+        <v>62</v>
+      </c>
+      <c r="H119" s="31" t="s">
+        <v>867</v>
+      </c>
+      <c r="I119" s="30" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="120" spans="1:17" s="49" customFormat="1">
+      <c r="A120" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="B120" s="49" t="s">
+        <v>216</v>
+      </c>
+      <c r="C120" s="49" t="s">
+        <v>217</v>
+      </c>
+      <c r="D120" s="49" t="s">
+        <v>217</v>
+      </c>
+      <c r="E120" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="J120" s="50"/>
+      <c r="K120" s="51"/>
+      <c r="L120" s="51"/>
+      <c r="M120" s="51"/>
+      <c r="N120" s="51"/>
+      <c r="O120" s="51"/>
+      <c r="Q120" s="52"/>
     </row>
     <row r="121" spans="1:17">
       <c r="B121" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D121" s="31" t="s">
-        <v>794</v>
+        <v>834</v>
       </c>
       <c r="E121" s="31" t="s">
-        <v>52</v>
+        <v>219</v>
       </c>
       <c r="F121" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G121" s="30" t="s">
-        <v>795</v>
-      </c>
-      <c r="H121" s="31">
-        <v>0</v>
-      </c>
-      <c r="I121" s="31"/>
+        <v>62</v>
+      </c>
+      <c r="H121" s="31" t="s">
+        <v>873</v>
+      </c>
+      <c r="I121" s="30" t="s">
+        <v>874</v>
+      </c>
     </row>
     <row r="122" spans="1:17">
       <c r="B122" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D122" s="31" t="s">
-        <v>796</v>
+        <v>835</v>
       </c>
       <c r="E122" s="31" t="s">
-        <v>54</v>
+        <v>221</v>
       </c>
       <c r="F122" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="G122" s="30"/>
-      <c r="H122" s="31" t="b">
-        <v>0</v>
+        <v>64</v>
+      </c>
+      <c r="G122" s="31" t="s">
+        <v>836</v>
+      </c>
+      <c r="H122" s="31">
+        <v>69</v>
       </c>
       <c r="I122" s="31"/>
     </row>
@@ -10157,403 +10159,124 @@
       <c r="B123" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D123" s="30" t="s">
-        <v>797</v>
-      </c>
-      <c r="E123" s="30" t="s">
-        <v>56</v>
+      <c r="D123" s="31" t="s">
+        <v>837</v>
+      </c>
+      <c r="E123" s="31" t="s">
+        <v>227</v>
       </c>
       <c r="F123" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G123" s="30" t="s">
-        <v>795</v>
+        <v>64</v>
+      </c>
+      <c r="G123" s="31" t="s">
+        <v>836</v>
       </c>
       <c r="H123" s="31">
-        <v>15</v>
+        <v>-148</v>
       </c>
       <c r="I123" s="31"/>
     </row>
     <row r="124" spans="1:17">
-      <c r="B124" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D124" s="30" t="s">
-        <v>850</v>
-      </c>
-      <c r="E124" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="F124" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G124" s="30" t="s">
-        <v>791</v>
-      </c>
-      <c r="H124" s="31">
-        <v>0</v>
-      </c>
+      <c r="H124" s="31"/>
       <c r="I124" s="31"/>
     </row>
     <row r="125" spans="1:17">
-      <c r="B125" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D125" s="30" t="s">
-        <v>799</v>
-      </c>
-      <c r="E125" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="F125" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G125" s="30" t="s">
-        <v>795</v>
-      </c>
-      <c r="H125" s="31">
-        <v>1</v>
-      </c>
+      <c r="H125" s="31"/>
       <c r="I125" s="31"/>
     </row>
-    <row r="126" spans="1:17" s="49" customFormat="1">
-      <c r="A126" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B126" s="49" t="s">
-        <v>216</v>
-      </c>
-      <c r="C126" s="49" t="s">
-        <v>217</v>
-      </c>
-      <c r="D126" s="49" t="s">
-        <v>217</v>
-      </c>
-      <c r="E126" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="J126" s="50"/>
-      <c r="K126" s="51"/>
-      <c r="L126" s="51"/>
-      <c r="M126" s="51"/>
-      <c r="N126" s="51"/>
-      <c r="O126" s="51"/>
-      <c r="Q126" s="52"/>
+    <row r="126" spans="1:17">
+      <c r="H126" s="31"/>
+      <c r="I126" s="31"/>
     </row>
     <row r="127" spans="1:17">
-      <c r="B127" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D127" s="31" t="s">
-        <v>834</v>
-      </c>
-      <c r="E127" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="F127" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H127" s="31" t="s">
-        <v>417</v>
-      </c>
-      <c r="I127" s="30" t="s">
-        <v>418</v>
-      </c>
+      <c r="H127" s="31"/>
+      <c r="I127" s="31"/>
     </row>
     <row r="128" spans="1:17">
-      <c r="B128" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D128" s="31" t="s">
-        <v>840</v>
-      </c>
-      <c r="E128" s="31" t="s">
-        <v>219</v>
-      </c>
-      <c r="F128" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H128" s="31" t="s">
-        <v>838</v>
-      </c>
-      <c r="I128" s="30" t="s">
-        <v>839</v>
-      </c>
-    </row>
-    <row r="129" spans="2:9">
-      <c r="B129" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D129" s="31" t="s">
-        <v>841</v>
-      </c>
-      <c r="E129" s="31" t="s">
-        <v>221</v>
-      </c>
-      <c r="F129" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G129" s="31" t="s">
-        <v>842</v>
-      </c>
-      <c r="H129" s="31">
-        <v>69</v>
-      </c>
+      <c r="H128" s="31"/>
+      <c r="I128" s="31"/>
+    </row>
+    <row r="129" spans="8:9">
+      <c r="H129" s="31"/>
       <c r="I129" s="31"/>
     </row>
-    <row r="130" spans="2:9">
-      <c r="B130" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D130" s="31" t="s">
-        <v>844</v>
-      </c>
-      <c r="E130" s="31" t="s">
-        <v>223</v>
-      </c>
-      <c r="F130" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G130" s="31" t="s">
-        <v>843</v>
-      </c>
-      <c r="H130" s="31">
-        <v>28</v>
-      </c>
+    <row r="130" spans="8:9">
+      <c r="H130" s="31"/>
       <c r="I130" s="31"/>
     </row>
-    <row r="131" spans="2:9">
-      <c r="B131" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D131" s="31" t="s">
-        <v>845</v>
-      </c>
-      <c r="E131" s="31" t="s">
-        <v>225</v>
-      </c>
-      <c r="F131" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G131" s="31" t="s">
-        <v>842</v>
-      </c>
-      <c r="H131" s="31">
-        <v>55</v>
-      </c>
+    <row r="131" spans="8:9" ht="409.6">
+      <c r="H131" s="31"/>
       <c r="I131" s="31"/>
     </row>
-    <row r="132" spans="2:9">
-      <c r="B132" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D132" s="31" t="s">
-        <v>846</v>
-      </c>
-      <c r="E132" s="31" t="s">
-        <v>227</v>
-      </c>
-      <c r="F132" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G132" s="31" t="s">
-        <v>842</v>
-      </c>
-      <c r="H132" s="31">
-        <v>-148</v>
-      </c>
+    <row r="132" spans="8:9" ht="409.6">
+      <c r="H132" s="31"/>
       <c r="I132" s="31"/>
     </row>
-    <row r="133" spans="2:9">
-      <c r="B133" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D133" s="31" t="s">
-        <v>835</v>
-      </c>
-      <c r="E133" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="F133" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="H133" s="31" t="b">
-        <v>0</v>
-      </c>
+    <row r="133" spans="8:9" ht="409.6">
+      <c r="H133" s="31"/>
       <c r="I133" s="31"/>
     </row>
-    <row r="134" spans="2:9">
-      <c r="B134" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D134" s="31" t="s">
-        <v>847</v>
-      </c>
-      <c r="E134" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="F134" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="H134" s="31">
-        <v>0</v>
-      </c>
+    <row r="134" spans="8:9" ht="409.6">
+      <c r="H134" s="31"/>
       <c r="I134" s="31"/>
     </row>
-    <row r="135" spans="2:9">
-      <c r="B135" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D135" s="31" t="s">
-        <v>848</v>
-      </c>
-      <c r="E135" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="F135" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="H135" s="31">
-        <v>0</v>
-      </c>
+    <row r="135" spans="8:9" ht="409.6">
+      <c r="H135" s="31"/>
       <c r="I135" s="31"/>
     </row>
-    <row r="136" spans="2:9">
-      <c r="B136" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D136" s="31" t="s">
-        <v>794</v>
-      </c>
-      <c r="E136" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="F136" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G136" s="30" t="s">
-        <v>795</v>
-      </c>
-      <c r="H136" s="31">
-        <v>0</v>
-      </c>
+    <row r="136" spans="8:9" ht="409.6">
+      <c r="H136" s="31"/>
       <c r="I136" s="31"/>
     </row>
-    <row r="137" spans="2:9">
-      <c r="B137" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D137" s="31" t="s">
-        <v>796</v>
-      </c>
-      <c r="E137" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="F137" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="G137" s="30"/>
-      <c r="H137" s="31" t="b">
-        <v>0</v>
-      </c>
+    <row r="137" spans="8:9" ht="409.6">
+      <c r="H137" s="31"/>
       <c r="I137" s="31"/>
     </row>
-    <row r="138" spans="2:9">
-      <c r="B138" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D138" s="30" t="s">
-        <v>797</v>
-      </c>
-      <c r="E138" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="F138" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G138" s="30" t="s">
-        <v>795</v>
-      </c>
-      <c r="H138" s="31">
-        <v>15</v>
-      </c>
+    <row r="138" spans="8:9" ht="409.6">
+      <c r="H138" s="31"/>
       <c r="I138" s="31"/>
     </row>
-    <row r="139" spans="2:9">
-      <c r="B139" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D139" s="30" t="s">
-        <v>849</v>
-      </c>
-      <c r="E139" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="F139" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G139" s="30" t="s">
-        <v>791</v>
-      </c>
-      <c r="H139" s="31">
-        <v>0</v>
-      </c>
+    <row r="139" spans="8:9" ht="409.6">
+      <c r="H139" s="31"/>
       <c r="I139" s="31"/>
     </row>
-    <row r="140" spans="2:9">
-      <c r="B140" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D140" s="30" t="s">
-        <v>799</v>
-      </c>
-      <c r="E140" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="F140" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G140" s="30" t="s">
-        <v>795</v>
-      </c>
-      <c r="H140" s="31">
-        <v>1</v>
-      </c>
+    <row r="140" spans="8:9" ht="409.6">
+      <c r="H140" s="31"/>
       <c r="I140" s="31"/>
     </row>
-    <row r="141" spans="2:9">
+    <row r="141" spans="8:9" ht="409.6">
       <c r="H141" s="31"/>
       <c r="I141" s="31"/>
     </row>
-    <row r="142" spans="2:9">
+    <row r="142" spans="8:9">
       <c r="H142" s="31"/>
       <c r="I142" s="31"/>
     </row>
-    <row r="143" spans="2:9">
+    <row r="143" spans="8:9">
       <c r="H143" s="31"/>
       <c r="I143" s="31"/>
     </row>
-    <row r="144" spans="2:9">
+    <row r="144" spans="8:9">
       <c r="H144" s="31"/>
       <c r="I144" s="31"/>
     </row>
-    <row r="145" spans="8:9">
+    <row r="145" spans="8:9" ht="409.6">
       <c r="H145" s="31"/>
       <c r="I145" s="31"/>
     </row>
-    <row r="146" spans="8:9">
+    <row r="146" spans="8:9" ht="409.6">
       <c r="H146" s="31"/>
       <c r="I146" s="31"/>
     </row>
-    <row r="147" spans="8:9">
+    <row r="147" spans="8:9" ht="409.6">
       <c r="H147" s="31"/>
       <c r="I147" s="31"/>
     </row>
-    <row r="148" spans="8:9">
+    <row r="148" spans="8:9" ht="409.6">
       <c r="H148" s="31"/>
       <c r="I148" s="31"/>
     </row>
-    <row r="149" spans="8:9">
+    <row r="149" spans="8:9" ht="409.6">
       <c r="H149" s="31"/>
       <c r="I149" s="31"/>
     </row>
@@ -10777,76 +10500,8 @@
       <c r="H204" s="31"/>
       <c r="I204" s="31"/>
     </row>
-    <row r="205" spans="8:9">
-      <c r="H205" s="31"/>
-      <c r="I205" s="31"/>
-    </row>
-    <row r="206" spans="8:9">
-      <c r="H206" s="31"/>
-      <c r="I206" s="31"/>
-    </row>
-    <row r="207" spans="8:9">
-      <c r="H207" s="31"/>
-      <c r="I207" s="31"/>
-    </row>
-    <row r="208" spans="8:9">
-      <c r="H208" s="31"/>
-      <c r="I208" s="31"/>
-    </row>
-    <row r="209" spans="8:9">
-      <c r="H209" s="31"/>
-      <c r="I209" s="31"/>
-    </row>
-    <row r="210" spans="8:9">
-      <c r="H210" s="31"/>
-      <c r="I210" s="31"/>
-    </row>
-    <row r="211" spans="8:9">
-      <c r="H211" s="31"/>
-      <c r="I211" s="31"/>
-    </row>
-    <row r="212" spans="8:9">
-      <c r="H212" s="31"/>
-      <c r="I212" s="31"/>
-    </row>
-    <row r="213" spans="8:9">
-      <c r="H213" s="31"/>
-      <c r="I213" s="31"/>
-    </row>
-    <row r="214" spans="8:9">
-      <c r="H214" s="31"/>
-      <c r="I214" s="31"/>
-    </row>
-    <row r="215" spans="8:9">
-      <c r="H215" s="31"/>
-      <c r="I215" s="31"/>
-    </row>
-    <row r="216" spans="8:9">
-      <c r="H216" s="31"/>
-      <c r="I216" s="31"/>
-    </row>
-    <row r="217" spans="8:9">
-      <c r="H217" s="31"/>
-      <c r="I217" s="31"/>
-    </row>
-    <row r="218" spans="8:9">
-      <c r="H218" s="31"/>
-      <c r="I218" s="31"/>
-    </row>
-    <row r="219" spans="8:9">
-      <c r="H219" s="31"/>
-      <c r="I219" s="31"/>
-    </row>
-    <row r="220" spans="8:9">
-      <c r="H220" s="31"/>
-      <c r="I220" s="31"/>
-    </row>
-    <row r="221" spans="8:9">
-      <c r="H221" s="31"/>
-      <c r="I221" s="31"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A2:Z148"/>
+  <autoFilter ref="A2:Z131"/>
   <mergeCells count="1">
     <mergeCell ref="T1:Y1"/>
   </mergeCells>
@@ -10869,20 +10524,20 @@
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="29.5" style="31" customWidth="1"/>
+    <col min="1" max="2" width="29.42578125" style="31" customWidth="1"/>
     <col min="3" max="3" width="71" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" style="31" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.5" style="31" customWidth="1"/>
-    <col min="8" max="8" width="14.5" style="31" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" style="31" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" style="31" customWidth="1"/>
-    <col min="11" max="16384" width="11.5" style="31"/>
+    <col min="4" max="4" width="10.42578125" style="31" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.42578125" style="31" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="31" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="31" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" style="31" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18">
+    <row r="1" spans="1:12" ht="18.75">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -10897,7 +10552,7 @@
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
     </row>
-    <row r="2" spans="1:12" s="8" customFormat="1" ht="15">
+    <row r="2" spans="1:12" s="8" customFormat="1" ht="15.75">
       <c r="A2" s="8" t="s">
         <v>459</v>
       </c>
@@ -10932,7 +10587,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="14" customFormat="1" ht="30">
+    <row r="3" spans="1:12" s="14" customFormat="1" ht="47.25">
       <c r="A3" s="14" t="s">
         <v>628</v>
       </c>
@@ -11796,19 +11451,19 @@
       <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="80.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="255.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15">
+    <row r="1" spans="1:9" ht="15.75">
       <c r="A1" s="17" t="b">
         <v>0</v>
       </c>
@@ -11827,7 +11482,7 @@
       <c r="H1" s="17"/>
       <c r="I1" s="17"/>
     </row>
-    <row r="2" spans="1:9" ht="15">
+    <row r="2" spans="1:9" ht="15.75">
       <c r="A2" s="17"/>
       <c r="B2" s="17" t="s">
         <v>21</v>
@@ -11848,7 +11503,7 @@
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
     </row>
-    <row r="3" spans="1:9" ht="15">
+    <row r="3" spans="1:9" ht="15.75">
       <c r="A3" s="17"/>
       <c r="B3" s="17" t="s">
         <v>21</v>
@@ -11871,7 +11526,7 @@
       </c>
       <c r="I3" s="17"/>
     </row>
-    <row r="4" spans="1:9" ht="15">
+    <row r="4" spans="1:9" ht="15.75">
       <c r="A4" s="17"/>
       <c r="B4" s="17" t="s">
         <v>21</v>
@@ -11894,7 +11549,7 @@
       </c>
       <c r="I4" s="17"/>
     </row>
-    <row r="5" spans="1:9" ht="15">
+    <row r="5" spans="1:9" ht="15.75">
       <c r="A5" s="17"/>
       <c r="B5" s="17" t="s">
         <v>21</v>
@@ -11917,7 +11572,7 @@
       </c>
       <c r="I5" s="17"/>
     </row>
-    <row r="6" spans="1:9" ht="15">
+    <row r="6" spans="1:9" ht="15.75">
       <c r="A6" s="17"/>
       <c r="B6" s="17" t="s">
         <v>21</v>
@@ -11940,7 +11595,7 @@
       </c>
       <c r="I6" s="17"/>
     </row>
-    <row r="7" spans="1:9" ht="15">
+    <row r="7" spans="1:9" ht="15.75">
       <c r="A7" s="17"/>
       <c r="B7" s="17" t="s">
         <v>21</v>
@@ -11963,7 +11618,7 @@
       </c>
       <c r="I7" s="17"/>
     </row>
-    <row r="8" spans="1:9" ht="15">
+    <row r="8" spans="1:9" ht="15.75">
       <c r="A8" s="17"/>
       <c r="B8" s="17" t="s">
         <v>21</v>
@@ -11986,7 +11641,7 @@
       </c>
       <c r="I8" s="17"/>
     </row>
-    <row r="9" spans="1:9" ht="15">
+    <row r="9" spans="1:9" ht="15.75">
       <c r="A9" s="17"/>
       <c r="B9" s="17" t="s">
         <v>21</v>
@@ -12009,7 +11664,7 @@
       </c>
       <c r="I9" s="17"/>
     </row>
-    <row r="10" spans="1:9" ht="15">
+    <row r="10" spans="1:9" ht="15.75">
       <c r="A10" s="17"/>
       <c r="B10" s="17" t="s">
         <v>21</v>
@@ -12032,7 +11687,7 @@
       </c>
       <c r="I10" s="17"/>
     </row>
-    <row r="11" spans="1:9" ht="15">
+    <row r="11" spans="1:9" ht="15.75">
       <c r="A11" s="17" t="b">
         <v>0</v>
       </c>
@@ -12051,7 +11706,7 @@
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
     </row>
-    <row r="12" spans="1:9" ht="15">
+    <row r="12" spans="1:9" ht="15.75">
       <c r="A12" s="17"/>
       <c r="B12" s="17" t="s">
         <v>21</v>
@@ -12072,7 +11727,7 @@
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
     </row>
-    <row r="13" spans="1:9" ht="15">
+    <row r="13" spans="1:9" ht="15.75">
       <c r="A13" s="17"/>
       <c r="B13" s="17" t="s">
         <v>21</v>
@@ -12095,7 +11750,7 @@
       </c>
       <c r="I13" s="17"/>
     </row>
-    <row r="14" spans="1:9" ht="15">
+    <row r="14" spans="1:9" ht="15.75">
       <c r="A14" s="17"/>
       <c r="B14" s="17" t="s">
         <v>21</v>
@@ -12118,7 +11773,7 @@
       </c>
       <c r="I14" s="17"/>
     </row>
-    <row r="15" spans="1:9" ht="15">
+    <row r="15" spans="1:9" ht="15.75">
       <c r="A15" s="17"/>
       <c r="B15" s="17" t="s">
         <v>21</v>
@@ -12141,7 +11796,7 @@
       </c>
       <c r="I15" s="17"/>
     </row>
-    <row r="16" spans="1:9" ht="15">
+    <row r="16" spans="1:9" ht="15.75">
       <c r="A16" s="17"/>
       <c r="B16" s="17" t="s">
         <v>21</v>
@@ -12164,7 +11819,7 @@
       </c>
       <c r="I16" s="17"/>
     </row>
-    <row r="17" spans="1:9" ht="15">
+    <row r="17" spans="1:9" ht="15.75">
       <c r="A17" s="17"/>
       <c r="B17" s="17" t="s">
         <v>21</v>
@@ -12187,7 +11842,7 @@
       </c>
       <c r="I17" s="17"/>
     </row>
-    <row r="18" spans="1:9" ht="15">
+    <row r="18" spans="1:9" ht="15.75">
       <c r="A18" s="17"/>
       <c r="B18" s="17" t="s">
         <v>21</v>
@@ -12210,7 +11865,7 @@
       </c>
       <c r="I18" s="17"/>
     </row>
-    <row r="19" spans="1:9" ht="15">
+    <row r="19" spans="1:9" ht="15.75">
       <c r="A19" s="17"/>
       <c r="B19" s="17" t="s">
         <v>21</v>
@@ -12233,7 +11888,7 @@
       </c>
       <c r="I19" s="17"/>
     </row>
-    <row r="20" spans="1:9" ht="15">
+    <row r="20" spans="1:9" ht="15.75">
       <c r="A20" s="17"/>
       <c r="B20" s="17" t="s">
         <v>21</v>
@@ -12256,7 +11911,7 @@
       </c>
       <c r="I20" s="17"/>
     </row>
-    <row r="21" spans="1:9" ht="15">
+    <row r="21" spans="1:9" ht="15.75">
       <c r="A21" s="17" t="b">
         <v>0</v>
       </c>
@@ -12275,7 +11930,7 @@
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
     </row>
-    <row r="22" spans="1:9" ht="15">
+    <row r="22" spans="1:9" ht="15.75">
       <c r="A22" s="17"/>
       <c r="B22" s="17" t="s">
         <v>21</v>
@@ -12298,7 +11953,7 @@
       </c>
       <c r="I22" s="17"/>
     </row>
-    <row r="23" spans="1:9" ht="15">
+    <row r="23" spans="1:9" ht="15.75">
       <c r="A23" s="17"/>
       <c r="B23" s="17" t="s">
         <v>21</v>
@@ -12321,7 +11976,7 @@
       </c>
       <c r="I23" s="17"/>
     </row>
-    <row r="24" spans="1:9" ht="15">
+    <row r="24" spans="1:9" ht="15.75">
       <c r="A24" s="17"/>
       <c r="B24" s="17" t="s">
         <v>21</v>
@@ -12344,7 +11999,7 @@
       </c>
       <c r="I24" s="17"/>
     </row>
-    <row r="25" spans="1:9" ht="15">
+    <row r="25" spans="1:9" ht="15.75">
       <c r="A25" s="17"/>
       <c r="B25" s="17" t="s">
         <v>21</v>
@@ -12367,7 +12022,7 @@
       </c>
       <c r="I25" s="17"/>
     </row>
-    <row r="26" spans="1:9" ht="15">
+    <row r="26" spans="1:9" ht="15.75">
       <c r="A26" s="17"/>
       <c r="B26" s="17" t="s">
         <v>21</v>
@@ -12390,7 +12045,7 @@
       </c>
       <c r="I26" s="17"/>
     </row>
-    <row r="27" spans="1:9" ht="15">
+    <row r="27" spans="1:9" ht="15.75">
       <c r="A27" s="17"/>
       <c r="B27" s="17" t="s">
         <v>21</v>
@@ -12413,7 +12068,7 @@
       </c>
       <c r="I27" s="17"/>
     </row>
-    <row r="28" spans="1:9" ht="15">
+    <row r="28" spans="1:9" ht="15.75">
       <c r="A28" s="17"/>
       <c r="B28" s="17" t="s">
         <v>21</v>
@@ -12436,7 +12091,7 @@
       </c>
       <c r="I28" s="17"/>
     </row>
-    <row r="29" spans="1:9" ht="15">
+    <row r="29" spans="1:9" ht="15.75">
       <c r="A29" s="17"/>
       <c r="B29" s="17" t="s">
         <v>21</v>
@@ -12459,7 +12114,7 @@
       </c>
       <c r="I29" s="17"/>
     </row>
-    <row r="30" spans="1:9" ht="15">
+    <row r="30" spans="1:9" ht="15.75">
       <c r="A30" s="17"/>
       <c r="B30" s="17" t="s">
         <v>21</v>
@@ -12482,7 +12137,7 @@
       </c>
       <c r="I30" s="17"/>
     </row>
-    <row r="31" spans="1:9" ht="15">
+    <row r="31" spans="1:9" ht="15.75">
       <c r="A31" s="17" t="b">
         <v>0</v>
       </c>
@@ -12501,7 +12156,7 @@
       <c r="H31" s="17"/>
       <c r="I31" s="17"/>
     </row>
-    <row r="32" spans="1:9" ht="15">
+    <row r="32" spans="1:9" ht="15.75">
       <c r="A32" s="17"/>
       <c r="B32" s="17" t="s">
         <v>21</v>
@@ -12522,7 +12177,7 @@
       <c r="H32" s="17"/>
       <c r="I32" s="17"/>
     </row>
-    <row r="33" spans="1:9" ht="15">
+    <row r="33" spans="1:9" ht="15.75">
       <c r="A33" s="17"/>
       <c r="B33" s="17" t="s">
         <v>21</v>
@@ -12545,7 +12200,7 @@
       </c>
       <c r="I33" s="17"/>
     </row>
-    <row r="34" spans="1:9" ht="15">
+    <row r="34" spans="1:9" ht="15.75">
       <c r="A34" s="17"/>
       <c r="B34" s="17" t="s">
         <v>21</v>
@@ -12568,7 +12223,7 @@
       </c>
       <c r="I34" s="17"/>
     </row>
-    <row r="35" spans="1:9" ht="15">
+    <row r="35" spans="1:9" ht="15.75">
       <c r="A35" s="17"/>
       <c r="B35" s="17" t="s">
         <v>21</v>
@@ -12591,7 +12246,7 @@
       </c>
       <c r="I35" s="17"/>
     </row>
-    <row r="36" spans="1:9" ht="15">
+    <row r="36" spans="1:9" ht="15.75">
       <c r="A36" s="17"/>
       <c r="B36" s="17" t="s">
         <v>21</v>
@@ -12614,7 +12269,7 @@
       </c>
       <c r="I36" s="17"/>
     </row>
-    <row r="37" spans="1:9" ht="15">
+    <row r="37" spans="1:9" ht="15.75">
       <c r="A37" s="17"/>
       <c r="B37" s="17" t="s">
         <v>21</v>
@@ -12637,7 +12292,7 @@
       </c>
       <c r="I37" s="17"/>
     </row>
-    <row r="38" spans="1:9" ht="15">
+    <row r="38" spans="1:9" ht="15.75">
       <c r="A38" s="17"/>
       <c r="B38" s="17" t="s">
         <v>21</v>
@@ -12660,7 +12315,7 @@
       </c>
       <c r="I38" s="17"/>
     </row>
-    <row r="39" spans="1:9" ht="15">
+    <row r="39" spans="1:9" ht="15.75">
       <c r="A39" s="17"/>
       <c r="B39" s="17" t="s">
         <v>21</v>
@@ -12683,7 +12338,7 @@
       </c>
       <c r="I39" s="17"/>
     </row>
-    <row r="40" spans="1:9" ht="15">
+    <row r="40" spans="1:9" ht="15.75">
       <c r="A40" s="17"/>
       <c r="B40" s="17" t="s">
         <v>21</v>
@@ -12706,7 +12361,7 @@
       </c>
       <c r="I40" s="17"/>
     </row>
-    <row r="41" spans="1:9" ht="15">
+    <row r="41" spans="1:9" ht="15.75">
       <c r="A41" s="17" t="b">
         <v>0</v>
       </c>
@@ -12725,7 +12380,7 @@
       <c r="H41" s="17"/>
       <c r="I41" s="17"/>
     </row>
-    <row r="42" spans="1:9" ht="15">
+    <row r="42" spans="1:9" ht="15.75">
       <c r="A42" s="17"/>
       <c r="B42" s="17" t="s">
         <v>21</v>
@@ -12746,7 +12401,7 @@
       <c r="H42" s="17"/>
       <c r="I42" s="17"/>
     </row>
-    <row r="43" spans="1:9" ht="15">
+    <row r="43" spans="1:9" ht="15.75">
       <c r="A43" s="17"/>
       <c r="B43" s="17" t="s">
         <v>21</v>
@@ -12769,7 +12424,7 @@
       </c>
       <c r="I43" s="17"/>
     </row>
-    <row r="44" spans="1:9" ht="15">
+    <row r="44" spans="1:9" ht="15.75">
       <c r="A44" s="17"/>
       <c r="B44" s="17" t="s">
         <v>21</v>
@@ -12792,7 +12447,7 @@
       </c>
       <c r="I44" s="17"/>
     </row>
-    <row r="45" spans="1:9" ht="15">
+    <row r="45" spans="1:9" ht="15.75">
       <c r="A45" s="17"/>
       <c r="B45" s="17" t="s">
         <v>21</v>
@@ -12815,7 +12470,7 @@
       </c>
       <c r="I45" s="17"/>
     </row>
-    <row r="46" spans="1:9" ht="15">
+    <row r="46" spans="1:9" ht="15.75">
       <c r="A46" s="17"/>
       <c r="B46" s="17" t="s">
         <v>21</v>
@@ -12838,7 +12493,7 @@
       </c>
       <c r="I46" s="17"/>
     </row>
-    <row r="47" spans="1:9" ht="15">
+    <row r="47" spans="1:9" ht="15.75">
       <c r="A47" s="17"/>
       <c r="B47" s="17" t="s">
         <v>21</v>
@@ -12861,7 +12516,7 @@
       </c>
       <c r="I47" s="17"/>
     </row>
-    <row r="48" spans="1:9" ht="15">
+    <row r="48" spans="1:9" ht="15.75">
       <c r="A48" s="17"/>
       <c r="B48" s="17" t="s">
         <v>21</v>
@@ -12884,7 +12539,7 @@
       </c>
       <c r="I48" s="17"/>
     </row>
-    <row r="49" spans="1:9" ht="15">
+    <row r="49" spans="1:9" ht="15.75">
       <c r="A49" s="17"/>
       <c r="B49" s="17" t="s">
         <v>21</v>
@@ -12907,7 +12562,7 @@
       </c>
       <c r="I49" s="17"/>
     </row>
-    <row r="50" spans="1:9" ht="15">
+    <row r="50" spans="1:9" ht="15.75">
       <c r="A50" s="17"/>
       <c r="B50" s="17" t="s">
         <v>21</v>
@@ -12930,7 +12585,7 @@
       </c>
       <c r="I50" s="17"/>
     </row>
-    <row r="51" spans="1:9" ht="15">
+    <row r="51" spans="1:9" ht="15.75">
       <c r="A51" s="17" t="b">
         <v>0</v>
       </c>
@@ -12949,7 +12604,7 @@
       <c r="H51" s="17"/>
       <c r="I51" s="17"/>
     </row>
-    <row r="52" spans="1:9" ht="15">
+    <row r="52" spans="1:9" ht="15.75">
       <c r="A52" s="17"/>
       <c r="B52" s="17" t="s">
         <v>21</v>
@@ -12970,7 +12625,7 @@
       <c r="H52" s="17"/>
       <c r="I52" s="17"/>
     </row>
-    <row r="53" spans="1:9" ht="15">
+    <row r="53" spans="1:9" ht="15.75">
       <c r="A53" s="17"/>
       <c r="B53" s="17" t="s">
         <v>21</v>
@@ -12993,7 +12648,7 @@
       </c>
       <c r="I53" s="17"/>
     </row>
-    <row r="54" spans="1:9" ht="15">
+    <row r="54" spans="1:9" ht="15.75">
       <c r="A54" s="17"/>
       <c r="B54" s="17" t="s">
         <v>21</v>
@@ -13016,7 +12671,7 @@
       </c>
       <c r="I54" s="17"/>
     </row>
-    <row r="55" spans="1:9" ht="15">
+    <row r="55" spans="1:9" ht="15.75">
       <c r="A55" s="17"/>
       <c r="B55" s="17" t="s">
         <v>21</v>
@@ -13039,7 +12694,7 @@
       </c>
       <c r="I55" s="17"/>
     </row>
-    <row r="56" spans="1:9" ht="15">
+    <row r="56" spans="1:9" ht="15.75">
       <c r="A56" s="17"/>
       <c r="B56" s="17" t="s">
         <v>21</v>
@@ -13062,7 +12717,7 @@
       </c>
       <c r="I56" s="17"/>
     </row>
-    <row r="57" spans="1:9" ht="15">
+    <row r="57" spans="1:9" ht="15.75">
       <c r="A57" s="17"/>
       <c r="B57" s="17" t="s">
         <v>21</v>
@@ -13085,7 +12740,7 @@
       </c>
       <c r="I57" s="17"/>
     </row>
-    <row r="58" spans="1:9" ht="15">
+    <row r="58" spans="1:9" ht="15.75">
       <c r="A58" s="17"/>
       <c r="B58" s="17" t="s">
         <v>21</v>
@@ -13108,7 +12763,7 @@
       </c>
       <c r="I58" s="17"/>
     </row>
-    <row r="59" spans="1:9" ht="15">
+    <row r="59" spans="1:9" ht="15.75">
       <c r="A59" s="17"/>
       <c r="B59" s="17" t="s">
         <v>21</v>
@@ -13131,7 +12786,7 @@
       </c>
       <c r="I59" s="17"/>
     </row>
-    <row r="60" spans="1:9" ht="15">
+    <row r="60" spans="1:9" ht="15.75">
       <c r="A60" s="17"/>
       <c r="B60" s="17" t="s">
         <v>21</v>
@@ -13154,7 +12809,7 @@
       </c>
       <c r="I60" s="17"/>
     </row>
-    <row r="61" spans="1:9" ht="15">
+    <row r="61" spans="1:9" ht="15.75">
       <c r="A61" s="17" t="b">
         <v>0</v>
       </c>
@@ -13173,7 +12828,7 @@
       <c r="H61" s="17"/>
       <c r="I61" s="17"/>
     </row>
-    <row r="62" spans="1:9" ht="15">
+    <row r="62" spans="1:9" ht="15.75">
       <c r="A62" s="17"/>
       <c r="B62" s="17" t="s">
         <v>21</v>
@@ -13194,7 +12849,7 @@
       <c r="H62" s="17"/>
       <c r="I62" s="17"/>
     </row>
-    <row r="63" spans="1:9" ht="15">
+    <row r="63" spans="1:9" ht="15.75">
       <c r="A63" s="17"/>
       <c r="B63" s="17" t="s">
         <v>21</v>
@@ -13219,7 +12874,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="15">
+    <row r="64" spans="1:9" ht="15.75">
       <c r="A64" s="17"/>
       <c r="B64" s="17" t="s">
         <v>21</v>
@@ -13242,7 +12897,7 @@
       </c>
       <c r="I64" s="17"/>
     </row>
-    <row r="65" spans="1:9" ht="15">
+    <row r="65" spans="1:9" ht="15.75">
       <c r="A65" s="17"/>
       <c r="B65" s="17" t="s">
         <v>21</v>
@@ -13265,7 +12920,7 @@
       </c>
       <c r="I65" s="17"/>
     </row>
-    <row r="66" spans="1:9" ht="15">
+    <row r="66" spans="1:9" ht="15.75">
       <c r="A66" s="17"/>
       <c r="B66" s="17" t="s">
         <v>21</v>
@@ -13288,7 +12943,7 @@
       </c>
       <c r="I66" s="17"/>
     </row>
-    <row r="67" spans="1:9" ht="15">
+    <row r="67" spans="1:9" ht="15.75">
       <c r="A67" s="17"/>
       <c r="B67" s="17" t="s">
         <v>21</v>
@@ -13311,7 +12966,7 @@
       </c>
       <c r="I67" s="17"/>
     </row>
-    <row r="68" spans="1:9" ht="15">
+    <row r="68" spans="1:9" ht="15.75">
       <c r="A68" s="17"/>
       <c r="B68" s="17" t="s">
         <v>21</v>
@@ -13334,7 +12989,7 @@
       </c>
       <c r="I68" s="17"/>
     </row>
-    <row r="69" spans="1:9" ht="15">
+    <row r="69" spans="1:9" ht="15.75">
       <c r="A69" s="17"/>
       <c r="B69" s="17" t="s">
         <v>21</v>
@@ -13357,7 +13012,7 @@
       </c>
       <c r="I69" s="17"/>
     </row>
-    <row r="70" spans="1:9" ht="15">
+    <row r="70" spans="1:9" ht="15.75">
       <c r="A70" s="17"/>
       <c r="B70" s="17" t="s">
         <v>21</v>
@@ -13380,7 +13035,7 @@
       </c>
       <c r="I70" s="17"/>
     </row>
-    <row r="71" spans="1:9" ht="15">
+    <row r="71" spans="1:9" ht="15.75">
       <c r="A71" s="17"/>
       <c r="B71" s="17" t="s">
         <v>21</v>
@@ -13403,7 +13058,7 @@
       </c>
       <c r="I71" s="17"/>
     </row>
-    <row r="72" spans="1:9" ht="15">
+    <row r="72" spans="1:9" ht="15.75">
       <c r="A72" s="17" t="b">
         <v>0</v>
       </c>
@@ -13422,7 +13077,7 @@
       <c r="H72" s="17"/>
       <c r="I72" s="17"/>
     </row>
-    <row r="73" spans="1:9" ht="15">
+    <row r="73" spans="1:9" ht="15.75">
       <c r="A73" s="17"/>
       <c r="B73" s="17" t="s">
         <v>21</v>
@@ -13443,7 +13098,7 @@
       <c r="H73" s="17"/>
       <c r="I73" s="17"/>
     </row>
-    <row r="74" spans="1:9" ht="15">
+    <row r="74" spans="1:9" ht="15.75">
       <c r="A74" s="17"/>
       <c r="B74" s="17" t="s">
         <v>21</v>
@@ -13466,7 +13121,7 @@
       </c>
       <c r="I74" s="17"/>
     </row>
-    <row r="75" spans="1:9" ht="15">
+    <row r="75" spans="1:9" ht="15.75">
       <c r="A75" s="17"/>
       <c r="B75" s="17" t="s">
         <v>21</v>
@@ -13491,7 +13146,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="15">
+    <row r="76" spans="1:9" ht="15.75">
       <c r="A76" s="17"/>
       <c r="B76" s="17" t="s">
         <v>21</v>
@@ -13514,7 +13169,7 @@
       </c>
       <c r="I76" s="17"/>
     </row>
-    <row r="77" spans="1:9" ht="15">
+    <row r="77" spans="1:9" ht="15.75">
       <c r="A77" s="17"/>
       <c r="B77" s="17" t="s">
         <v>21</v>
@@ -13537,7 +13192,7 @@
       </c>
       <c r="I77" s="17"/>
     </row>
-    <row r="78" spans="1:9" ht="15">
+    <row r="78" spans="1:9" ht="15.75">
       <c r="A78" s="17"/>
       <c r="B78" s="17" t="s">
         <v>21</v>
@@ -13560,7 +13215,7 @@
       </c>
       <c r="I78" s="17"/>
     </row>
-    <row r="79" spans="1:9" ht="15">
+    <row r="79" spans="1:9" ht="15.75">
       <c r="A79" s="17"/>
       <c r="B79" s="17" t="s">
         <v>21</v>
@@ -13583,7 +13238,7 @@
       </c>
       <c r="I79" s="17"/>
     </row>
-    <row r="80" spans="1:9" ht="15">
+    <row r="80" spans="1:9" ht="15.75">
       <c r="A80" s="17"/>
       <c r="B80" s="17" t="s">
         <v>21</v>
@@ -13606,7 +13261,7 @@
       </c>
       <c r="I80" s="17"/>
     </row>
-    <row r="81" spans="1:9" ht="15">
+    <row r="81" spans="1:9" ht="15.75">
       <c r="A81" s="17"/>
       <c r="B81" s="17" t="s">
         <v>21</v>
@@ -13629,7 +13284,7 @@
       </c>
       <c r="I81" s="17"/>
     </row>
-    <row r="82" spans="1:9" ht="15">
+    <row r="82" spans="1:9" ht="15.75">
       <c r="A82" s="17"/>
       <c r="B82" s="17" t="s">
         <v>21</v>
@@ -13652,7 +13307,7 @@
       </c>
       <c r="I82" s="17"/>
     </row>
-    <row r="83" spans="1:9" ht="15">
+    <row r="83" spans="1:9" ht="15.75">
       <c r="A83" s="17"/>
       <c r="B83" s="17" t="s">
         <v>21</v>
@@ -13675,7 +13330,7 @@
       </c>
       <c r="I83" s="17"/>
     </row>
-    <row r="84" spans="1:9" ht="15">
+    <row r="84" spans="1:9" ht="15.75">
       <c r="A84" s="17"/>
       <c r="B84" s="17" t="s">
         <v>21</v>
@@ -13698,7 +13353,7 @@
       </c>
       <c r="I84" s="17"/>
     </row>
-    <row r="85" spans="1:9" ht="15">
+    <row r="85" spans="1:9" ht="15.75">
       <c r="A85" s="17"/>
       <c r="B85" s="17" t="s">
         <v>21</v>
@@ -13721,7 +13376,7 @@
       </c>
       <c r="I85" s="17"/>
     </row>
-    <row r="86" spans="1:9" ht="15">
+    <row r="86" spans="1:9" ht="15.75">
       <c r="A86" s="17" t="b">
         <v>0</v>
       </c>
@@ -13740,7 +13395,7 @@
       <c r="H86" s="17"/>
       <c r="I86" s="17"/>
     </row>
-    <row r="87" spans="1:9" ht="15">
+    <row r="87" spans="1:9" ht="15.75">
       <c r="A87" s="17"/>
       <c r="B87" s="17" t="s">
         <v>21</v>
@@ -13763,7 +13418,7 @@
       </c>
       <c r="I87" s="17"/>
     </row>
-    <row r="88" spans="1:9" ht="15">
+    <row r="88" spans="1:9" ht="15.75">
       <c r="A88" s="17"/>
       <c r="B88" s="17" t="s">
         <v>21</v>
@@ -13786,7 +13441,7 @@
       </c>
       <c r="I88" s="17"/>
     </row>
-    <row r="89" spans="1:9" ht="15">
+    <row r="89" spans="1:9" ht="15.75">
       <c r="A89" s="17"/>
       <c r="B89" s="17" t="s">
         <v>21</v>
@@ -13809,7 +13464,7 @@
       </c>
       <c r="I89" s="17"/>
     </row>
-    <row r="90" spans="1:9" ht="15">
+    <row r="90" spans="1:9" ht="15.75">
       <c r="A90" s="17"/>
       <c r="B90" s="17" t="s">
         <v>21</v>
@@ -13832,7 +13487,7 @@
       </c>
       <c r="I90" s="17"/>
     </row>
-    <row r="91" spans="1:9" ht="15">
+    <row r="91" spans="1:9" ht="15.75">
       <c r="A91" s="17"/>
       <c r="B91" s="17" t="s">
         <v>21</v>
@@ -13855,7 +13510,7 @@
       </c>
       <c r="I91" s="17"/>
     </row>
-    <row r="92" spans="1:9" ht="15">
+    <row r="92" spans="1:9" ht="15.75">
       <c r="A92" s="17"/>
       <c r="B92" s="17" t="s">
         <v>21</v>
@@ -13878,7 +13533,7 @@
       </c>
       <c r="I92" s="17"/>
     </row>
-    <row r="93" spans="1:9" ht="15">
+    <row r="93" spans="1:9" ht="15.75">
       <c r="A93" s="17"/>
       <c r="B93" s="17" t="s">
         <v>21</v>
@@ -13901,7 +13556,7 @@
       </c>
       <c r="I93" s="17"/>
     </row>
-    <row r="94" spans="1:9" ht="15">
+    <row r="94" spans="1:9" ht="15.75">
       <c r="A94" s="17"/>
       <c r="B94" s="17" t="s">
         <v>21</v>
@@ -13924,7 +13579,7 @@
       </c>
       <c r="I94" s="17"/>
     </row>
-    <row r="95" spans="1:9" ht="15">
+    <row r="95" spans="1:9" ht="15.75">
       <c r="A95" s="17"/>
       <c r="B95" s="17" t="s">
         <v>21</v>
@@ -13947,7 +13602,7 @@
       </c>
       <c r="I95" s="17"/>
     </row>
-    <row r="96" spans="1:9" ht="15">
+    <row r="96" spans="1:9" ht="15.75">
       <c r="A96" s="17"/>
       <c r="B96" s="17" t="s">
         <v>21</v>
@@ -13970,7 +13625,7 @@
       </c>
       <c r="I96" s="17"/>
     </row>
-    <row r="97" spans="1:9" ht="15">
+    <row r="97" spans="1:9" ht="15.75">
       <c r="A97" s="17" t="b">
         <v>0</v>
       </c>
@@ -13989,7 +13644,7 @@
       <c r="H97" s="17"/>
       <c r="I97" s="17"/>
     </row>
-    <row r="98" spans="1:9" ht="15">
+    <row r="98" spans="1:9" ht="15.75">
       <c r="A98" s="17"/>
       <c r="B98" s="17" t="s">
         <v>21</v>
@@ -14014,7 +13669,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="15">
+    <row r="99" spans="1:9" ht="15.75">
       <c r="A99" s="17" t="b">
         <v>0</v>
       </c>
@@ -14033,7 +13688,7 @@
       <c r="H99" s="17"/>
       <c r="I99" s="17"/>
     </row>
-    <row r="100" spans="1:9" ht="15">
+    <row r="100" spans="1:9" ht="15.75">
       <c r="A100" s="17"/>
       <c r="B100" s="17" t="s">
         <v>21</v>
@@ -14054,7 +13709,7 @@
       <c r="H100" s="17"/>
       <c r="I100" s="17"/>
     </row>
-    <row r="101" spans="1:9" ht="15">
+    <row r="101" spans="1:9" ht="15.75">
       <c r="A101" s="17"/>
       <c r="B101" s="17" t="s">
         <v>21</v>
@@ -14079,7 +13734,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="15">
+    <row r="102" spans="1:9" ht="15.75">
       <c r="A102" s="17" t="b">
         <v>0</v>
       </c>
@@ -14098,7 +13753,7 @@
       <c r="H102" s="17"/>
       <c r="I102" s="17"/>
     </row>
-    <row r="103" spans="1:9" ht="15">
+    <row r="103" spans="1:9" ht="15.75">
       <c r="A103" s="17"/>
       <c r="B103" s="17" t="s">
         <v>21</v>
@@ -14121,7 +13776,7 @@
       </c>
       <c r="I103" s="17"/>
     </row>
-    <row r="104" spans="1:9" ht="15">
+    <row r="104" spans="1:9" ht="15.75">
       <c r="A104" s="17"/>
       <c r="B104" s="17" t="s">
         <v>21</v>
@@ -14146,7 +13801,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="15">
+    <row r="105" spans="1:9" ht="15.75">
       <c r="A105" s="17"/>
       <c r="B105" s="17" t="s">
         <v>21</v>
@@ -14169,7 +13824,7 @@
       </c>
       <c r="I105" s="17"/>
     </row>
-    <row r="106" spans="1:9" ht="15">
+    <row r="106" spans="1:9" ht="15.75">
       <c r="A106" s="17"/>
       <c r="B106" s="17" t="s">
         <v>21</v>
@@ -14190,7 +13845,7 @@
       <c r="H106" s="17"/>
       <c r="I106" s="17"/>
     </row>
-    <row r="107" spans="1:9" ht="15">
+    <row r="107" spans="1:9" ht="15.75">
       <c r="A107" s="17" t="b">
         <v>0</v>
       </c>
@@ -14209,7 +13864,7 @@
       <c r="H107" s="17"/>
       <c r="I107" s="17"/>
     </row>
-    <row r="108" spans="1:9" ht="15">
+    <row r="108" spans="1:9" ht="15.75">
       <c r="A108" s="17"/>
       <c r="B108" s="17" t="s">
         <v>21</v>
@@ -14234,7 +13889,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="15">
+    <row r="109" spans="1:9" ht="15.75">
       <c r="A109" s="17"/>
       <c r="B109" s="17" t="s">
         <v>21</v>
@@ -14257,7 +13912,7 @@
       </c>
       <c r="I109" s="17"/>
     </row>
-    <row r="110" spans="1:9" ht="15">
+    <row r="110" spans="1:9" ht="15.75">
       <c r="A110" s="17"/>
       <c r="B110" s="17" t="s">
         <v>21</v>
@@ -14280,7 +13935,7 @@
       </c>
       <c r="I110" s="17"/>
     </row>
-    <row r="111" spans="1:9" ht="15">
+    <row r="111" spans="1:9" ht="15.75">
       <c r="A111" s="17"/>
       <c r="B111" s="17" t="s">
         <v>21</v>
@@ -14303,7 +13958,7 @@
       </c>
       <c r="I111" s="17"/>
     </row>
-    <row r="112" spans="1:9" ht="15">
+    <row r="112" spans="1:9" ht="15.75">
       <c r="A112" s="17"/>
       <c r="B112" s="17" t="s">
         <v>21</v>
@@ -14326,7 +13981,7 @@
       </c>
       <c r="I112" s="17"/>
     </row>
-    <row r="113" spans="1:9" ht="15">
+    <row r="113" spans="1:9" ht="15.75">
       <c r="A113" s="17"/>
       <c r="B113" s="17" t="s">
         <v>21</v>
@@ -14349,7 +14004,7 @@
       </c>
       <c r="I113" s="17"/>
     </row>
-    <row r="114" spans="1:9" ht="15">
+    <row r="114" spans="1:9" ht="15.75">
       <c r="A114" s="17"/>
       <c r="B114" s="17" t="s">
         <v>21</v>
@@ -14372,7 +14027,7 @@
       </c>
       <c r="I114" s="17"/>
     </row>
-    <row r="115" spans="1:9" ht="15">
+    <row r="115" spans="1:9" ht="15.75">
       <c r="A115" s="17" t="b">
         <v>0</v>
       </c>
@@ -14391,7 +14046,7 @@
       <c r="H115" s="17"/>
       <c r="I115" s="17"/>
     </row>
-    <row r="116" spans="1:9" ht="15">
+    <row r="116" spans="1:9" ht="15.75">
       <c r="A116" s="17"/>
       <c r="B116" s="17" t="s">
         <v>21</v>
@@ -14414,7 +14069,7 @@
       </c>
       <c r="I116" s="17"/>
     </row>
-    <row r="117" spans="1:9" ht="15">
+    <row r="117" spans="1:9" ht="15.75">
       <c r="A117" s="17"/>
       <c r="B117" s="17" t="s">
         <v>21</v>
@@ -14437,7 +14092,7 @@
       </c>
       <c r="I117" s="17"/>
     </row>
-    <row r="118" spans="1:9" ht="15">
+    <row r="118" spans="1:9" ht="15.75">
       <c r="A118" s="17"/>
       <c r="B118" s="17" t="s">
         <v>21</v>
@@ -14460,7 +14115,7 @@
       </c>
       <c r="I118" s="17"/>
     </row>
-    <row r="119" spans="1:9" ht="15">
+    <row r="119" spans="1:9" ht="15.75">
       <c r="A119" s="17" t="b">
         <v>0</v>
       </c>
@@ -14479,7 +14134,7 @@
       <c r="H119" s="17"/>
       <c r="I119" s="17"/>
     </row>
-    <row r="120" spans="1:9" ht="15">
+    <row r="120" spans="1:9" ht="15.75">
       <c r="A120" s="17"/>
       <c r="B120" s="17" t="s">
         <v>21</v>
@@ -14502,7 +14157,7 @@
       </c>
       <c r="I120" s="17"/>
     </row>
-    <row r="121" spans="1:9" ht="15">
+    <row r="121" spans="1:9" ht="15.75">
       <c r="A121" s="17"/>
       <c r="B121" s="17" t="s">
         <v>21</v>
@@ -14525,7 +14180,7 @@
       </c>
       <c r="I121" s="17"/>
     </row>
-    <row r="122" spans="1:9" ht="15">
+    <row r="122" spans="1:9" ht="15.75">
       <c r="A122" s="17"/>
       <c r="B122" s="17" t="s">
         <v>21</v>
@@ -14548,7 +14203,7 @@
       </c>
       <c r="I122" s="17"/>
     </row>
-    <row r="123" spans="1:9" ht="15">
+    <row r="123" spans="1:9" ht="15.75">
       <c r="A123" s="17"/>
       <c r="B123" s="17" t="s">
         <v>21</v>
@@ -14571,7 +14226,7 @@
       </c>
       <c r="I123" s="17"/>
     </row>
-    <row r="124" spans="1:9" ht="15">
+    <row r="124" spans="1:9" ht="15.75">
       <c r="A124" s="17"/>
       <c r="B124" s="17" t="s">
         <v>21</v>
@@ -14594,7 +14249,7 @@
       </c>
       <c r="I124" s="17"/>
     </row>
-    <row r="125" spans="1:9" ht="15">
+    <row r="125" spans="1:9" ht="15.75">
       <c r="A125" s="17"/>
       <c r="B125" s="17" t="s">
         <v>21</v>
@@ -14617,7 +14272,7 @@
       </c>
       <c r="I125" s="17"/>
     </row>
-    <row r="126" spans="1:9" ht="15">
+    <row r="126" spans="1:9" ht="15.75">
       <c r="A126" s="17" t="b">
         <v>0</v>
       </c>
@@ -14636,7 +14291,7 @@
       <c r="H126" s="17"/>
       <c r="I126" s="17"/>
     </row>
-    <row r="127" spans="1:9" ht="15">
+    <row r="127" spans="1:9" ht="15.75">
       <c r="A127" s="17"/>
       <c r="B127" s="17" t="s">
         <v>21</v>
@@ -14661,7 +14316,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="15">
+    <row r="128" spans="1:9" ht="15.75">
       <c r="A128" s="17"/>
       <c r="B128" s="17" t="s">
         <v>21</v>
@@ -14684,7 +14339,7 @@
       </c>
       <c r="I128" s="17"/>
     </row>
-    <row r="129" spans="1:9" ht="15">
+    <row r="129" spans="1:9" ht="15.75">
       <c r="A129" s="17"/>
       <c r="B129" s="17" t="s">
         <v>21</v>
@@ -14707,7 +14362,7 @@
       </c>
       <c r="I129" s="17"/>
     </row>
-    <row r="130" spans="1:9" ht="15">
+    <row r="130" spans="1:9" ht="15.75">
       <c r="A130" s="17"/>
       <c r="B130" s="17" t="s">
         <v>21</v>
@@ -14730,7 +14385,7 @@
       </c>
       <c r="I130" s="17"/>
     </row>
-    <row r="131" spans="1:9" ht="15">
+    <row r="131" spans="1:9" ht="15.75">
       <c r="A131" s="17"/>
       <c r="B131" s="17" t="s">
         <v>21</v>
@@ -14753,7 +14408,7 @@
       </c>
       <c r="I131" s="17"/>
     </row>
-    <row r="132" spans="1:9" ht="15">
+    <row r="132" spans="1:9" ht="15.75">
       <c r="A132" s="17"/>
       <c r="B132" s="17" t="s">
         <v>21</v>
@@ -14776,7 +14431,7 @@
       </c>
       <c r="I132" s="17"/>
     </row>
-    <row r="133" spans="1:9" ht="15">
+    <row r="133" spans="1:9" ht="15.75">
       <c r="A133" s="17"/>
       <c r="B133" s="17" t="s">
         <v>21</v>
@@ -14799,7 +14454,7 @@
       </c>
       <c r="I133" s="17"/>
     </row>
-    <row r="134" spans="1:9" ht="15">
+    <row r="134" spans="1:9" ht="15.75">
       <c r="A134" s="17"/>
       <c r="B134" s="17" t="s">
         <v>21</v>
@@ -14822,7 +14477,7 @@
       </c>
       <c r="I134" s="17"/>
     </row>
-    <row r="135" spans="1:9" ht="15">
+    <row r="135" spans="1:9" ht="15.75">
       <c r="A135" s="17"/>
       <c r="B135" s="17" t="s">
         <v>21</v>
@@ -14845,7 +14500,7 @@
       </c>
       <c r="I135" s="17"/>
     </row>
-    <row r="136" spans="1:9" ht="15">
+    <row r="136" spans="1:9" ht="15.75">
       <c r="A136" s="17" t="b">
         <v>0</v>
       </c>
@@ -14864,7 +14519,7 @@
       <c r="H136" s="17"/>
       <c r="I136" s="17"/>
     </row>
-    <row r="137" spans="1:9" ht="15">
+    <row r="137" spans="1:9" ht="15.75">
       <c r="A137" s="17"/>
       <c r="B137" s="17" t="s">
         <v>21</v>
@@ -14889,7 +14544,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="15">
+    <row r="138" spans="1:9" ht="15.75">
       <c r="A138" s="17"/>
       <c r="B138" s="17" t="s">
         <v>21</v>
@@ -14910,7 +14565,7 @@
       <c r="H138" s="17"/>
       <c r="I138" s="17"/>
     </row>
-    <row r="139" spans="1:9" ht="15">
+    <row r="139" spans="1:9" ht="15.75">
       <c r="A139" s="17"/>
       <c r="B139" s="17" t="s">
         <v>21</v>
@@ -14933,7 +14588,7 @@
       </c>
       <c r="I139" s="17"/>
     </row>
-    <row r="140" spans="1:9" ht="15">
+    <row r="140" spans="1:9" ht="15.75">
       <c r="A140" s="17"/>
       <c r="B140" s="17" t="s">
         <v>21</v>
@@ -14956,7 +14611,7 @@
       </c>
       <c r="I140" s="17"/>
     </row>
-    <row r="141" spans="1:9" ht="15">
+    <row r="141" spans="1:9" ht="15.75">
       <c r="A141" s="17"/>
       <c r="B141" s="17" t="s">
         <v>21</v>
@@ -14979,7 +14634,7 @@
       </c>
       <c r="I141" s="17"/>
     </row>
-    <row r="142" spans="1:9" ht="15">
+    <row r="142" spans="1:9" ht="15.75">
       <c r="A142" s="17"/>
       <c r="B142" s="17" t="s">
         <v>21</v>
@@ -15002,7 +14657,7 @@
       </c>
       <c r="I142" s="17"/>
     </row>
-    <row r="143" spans="1:9" ht="15">
+    <row r="143" spans="1:9" ht="15.75">
       <c r="A143" s="17"/>
       <c r="B143" s="17" t="s">
         <v>21</v>
@@ -15025,7 +14680,7 @@
       </c>
       <c r="I143" s="17"/>
     </row>
-    <row r="144" spans="1:9" ht="15">
+    <row r="144" spans="1:9" ht="15.75">
       <c r="A144" s="17"/>
       <c r="B144" s="17" t="s">
         <v>21</v>
@@ -15048,7 +14703,7 @@
       </c>
       <c r="I144" s="17"/>
     </row>
-    <row r="145" spans="1:9" ht="15">
+    <row r="145" spans="1:9" ht="15.75">
       <c r="A145" s="17"/>
       <c r="B145" s="17" t="s">
         <v>21</v>
@@ -15071,7 +14726,7 @@
       </c>
       <c r="I145" s="17"/>
     </row>
-    <row r="146" spans="1:9" ht="15">
+    <row r="146" spans="1:9" ht="15.75">
       <c r="A146" s="17"/>
       <c r="B146" s="17" t="s">
         <v>21</v>
@@ -15094,7 +14749,7 @@
       </c>
       <c r="I146" s="17"/>
     </row>
-    <row r="147" spans="1:9" ht="15">
+    <row r="147" spans="1:9" ht="15.75">
       <c r="A147" s="17"/>
       <c r="B147" s="17" t="s">
         <v>21</v>
@@ -15117,7 +14772,7 @@
       </c>
       <c r="I147" s="17"/>
     </row>
-    <row r="148" spans="1:9" ht="15">
+    <row r="148" spans="1:9" ht="15.75">
       <c r="A148" s="17"/>
       <c r="B148" s="17" t="s">
         <v>21</v>
@@ -15140,7 +14795,7 @@
       </c>
       <c r="I148" s="17"/>
     </row>
-    <row r="149" spans="1:9" ht="15">
+    <row r="149" spans="1:9" ht="15.75">
       <c r="A149" s="17"/>
       <c r="B149" s="17" t="s">
         <v>21</v>
@@ -15163,7 +14818,7 @@
       </c>
       <c r="I149" s="17"/>
     </row>
-    <row r="150" spans="1:9" ht="15">
+    <row r="150" spans="1:9" ht="15.75">
       <c r="A150" s="17"/>
       <c r="B150" s="17" t="s">
         <v>21</v>
@@ -15186,7 +14841,7 @@
       </c>
       <c r="I150" s="17"/>
     </row>
-    <row r="151" spans="1:9" ht="15">
+    <row r="151" spans="1:9" ht="15.75">
       <c r="A151" s="17" t="b">
         <v>0</v>
       </c>
@@ -15205,7 +14860,7 @@
       <c r="H151" s="17"/>
       <c r="I151" s="17"/>
     </row>
-    <row r="152" spans="1:9" ht="15">
+    <row r="152" spans="1:9" ht="15.75">
       <c r="A152" s="17"/>
       <c r="B152" s="17" t="s">
         <v>21</v>
@@ -15228,7 +14883,7 @@
       </c>
       <c r="I152" s="17"/>
     </row>
-    <row r="153" spans="1:9" ht="15">
+    <row r="153" spans="1:9" ht="15.75">
       <c r="A153" s="17" t="b">
         <v>0</v>
       </c>
@@ -15247,7 +14902,7 @@
       <c r="H153" s="17"/>
       <c r="I153" s="17"/>
     </row>
-    <row r="154" spans="1:9" ht="15">
+    <row r="154" spans="1:9" ht="15.75">
       <c r="A154" s="17"/>
       <c r="B154" s="17" t="s">
         <v>21</v>
@@ -15270,7 +14925,7 @@
       </c>
       <c r="I154" s="17"/>
     </row>
-    <row r="155" spans="1:9" ht="15">
+    <row r="155" spans="1:9" ht="15.75">
       <c r="A155" s="17"/>
       <c r="B155" s="17" t="s">
         <v>21</v>
@@ -15293,7 +14948,7 @@
       </c>
       <c r="I155" s="17"/>
     </row>
-    <row r="156" spans="1:9" ht="15">
+    <row r="156" spans="1:9" ht="15.75">
       <c r="A156" s="17" t="b">
         <v>0</v>
       </c>
@@ -15312,7 +14967,7 @@
       <c r="H156" s="17"/>
       <c r="I156" s="17"/>
     </row>
-    <row r="157" spans="1:9" ht="15">
+    <row r="157" spans="1:9" ht="15.75">
       <c r="A157" s="17"/>
       <c r="B157" s="17" t="s">
         <v>21</v>
@@ -15337,7 +14992,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="158" spans="1:9" ht="15">
+    <row r="158" spans="1:9" ht="15.75">
       <c r="A158" s="17"/>
       <c r="B158" s="17" t="s">
         <v>21</v>
@@ -15360,7 +15015,7 @@
       </c>
       <c r="I158" s="17"/>
     </row>
-    <row r="159" spans="1:9" ht="15">
+    <row r="159" spans="1:9" ht="15.75">
       <c r="A159" s="17"/>
       <c r="B159" s="17" t="s">
         <v>21</v>
@@ -15383,7 +15038,7 @@
       </c>
       <c r="I159" s="17"/>
     </row>
-    <row r="160" spans="1:9" ht="15">
+    <row r="160" spans="1:9" ht="15.75">
       <c r="A160" s="17"/>
       <c r="B160" s="17" t="s">
         <v>21</v>
@@ -15406,7 +15061,7 @@
       </c>
       <c r="I160" s="17"/>
     </row>
-    <row r="161" spans="1:9" ht="15">
+    <row r="161" spans="1:9" ht="15.75">
       <c r="A161" s="17"/>
       <c r="B161" s="17" t="s">
         <v>21</v>
@@ -15429,7 +15084,7 @@
       </c>
       <c r="I161" s="17"/>
     </row>
-    <row r="162" spans="1:9" ht="15">
+    <row r="162" spans="1:9" ht="15.75">
       <c r="A162" s="17"/>
       <c r="B162" s="17" t="s">
         <v>21</v>
@@ -15452,7 +15107,7 @@
       </c>
       <c r="I162" s="17"/>
     </row>
-    <row r="163" spans="1:9" ht="15">
+    <row r="163" spans="1:9" ht="15.75">
       <c r="A163" s="17"/>
       <c r="B163" s="17" t="s">
         <v>21</v>
@@ -15475,7 +15130,7 @@
       </c>
       <c r="I163" s="17"/>
     </row>
-    <row r="164" spans="1:9" ht="15">
+    <row r="164" spans="1:9" ht="15.75">
       <c r="A164" s="17"/>
       <c r="B164" s="17" t="s">
         <v>21</v>
@@ -15498,7 +15153,7 @@
       </c>
       <c r="I164" s="17"/>
     </row>
-    <row r="165" spans="1:9" ht="15">
+    <row r="165" spans="1:9" ht="15.75">
       <c r="A165" s="17"/>
       <c r="B165" s="17" t="s">
         <v>21</v>
@@ -15521,7 +15176,7 @@
       </c>
       <c r="I165" s="17"/>
     </row>
-    <row r="166" spans="1:9" ht="15">
+    <row r="166" spans="1:9" ht="15.75">
       <c r="A166" s="17"/>
       <c r="B166" s="17" t="s">
         <v>21</v>
@@ -15544,7 +15199,7 @@
       </c>
       <c r="I166" s="17"/>
     </row>
-    <row r="167" spans="1:9" ht="15">
+    <row r="167" spans="1:9" ht="15.75">
       <c r="A167" s="17" t="b">
         <v>0</v>
       </c>
@@ -15563,7 +15218,7 @@
       <c r="H167" s="17"/>
       <c r="I167" s="17"/>
     </row>
-    <row r="168" spans="1:9" ht="15">
+    <row r="168" spans="1:9" ht="15.75">
       <c r="A168" s="17"/>
       <c r="B168" s="17" t="s">
         <v>21</v>
@@ -15588,7 +15243,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="169" spans="1:9" ht="15">
+    <row r="169" spans="1:9" ht="15.75">
       <c r="A169" s="17"/>
       <c r="B169" s="17" t="s">
         <v>21</v>
@@ -15611,7 +15266,7 @@
       </c>
       <c r="I169" s="17"/>
     </row>
-    <row r="170" spans="1:9" ht="15">
+    <row r="170" spans="1:9" ht="15.75">
       <c r="A170" s="17"/>
       <c r="B170" s="17" t="s">
         <v>21</v>
@@ -15634,7 +15289,7 @@
       </c>
       <c r="I170" s="17"/>
     </row>
-    <row r="171" spans="1:9" ht="15">
+    <row r="171" spans="1:9" ht="15.75">
       <c r="A171" s="17"/>
       <c r="B171" s="17" t="s">
         <v>21</v>
@@ -15657,7 +15312,7 @@
       </c>
       <c r="I171" s="17"/>
     </row>
-    <row r="172" spans="1:9" ht="15">
+    <row r="172" spans="1:9" ht="15.75">
       <c r="A172" s="17"/>
       <c r="B172" s="17" t="s">
         <v>21</v>
@@ -15680,7 +15335,7 @@
       </c>
       <c r="I172" s="17"/>
     </row>
-    <row r="173" spans="1:9" ht="15">
+    <row r="173" spans="1:9" ht="15.75">
       <c r="A173" s="17"/>
       <c r="B173" s="17" t="s">
         <v>21</v>
@@ -15703,7 +15358,7 @@
       </c>
       <c r="I173" s="17"/>
     </row>
-    <row r="174" spans="1:9" ht="15">
+    <row r="174" spans="1:9" ht="15.75">
       <c r="A174" s="17"/>
       <c r="B174" s="17" t="s">
         <v>21</v>
@@ -15726,7 +15381,7 @@
       </c>
       <c r="I174" s="17"/>
     </row>
-    <row r="175" spans="1:9" ht="15">
+    <row r="175" spans="1:9" ht="15.75">
       <c r="A175" s="17"/>
       <c r="B175" s="17" t="s">
         <v>21</v>
@@ -15749,7 +15404,7 @@
       </c>
       <c r="I175" s="17"/>
     </row>
-    <row r="176" spans="1:9" ht="15">
+    <row r="176" spans="1:9" ht="15.75">
       <c r="A176" s="17"/>
       <c r="B176" s="17" t="s">
         <v>21</v>
@@ -15772,7 +15427,7 @@
       </c>
       <c r="I176" s="17"/>
     </row>
-    <row r="177" spans="1:9" ht="15">
+    <row r="177" spans="1:9" ht="15.75">
       <c r="A177" s="17"/>
       <c r="B177" s="17" t="s">
         <v>21</v>
@@ -15795,7 +15450,7 @@
       </c>
       <c r="I177" s="17"/>
     </row>
-    <row r="178" spans="1:9" ht="15">
+    <row r="178" spans="1:9" ht="15.75">
       <c r="A178" s="17" t="b">
         <v>0</v>
       </c>
@@ -15814,7 +15469,7 @@
       <c r="H178" s="17"/>
       <c r="I178" s="17"/>
     </row>
-    <row r="179" spans="1:9" ht="15">
+    <row r="179" spans="1:9" ht="15.75">
       <c r="A179" s="17"/>
       <c r="B179" s="17" t="s">
         <v>21</v>
@@ -15837,7 +15492,7 @@
       </c>
       <c r="I179" s="17"/>
     </row>
-    <row r="180" spans="1:9" ht="15">
+    <row r="180" spans="1:9" ht="15.75">
       <c r="A180" s="17"/>
       <c r="B180" s="17" t="s">
         <v>21</v>
@@ -15860,7 +15515,7 @@
       </c>
       <c r="I180" s="17"/>
     </row>
-    <row r="181" spans="1:9" ht="15">
+    <row r="181" spans="1:9" ht="15.75">
       <c r="A181" s="17"/>
       <c r="B181" s="17" t="s">
         <v>21</v>
@@ -15883,7 +15538,7 @@
       </c>
       <c r="I181" s="17"/>
     </row>
-    <row r="182" spans="1:9" ht="15">
+    <row r="182" spans="1:9" ht="15.75">
       <c r="A182" s="17"/>
       <c r="B182" s="17" t="s">
         <v>21</v>
@@ -15906,7 +15561,7 @@
       </c>
       <c r="I182" s="17"/>
     </row>
-    <row r="183" spans="1:9" ht="15">
+    <row r="183" spans="1:9" ht="15.75">
       <c r="A183" s="17" t="b">
         <v>0</v>
       </c>
@@ -15925,7 +15580,7 @@
       <c r="H183" s="17"/>
       <c r="I183" s="17"/>
     </row>
-    <row r="184" spans="1:9" ht="15">
+    <row r="184" spans="1:9" ht="15.75">
       <c r="A184" s="17"/>
       <c r="B184" s="17" t="s">
         <v>21</v>
@@ -15948,7 +15603,7 @@
       </c>
       <c r="I184" s="17"/>
     </row>
-    <row r="185" spans="1:9" ht="15">
+    <row r="185" spans="1:9" ht="15.75">
       <c r="A185" s="17"/>
       <c r="B185" s="17" t="s">
         <v>21</v>
@@ -15971,7 +15626,7 @@
       </c>
       <c r="I185" s="17"/>
     </row>
-    <row r="186" spans="1:9" ht="15">
+    <row r="186" spans="1:9" ht="15.75">
       <c r="A186" s="17"/>
       <c r="B186" s="17" t="s">
         <v>21</v>
@@ -15994,7 +15649,7 @@
       </c>
       <c r="I186" s="17"/>
     </row>
-    <row r="187" spans="1:9" ht="15">
+    <row r="187" spans="1:9" ht="15.75">
       <c r="A187" s="17"/>
       <c r="B187" s="17" t="s">
         <v>21</v>
@@ -16017,7 +15672,7 @@
       </c>
       <c r="I187" s="17"/>
     </row>
-    <row r="188" spans="1:9" ht="15">
+    <row r="188" spans="1:9" ht="15.75">
       <c r="A188" s="17" t="b">
         <v>0</v>
       </c>
@@ -16036,7 +15691,7 @@
       <c r="H188" s="17"/>
       <c r="I188" s="17"/>
     </row>
-    <row r="189" spans="1:9" ht="15">
+    <row r="189" spans="1:9" ht="15.75">
       <c r="A189" s="17"/>
       <c r="B189" s="17" t="s">
         <v>21</v>
@@ -16057,7 +15712,7 @@
       <c r="H189" s="17"/>
       <c r="I189" s="17"/>
     </row>
-    <row r="190" spans="1:9" ht="15">
+    <row r="190" spans="1:9" ht="15.75">
       <c r="A190" s="17"/>
       <c r="B190" s="17" t="s">
         <v>21</v>
@@ -16080,7 +15735,7 @@
       </c>
       <c r="I190" s="17"/>
     </row>
-    <row r="191" spans="1:9" ht="15">
+    <row r="191" spans="1:9" ht="15.75">
       <c r="A191" s="17" t="b">
         <v>0</v>
       </c>
@@ -16099,7 +15754,7 @@
       <c r="H191" s="17"/>
       <c r="I191" s="17"/>
     </row>
-    <row r="192" spans="1:9" ht="15">
+    <row r="192" spans="1:9" ht="15.75">
       <c r="A192" s="17"/>
       <c r="B192" s="17" t="s">
         <v>21</v>
@@ -16122,7 +15777,7 @@
       </c>
       <c r="I192" s="17"/>
     </row>
-    <row r="193" spans="1:9" ht="15">
+    <row r="193" spans="1:9" ht="15.75">
       <c r="A193" s="17"/>
       <c r="B193" s="17" t="s">
         <v>21</v>
@@ -16147,7 +15802,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="194" spans="1:9" ht="15">
+    <row r="194" spans="1:9" ht="15.75">
       <c r="A194" s="17"/>
       <c r="B194" s="17" t="s">
         <v>21</v>
@@ -16168,7 +15823,7 @@
       <c r="H194" s="17"/>
       <c r="I194" s="17"/>
     </row>
-    <row r="195" spans="1:9" ht="15">
+    <row r="195" spans="1:9" ht="15.75">
       <c r="A195" s="17"/>
       <c r="B195" s="17" t="s">
         <v>21</v>
@@ -16193,7 +15848,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="196" spans="1:9" ht="15">
+    <row r="196" spans="1:9" ht="15.75">
       <c r="A196" s="17"/>
       <c r="B196" s="17" t="s">
         <v>21</v>
@@ -16218,7 +15873,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="197" spans="1:9" ht="15">
+    <row r="197" spans="1:9" ht="15.75">
       <c r="A197" s="17" t="b">
         <v>0</v>
       </c>
@@ -16237,7 +15892,7 @@
       <c r="H197" s="17"/>
       <c r="I197" s="17"/>
     </row>
-    <row r="198" spans="1:9" ht="15">
+    <row r="198" spans="1:9" ht="15.75">
       <c r="A198" s="17"/>
       <c r="B198" s="17" t="s">
         <v>21</v>
@@ -16262,7 +15917,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="199" spans="1:9" ht="15">
+    <row r="199" spans="1:9" ht="15.75">
       <c r="A199" s="17"/>
       <c r="B199" s="17" t="s">
         <v>21</v>
@@ -16285,7 +15940,7 @@
       </c>
       <c r="I199" s="17"/>
     </row>
-    <row r="200" spans="1:9" ht="15">
+    <row r="200" spans="1:9" ht="15.75">
       <c r="A200" s="17"/>
       <c r="B200" s="17" t="s">
         <v>21</v>
@@ -16308,7 +15963,7 @@
       </c>
       <c r="I200" s="17"/>
     </row>
-    <row r="201" spans="1:9" ht="15">
+    <row r="201" spans="1:9" ht="15.75">
       <c r="A201" s="17"/>
       <c r="B201" s="17" t="s">
         <v>21</v>
@@ -16331,7 +15986,7 @@
       </c>
       <c r="I201" s="17"/>
     </row>
-    <row r="202" spans="1:9" ht="15">
+    <row r="202" spans="1:9" ht="15.75">
       <c r="A202" s="17"/>
       <c r="B202" s="17" t="s">
         <v>21</v>
@@ -16354,7 +16009,7 @@
       </c>
       <c r="I202" s="17"/>
     </row>
-    <row r="203" spans="1:9" ht="15">
+    <row r="203" spans="1:9" ht="15.75">
       <c r="A203" s="17"/>
       <c r="B203" s="17" t="s">
         <v>21</v>
@@ -16377,7 +16032,7 @@
       </c>
       <c r="I203" s="17"/>
     </row>
-    <row r="204" spans="1:9" ht="15">
+    <row r="204" spans="1:9" ht="15.75">
       <c r="A204" s="17"/>
       <c r="B204" s="17" t="s">
         <v>21</v>
@@ -16400,7 +16055,7 @@
       </c>
       <c r="I204" s="17"/>
     </row>
-    <row r="205" spans="1:9" ht="15">
+    <row r="205" spans="1:9" ht="15.75">
       <c r="A205" s="17"/>
       <c r="B205" s="17" t="s">
         <v>21</v>
@@ -16423,7 +16078,7 @@
       </c>
       <c r="I205" s="17"/>
     </row>
-    <row r="206" spans="1:9" ht="15">
+    <row r="206" spans="1:9" ht="15.75">
       <c r="A206" s="17"/>
       <c r="B206" s="17" t="s">
         <v>21</v>
@@ -16446,7 +16101,7 @@
       </c>
       <c r="I206" s="17"/>
     </row>
-    <row r="207" spans="1:9" ht="15">
+    <row r="207" spans="1:9" ht="15.75">
       <c r="A207" s="17" t="b">
         <v>0</v>
       </c>
@@ -16465,7 +16120,7 @@
       <c r="H207" s="17"/>
       <c r="I207" s="17"/>
     </row>
-    <row r="208" spans="1:9" ht="15">
+    <row r="208" spans="1:9" ht="15.75">
       <c r="A208" s="17"/>
       <c r="B208" s="17" t="s">
         <v>21</v>
@@ -16490,7 +16145,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="209" spans="1:9" ht="15">
+    <row r="209" spans="1:9" ht="15.75">
       <c r="A209" s="17"/>
       <c r="B209" s="17" t="s">
         <v>21</v>
@@ -16513,7 +16168,7 @@
       </c>
       <c r="I209" s="17"/>
     </row>
-    <row r="210" spans="1:9" ht="15">
+    <row r="210" spans="1:9" ht="15.75">
       <c r="A210" s="17"/>
       <c r="B210" s="17" t="s">
         <v>21</v>
@@ -16536,7 +16191,7 @@
       </c>
       <c r="I210" s="17"/>
     </row>
-    <row r="211" spans="1:9" ht="15">
+    <row r="211" spans="1:9" ht="15.75">
       <c r="A211" s="17"/>
       <c r="B211" s="17" t="s">
         <v>21</v>
@@ -16559,7 +16214,7 @@
       </c>
       <c r="I211" s="17"/>
     </row>
-    <row r="212" spans="1:9" ht="15">
+    <row r="212" spans="1:9" ht="15.75">
       <c r="A212" s="17"/>
       <c r="B212" s="17" t="s">
         <v>21</v>
@@ -16582,7 +16237,7 @@
       </c>
       <c r="I212" s="17"/>
     </row>
-    <row r="213" spans="1:9" ht="15">
+    <row r="213" spans="1:9" ht="15.75">
       <c r="A213" s="17"/>
       <c r="B213" s="17" t="s">
         <v>21</v>
@@ -16605,7 +16260,7 @@
       </c>
       <c r="I213" s="17"/>
     </row>
-    <row r="214" spans="1:9" ht="15">
+    <row r="214" spans="1:9" ht="15.75">
       <c r="A214" s="17"/>
       <c r="B214" s="17" t="s">
         <v>21</v>
@@ -16628,7 +16283,7 @@
       </c>
       <c r="I214" s="17"/>
     </row>
-    <row r="215" spans="1:9" ht="15">
+    <row r="215" spans="1:9" ht="15.75">
       <c r="A215" s="17"/>
       <c r="B215" s="17" t="s">
         <v>21</v>
@@ -16651,7 +16306,7 @@
       </c>
       <c r="I215" s="17"/>
     </row>
-    <row r="216" spans="1:9" ht="15">
+    <row r="216" spans="1:9" ht="15.75">
       <c r="A216" s="17"/>
       <c r="B216" s="17" t="s">
         <v>21</v>
@@ -16674,7 +16329,7 @@
       </c>
       <c r="I216" s="17"/>
     </row>
-    <row r="217" spans="1:9" ht="15">
+    <row r="217" spans="1:9" ht="15.75">
       <c r="A217" s="17" t="b">
         <v>0</v>
       </c>
@@ -16693,7 +16348,7 @@
       <c r="H217" s="17"/>
       <c r="I217" s="17"/>
     </row>
-    <row r="218" spans="1:9" ht="15">
+    <row r="218" spans="1:9" ht="15.75">
       <c r="A218" s="17"/>
       <c r="B218" s="17" t="s">
         <v>21</v>
@@ -16714,7 +16369,7 @@
       <c r="H218" s="17"/>
       <c r="I218" s="17"/>
     </row>
-    <row r="219" spans="1:9" ht="15">
+    <row r="219" spans="1:9" ht="15.75">
       <c r="A219" s="17"/>
       <c r="B219" s="17" t="s">
         <v>21</v>
@@ -16737,7 +16392,7 @@
       </c>
       <c r="I219" s="17"/>
     </row>
-    <row r="220" spans="1:9" ht="15">
+    <row r="220" spans="1:9" ht="15.75">
       <c r="A220" s="17"/>
       <c r="B220" s="17" t="s">
         <v>21</v>
@@ -16760,7 +16415,7 @@
       </c>
       <c r="I220" s="17"/>
     </row>
-    <row r="221" spans="1:9" ht="15">
+    <row r="221" spans="1:9" ht="15.75">
       <c r="A221" s="17"/>
       <c r="B221" s="17" t="s">
         <v>21</v>
@@ -16783,7 +16438,7 @@
       </c>
       <c r="I221" s="17"/>
     </row>
-    <row r="222" spans="1:9" ht="15">
+    <row r="222" spans="1:9" ht="15.75">
       <c r="A222" s="17"/>
       <c r="B222" s="17" t="s">
         <v>21</v>
@@ -16806,7 +16461,7 @@
       </c>
       <c r="I222" s="17"/>
     </row>
-    <row r="223" spans="1:9" ht="15">
+    <row r="223" spans="1:9" ht="15.75">
       <c r="A223" s="17"/>
       <c r="B223" s="17" t="s">
         <v>21</v>
@@ -16829,7 +16484,7 @@
       </c>
       <c r="I223" s="17"/>
     </row>
-    <row r="224" spans="1:9" ht="15">
+    <row r="224" spans="1:9" ht="15.75">
       <c r="A224" s="17"/>
       <c r="B224" s="17" t="s">
         <v>21</v>
@@ -16852,7 +16507,7 @@
       </c>
       <c r="I224" s="17"/>
     </row>
-    <row r="225" spans="1:9" ht="15">
+    <row r="225" spans="1:9" ht="15.75">
       <c r="A225" s="17"/>
       <c r="B225" s="17" t="s">
         <v>21</v>
@@ -16875,7 +16530,7 @@
       </c>
       <c r="I225" s="17"/>
     </row>
-    <row r="226" spans="1:9" ht="15">
+    <row r="226" spans="1:9" ht="15.75">
       <c r="A226" s="17"/>
       <c r="B226" s="17" t="s">
         <v>21</v>
@@ -16898,7 +16553,7 @@
       </c>
       <c r="I226" s="17"/>
     </row>
-    <row r="227" spans="1:9" ht="15">
+    <row r="227" spans="1:9" ht="15.75">
       <c r="A227" s="17"/>
       <c r="B227" s="17" t="s">
         <v>21</v>
@@ -16921,7 +16576,7 @@
       </c>
       <c r="I227" s="17"/>
     </row>
-    <row r="228" spans="1:9" ht="15">
+    <row r="228" spans="1:9" ht="15.75">
       <c r="A228" s="17"/>
       <c r="B228" s="17" t="s">
         <v>21</v>
@@ -16944,7 +16599,7 @@
       </c>
       <c r="I228" s="17"/>
     </row>
-    <row r="229" spans="1:9" ht="15">
+    <row r="229" spans="1:9" ht="15.75">
       <c r="A229" s="17"/>
       <c r="B229" s="17" t="s">
         <v>21</v>
@@ -16967,7 +16622,7 @@
       </c>
       <c r="I229" s="17"/>
     </row>
-    <row r="230" spans="1:9" ht="15">
+    <row r="230" spans="1:9" ht="15.75">
       <c r="A230" s="17"/>
       <c r="B230" s="17" t="s">
         <v>21</v>
@@ -16990,7 +16645,7 @@
       </c>
       <c r="I230" s="17"/>
     </row>
-    <row r="231" spans="1:9" ht="15">
+    <row r="231" spans="1:9" ht="15.75">
       <c r="A231" s="17"/>
       <c r="B231" s="17" t="s">
         <v>21</v>
@@ -17013,7 +16668,7 @@
       </c>
       <c r="I231" s="17"/>
     </row>
-    <row r="232" spans="1:9" ht="15">
+    <row r="232" spans="1:9" ht="15.75">
       <c r="A232" s="17"/>
       <c r="B232" s="17" t="s">
         <v>21</v>
@@ -17036,7 +16691,7 @@
       </c>
       <c r="I232" s="17"/>
     </row>
-    <row r="233" spans="1:9" ht="15">
+    <row r="233" spans="1:9" ht="15.75">
       <c r="A233" s="17"/>
       <c r="B233" s="17" t="s">
         <v>21</v>
@@ -17059,7 +16714,7 @@
       </c>
       <c r="I233" s="17"/>
     </row>
-    <row r="234" spans="1:9" ht="15">
+    <row r="234" spans="1:9" ht="15.75">
       <c r="A234" s="17" t="b">
         <v>0</v>
       </c>
@@ -17078,7 +16733,7 @@
       <c r="H234" s="17"/>
       <c r="I234" s="17"/>
     </row>
-    <row r="235" spans="1:9" ht="15">
+    <row r="235" spans="1:9" ht="15.75">
       <c r="A235" s="17"/>
       <c r="B235" s="17" t="s">
         <v>21</v>
@@ -17099,7 +16754,7 @@
       <c r="H235" s="17"/>
       <c r="I235" s="17"/>
     </row>
-    <row r="236" spans="1:9" ht="15">
+    <row r="236" spans="1:9" ht="15.75">
       <c r="A236" s="17"/>
       <c r="B236" s="17" t="s">
         <v>21</v>
@@ -17122,7 +16777,7 @@
       </c>
       <c r="I236" s="17"/>
     </row>
-    <row r="237" spans="1:9" ht="15">
+    <row r="237" spans="1:9" ht="15.75">
       <c r="A237" s="17"/>
       <c r="B237" s="17" t="s">
         <v>21</v>
@@ -17145,7 +16800,7 @@
       </c>
       <c r="I237" s="17"/>
     </row>
-    <row r="238" spans="1:9" ht="15">
+    <row r="238" spans="1:9" ht="15.75">
       <c r="A238" s="17"/>
       <c r="B238" s="17" t="s">
         <v>21</v>
@@ -17168,7 +16823,7 @@
       </c>
       <c r="I238" s="17"/>
     </row>
-    <row r="239" spans="1:9" ht="15">
+    <row r="239" spans="1:9" ht="15.75">
       <c r="A239" s="17"/>
       <c r="B239" s="17" t="s">
         <v>21</v>
@@ -17191,7 +16846,7 @@
       </c>
       <c r="I239" s="17"/>
     </row>
-    <row r="240" spans="1:9" ht="15">
+    <row r="240" spans="1:9" ht="15.75">
       <c r="A240" s="17"/>
       <c r="B240" s="17" t="s">
         <v>21</v>
@@ -17214,7 +16869,7 @@
       </c>
       <c r="I240" s="17"/>
     </row>
-    <row r="241" spans="1:9" ht="15">
+    <row r="241" spans="1:9" ht="15.75">
       <c r="A241" s="17"/>
       <c r="B241" s="17" t="s">
         <v>21</v>
@@ -17237,7 +16892,7 @@
       </c>
       <c r="I241" s="17"/>
     </row>
-    <row r="242" spans="1:9" ht="15">
+    <row r="242" spans="1:9" ht="15.75">
       <c r="A242" s="17"/>
       <c r="B242" s="17" t="s">
         <v>21</v>
@@ -17260,7 +16915,7 @@
       </c>
       <c r="I242" s="17"/>
     </row>
-    <row r="243" spans="1:9" ht="15">
+    <row r="243" spans="1:9" ht="15.75">
       <c r="A243" s="17"/>
       <c r="B243" s="17" t="s">
         <v>21</v>
@@ -17283,7 +16938,7 @@
       </c>
       <c r="I243" s="17"/>
     </row>
-    <row r="244" spans="1:9" ht="15">
+    <row r="244" spans="1:9" ht="15.75">
       <c r="A244" s="17"/>
       <c r="B244" s="17" t="s">
         <v>21</v>
@@ -17306,7 +16961,7 @@
       </c>
       <c r="I244" s="17"/>
     </row>
-    <row r="245" spans="1:9" ht="15">
+    <row r="245" spans="1:9" ht="15.75">
       <c r="A245" s="17"/>
       <c r="B245" s="17" t="s">
         <v>21</v>
@@ -17329,7 +16984,7 @@
       </c>
       <c r="I245" s="17"/>
     </row>
-    <row r="246" spans="1:9" ht="15">
+    <row r="246" spans="1:9" ht="15.75">
       <c r="A246" s="17"/>
       <c r="B246" s="17" t="s">
         <v>21</v>
@@ -17352,7 +17007,7 @@
       </c>
       <c r="I246" s="17"/>
     </row>
-    <row r="247" spans="1:9" ht="15">
+    <row r="247" spans="1:9" ht="15.75">
       <c r="A247" s="17"/>
       <c r="B247" s="17" t="s">
         <v>21</v>
@@ -17375,7 +17030,7 @@
       </c>
       <c r="I247" s="17"/>
     </row>
-    <row r="248" spans="1:9" ht="15">
+    <row r="248" spans="1:9" ht="15.75">
       <c r="A248" s="17"/>
       <c r="B248" s="17" t="s">
         <v>21</v>
@@ -17398,7 +17053,7 @@
       </c>
       <c r="I248" s="17"/>
     </row>
-    <row r="249" spans="1:9" ht="15">
+    <row r="249" spans="1:9" ht="15.75">
       <c r="A249" s="17"/>
       <c r="B249" s="17" t="s">
         <v>21</v>
@@ -17421,7 +17076,7 @@
       </c>
       <c r="I249" s="17"/>
     </row>
-    <row r="250" spans="1:9" ht="15">
+    <row r="250" spans="1:9" ht="15.75">
       <c r="A250" s="17"/>
       <c r="B250" s="17" t="s">
         <v>21</v>
@@ -17444,7 +17099,7 @@
       </c>
       <c r="I250" s="17"/>
     </row>
-    <row r="251" spans="1:9" ht="15">
+    <row r="251" spans="1:9" ht="15.75">
       <c r="A251" s="17" t="b">
         <v>0</v>
       </c>
@@ -17463,7 +17118,7 @@
       <c r="H251" s="17"/>
       <c r="I251" s="17"/>
     </row>
-    <row r="252" spans="1:9" ht="15">
+    <row r="252" spans="1:9" ht="15.75">
       <c r="A252" s="17"/>
       <c r="B252" s="17" t="s">
         <v>21</v>
@@ -17488,7 +17143,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="253" spans="1:9" ht="15">
+    <row r="253" spans="1:9" ht="15.75">
       <c r="A253" s="17"/>
       <c r="B253" s="17" t="s">
         <v>21</v>
@@ -17511,7 +17166,7 @@
       </c>
       <c r="I253" s="17"/>
     </row>
-    <row r="254" spans="1:9" ht="15">
+    <row r="254" spans="1:9" ht="15.75">
       <c r="A254" s="17"/>
       <c r="B254" s="17" t="s">
         <v>21</v>
@@ -17534,7 +17189,7 @@
       </c>
       <c r="I254" s="17"/>
     </row>
-    <row r="255" spans="1:9" ht="15">
+    <row r="255" spans="1:9" ht="15.75">
       <c r="A255" s="17"/>
       <c r="B255" s="17" t="s">
         <v>21</v>
@@ -17557,7 +17212,7 @@
       </c>
       <c r="I255" s="17"/>
     </row>
-    <row r="256" spans="1:9" ht="15">
+    <row r="256" spans="1:9" ht="15.75">
       <c r="A256" s="17"/>
       <c r="B256" s="17" t="s">
         <v>21</v>
@@ -17580,7 +17235,7 @@
       </c>
       <c r="I256" s="17"/>
     </row>
-    <row r="257" spans="1:9" ht="15">
+    <row r="257" spans="1:9" ht="15.75">
       <c r="A257" s="17" t="b">
         <v>0</v>
       </c>
@@ -17599,7 +17254,7 @@
       <c r="H257" s="17"/>
       <c r="I257" s="17"/>
     </row>
-    <row r="258" spans="1:9" ht="15">
+    <row r="258" spans="1:9" ht="15.75">
       <c r="A258" s="17"/>
       <c r="B258" s="17" t="s">
         <v>21</v>
@@ -17624,7 +17279,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="259" spans="1:9" ht="15">
+    <row r="259" spans="1:9" ht="15.75">
       <c r="A259" s="17"/>
       <c r="B259" s="17" t="s">
         <v>21</v>
@@ -17647,7 +17302,7 @@
       </c>
       <c r="I259" s="17"/>
     </row>
-    <row r="260" spans="1:9" ht="15">
+    <row r="260" spans="1:9" ht="15.75">
       <c r="A260" s="17" t="b">
         <v>0</v>
       </c>
@@ -17666,7 +17321,7 @@
       <c r="H260" s="17"/>
       <c r="I260" s="17"/>
     </row>
-    <row r="261" spans="1:9" ht="15">
+    <row r="261" spans="1:9" ht="15.75">
       <c r="A261" s="17" t="b">
         <v>0</v>
       </c>
@@ -17685,7 +17340,7 @@
       <c r="H261" s="17"/>
       <c r="I261" s="17"/>
     </row>
-    <row r="262" spans="1:9" ht="15">
+    <row r="262" spans="1:9" ht="15.75">
       <c r="A262" s="17" t="b">
         <v>0</v>
       </c>
@@ -17704,7 +17359,7 @@
       <c r="H262" s="17"/>
       <c r="I262" s="17"/>
     </row>
-    <row r="263" spans="1:9" ht="15">
+    <row r="263" spans="1:9" ht="15.75">
       <c r="A263" s="17"/>
       <c r="B263" s="17" t="s">
         <v>21</v>
@@ -17725,7 +17380,7 @@
       <c r="H263" s="17"/>
       <c r="I263" s="17"/>
     </row>
-    <row r="264" spans="1:9" ht="15">
+    <row r="264" spans="1:9" ht="15.75">
       <c r="A264" s="17"/>
       <c r="B264" s="17" t="s">
         <v>21</v>
@@ -17748,7 +17403,7 @@
       </c>
       <c r="I264" s="17"/>
     </row>
-    <row r="265" spans="1:9" ht="15">
+    <row r="265" spans="1:9" ht="15.75">
       <c r="A265" s="17"/>
       <c r="B265" s="17" t="s">
         <v>21</v>
@@ -17771,7 +17426,7 @@
       </c>
       <c r="I265" s="17"/>
     </row>
-    <row r="266" spans="1:9" ht="15">
+    <row r="266" spans="1:9" ht="15.75">
       <c r="A266" s="17"/>
       <c r="B266" s="17" t="s">
         <v>21</v>
@@ -17794,7 +17449,7 @@
       </c>
       <c r="I266" s="17"/>
     </row>
-    <row r="267" spans="1:9" ht="15">
+    <row r="267" spans="1:9" ht="15.75">
       <c r="A267" s="17"/>
       <c r="B267" s="17" t="s">
         <v>21</v>
@@ -17817,7 +17472,7 @@
       </c>
       <c r="I267" s="17"/>
     </row>
-    <row r="268" spans="1:9" ht="15">
+    <row r="268" spans="1:9" ht="15.75">
       <c r="A268" s="17"/>
       <c r="B268" s="17" t="s">
         <v>21</v>
@@ -17840,7 +17495,7 @@
       </c>
       <c r="I268" s="17"/>
     </row>
-    <row r="269" spans="1:9" ht="15">
+    <row r="269" spans="1:9" ht="15.75">
       <c r="A269" s="17"/>
       <c r="B269" s="17" t="s">
         <v>21</v>
@@ -17863,7 +17518,7 @@
       </c>
       <c r="I269" s="17"/>
     </row>
-    <row r="270" spans="1:9" ht="15">
+    <row r="270" spans="1:9" ht="15.75">
       <c r="A270" s="17"/>
       <c r="B270" s="17" t="s">
         <v>21</v>
@@ -17886,7 +17541,7 @@
       </c>
       <c r="I270" s="17"/>
     </row>
-    <row r="271" spans="1:9" ht="15">
+    <row r="271" spans="1:9" ht="15.75">
       <c r="A271" s="17"/>
       <c r="B271" s="17" t="s">
         <v>21</v>
@@ -17909,7 +17564,7 @@
       </c>
       <c r="I271" s="17"/>
     </row>
-    <row r="272" spans="1:9" ht="15">
+    <row r="272" spans="1:9" ht="15.75">
       <c r="A272" s="17"/>
       <c r="B272" s="17" t="s">
         <v>21</v>
@@ -17932,7 +17587,7 @@
       </c>
       <c r="I272" s="17"/>
     </row>
-    <row r="273" spans="1:9" ht="15">
+    <row r="273" spans="1:9" ht="15.75">
       <c r="A273" s="17"/>
       <c r="B273" s="17" t="s">
         <v>21</v>
@@ -17955,7 +17610,7 @@
       </c>
       <c r="I273" s="17"/>
     </row>
-    <row r="274" spans="1:9" ht="15">
+    <row r="274" spans="1:9" ht="15.75">
       <c r="A274" s="17" t="b">
         <v>0</v>
       </c>
@@ -17974,7 +17629,7 @@
       <c r="H274" s="17"/>
       <c r="I274" s="17"/>
     </row>
-    <row r="275" spans="1:9" ht="15">
+    <row r="275" spans="1:9" ht="15.75">
       <c r="A275" s="17"/>
       <c r="B275" s="17" t="s">
         <v>21</v>
@@ -17997,7 +17652,7 @@
       </c>
       <c r="I275" s="17"/>
     </row>
-    <row r="276" spans="1:9" ht="15">
+    <row r="276" spans="1:9" ht="15.75">
       <c r="A276" s="17" t="b">
         <v>0</v>
       </c>
@@ -18016,7 +17671,7 @@
       <c r="H276" s="17"/>
       <c r="I276" s="17"/>
     </row>
-    <row r="277" spans="1:9" ht="15">
+    <row r="277" spans="1:9" ht="15.75">
       <c r="A277" s="17"/>
       <c r="B277" s="17" t="s">
         <v>21</v>
@@ -18041,7 +17696,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="278" spans="1:9" ht="15">
+    <row r="278" spans="1:9" ht="15.75">
       <c r="A278" s="17"/>
       <c r="B278" s="17" t="s">
         <v>21</v>
@@ -18064,7 +17719,7 @@
       </c>
       <c r="I278" s="17"/>
     </row>
-    <row r="279" spans="1:9" ht="15">
+    <row r="279" spans="1:9" ht="15.75">
       <c r="A279" s="17"/>
       <c r="B279" s="17" t="s">
         <v>21</v>
@@ -18087,7 +17742,7 @@
       </c>
       <c r="I279" s="17"/>
     </row>
-    <row r="280" spans="1:9" ht="15">
+    <row r="280" spans="1:9" ht="15.75">
       <c r="A280" s="17"/>
       <c r="B280" s="17" t="s">
         <v>21</v>
@@ -18110,7 +17765,7 @@
       </c>
       <c r="I280" s="17"/>
     </row>
-    <row r="281" spans="1:9" ht="15">
+    <row r="281" spans="1:9" ht="15.75">
       <c r="A281" s="17"/>
       <c r="B281" s="17" t="s">
         <v>21</v>
@@ -18133,7 +17788,7 @@
       </c>
       <c r="I281" s="17"/>
     </row>
-    <row r="282" spans="1:9" ht="15">
+    <row r="282" spans="1:9" ht="15.75">
       <c r="A282" s="17"/>
       <c r="B282" s="17" t="s">
         <v>21</v>
@@ -18156,7 +17811,7 @@
       </c>
       <c r="I282" s="17"/>
     </row>
-    <row r="283" spans="1:9" ht="15">
+    <row r="283" spans="1:9" ht="15.75">
       <c r="A283" s="17"/>
       <c r="B283" s="17" t="s">
         <v>21</v>
@@ -18179,7 +17834,7 @@
       </c>
       <c r="I283" s="17"/>
     </row>
-    <row r="284" spans="1:9" ht="15">
+    <row r="284" spans="1:9" ht="15.75">
       <c r="A284" s="17"/>
       <c r="B284" s="17" t="s">
         <v>21</v>
@@ -18202,7 +17857,7 @@
       </c>
       <c r="I284" s="17"/>
     </row>
-    <row r="285" spans="1:9" ht="15">
+    <row r="285" spans="1:9" ht="15.75">
       <c r="A285" s="17"/>
       <c r="B285" s="17" t="s">
         <v>21</v>
@@ -18225,7 +17880,7 @@
       </c>
       <c r="I285" s="17"/>
     </row>
-    <row r="286" spans="1:9" ht="15">
+    <row r="286" spans="1:9" ht="15.75">
       <c r="A286" s="17"/>
       <c r="B286" s="17" t="s">
         <v>21</v>
@@ -18248,7 +17903,7 @@
       </c>
       <c r="I286" s="17"/>
     </row>
-    <row r="287" spans="1:9" ht="15">
+    <row r="287" spans="1:9" ht="15.75">
       <c r="A287" s="17"/>
       <c r="B287" s="17" t="s">
         <v>21</v>
@@ -18271,7 +17926,7 @@
       </c>
       <c r="I287" s="17"/>
     </row>
-    <row r="288" spans="1:9" ht="15">
+    <row r="288" spans="1:9" ht="15.75">
       <c r="A288" s="17" t="b">
         <v>0</v>
       </c>
@@ -18290,7 +17945,7 @@
       <c r="H288" s="17"/>
       <c r="I288" s="17"/>
     </row>
-    <row r="289" spans="1:9" ht="15">
+    <row r="289" spans="1:9" ht="15.75">
       <c r="A289" s="17"/>
       <c r="B289" s="17" t="s">
         <v>21</v>
@@ -18313,7 +17968,7 @@
       </c>
       <c r="I289" s="17"/>
     </row>
-    <row r="290" spans="1:9" ht="15">
+    <row r="290" spans="1:9" ht="15.75">
       <c r="A290" s="17" t="b">
         <v>0</v>
       </c>
@@ -18332,7 +17987,7 @@
       <c r="H290" s="17"/>
       <c r="I290" s="17"/>
     </row>
-    <row r="291" spans="1:9" ht="15">
+    <row r="291" spans="1:9" ht="15.75">
       <c r="A291" s="17"/>
       <c r="B291" s="17" t="s">
         <v>21</v>
@@ -18353,7 +18008,7 @@
       <c r="H291" s="17"/>
       <c r="I291" s="17"/>
     </row>
-    <row r="292" spans="1:9" ht="15">
+    <row r="292" spans="1:9" ht="15.75">
       <c r="A292" s="17" t="b">
         <v>0</v>
       </c>
@@ -18372,7 +18027,7 @@
       <c r="H292" s="17"/>
       <c r="I292" s="17"/>
     </row>
-    <row r="293" spans="1:9" ht="15">
+    <row r="293" spans="1:9" ht="15.75">
       <c r="A293" s="17"/>
       <c r="B293" s="17" t="s">
         <v>21</v>
@@ -18393,7 +18048,7 @@
       <c r="H293" s="17"/>
       <c r="I293" s="17"/>
     </row>
-    <row r="294" spans="1:9" ht="15">
+    <row r="294" spans="1:9" ht="15.75">
       <c r="A294" s="17" t="b">
         <v>0</v>
       </c>
@@ -18412,7 +18067,7 @@
       <c r="H294" s="17"/>
       <c r="I294" s="17"/>
     </row>
-    <row r="295" spans="1:9" ht="15">
+    <row r="295" spans="1:9" ht="15.75">
       <c r="A295" s="17"/>
       <c r="B295" s="17" t="s">
         <v>21</v>
@@ -18433,7 +18088,7 @@
       <c r="H295" s="17"/>
       <c r="I295" s="17"/>
     </row>
-    <row r="296" spans="1:9" ht="15">
+    <row r="296" spans="1:9" ht="15.75">
       <c r="A296" s="17" t="b">
         <v>0</v>
       </c>
@@ -18452,7 +18107,7 @@
       <c r="H296" s="17"/>
       <c r="I296" s="17"/>
     </row>
-    <row r="297" spans="1:9" ht="15">
+    <row r="297" spans="1:9" ht="15.75">
       <c r="A297" s="17"/>
       <c r="B297" s="17" t="s">
         <v>21</v>
@@ -18475,7 +18130,7 @@
       </c>
       <c r="I297" s="17"/>
     </row>
-    <row r="298" spans="1:9" ht="15">
+    <row r="298" spans="1:9" ht="15.75">
       <c r="A298" s="17" t="b">
         <v>0</v>
       </c>
@@ -18494,7 +18149,7 @@
       <c r="H298" s="17"/>
       <c r="I298" s="17"/>
     </row>
-    <row r="299" spans="1:9" ht="15">
+    <row r="299" spans="1:9" ht="15.75">
       <c r="A299" s="17"/>
       <c r="B299" s="17" t="s">
         <v>21</v>
@@ -18519,7 +18174,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="300" spans="1:9" ht="15">
+    <row r="300" spans="1:9" ht="15.75">
       <c r="A300" s="17"/>
       <c r="B300" s="17" t="s">
         <v>21</v>
@@ -18542,7 +18197,7 @@
       </c>
       <c r="I300" s="17"/>
     </row>
-    <row r="301" spans="1:9" ht="15">
+    <row r="301" spans="1:9" ht="15.75">
       <c r="A301" s="17"/>
       <c r="B301" s="17" t="s">
         <v>21</v>
@@ -18565,7 +18220,7 @@
       </c>
       <c r="I301" s="17"/>
     </row>
-    <row r="302" spans="1:9" ht="15">
+    <row r="302" spans="1:9" ht="15.75">
       <c r="A302" s="17"/>
       <c r="B302" s="17" t="s">
         <v>21</v>
@@ -18588,7 +18243,7 @@
       </c>
       <c r="I302" s="17"/>
     </row>
-    <row r="303" spans="1:9" ht="15">
+    <row r="303" spans="1:9" ht="15.75">
       <c r="A303" s="17"/>
       <c r="B303" s="17" t="s">
         <v>21</v>
@@ -18611,7 +18266,7 @@
       </c>
       <c r="I303" s="17"/>
     </row>
-    <row r="304" spans="1:9" ht="15">
+    <row r="304" spans="1:9" ht="15.75">
       <c r="A304" s="17"/>
       <c r="B304" s="17" t="s">
         <v>21</v>
@@ -18634,7 +18289,7 @@
       </c>
       <c r="I304" s="17"/>
     </row>
-    <row r="305" spans="1:9" ht="15">
+    <row r="305" spans="1:9" ht="15.75">
       <c r="A305" s="17"/>
       <c r="B305" s="17" t="s">
         <v>21</v>
@@ -18657,7 +18312,7 @@
       </c>
       <c r="I305" s="17"/>
     </row>
-    <row r="306" spans="1:9" ht="15">
+    <row r="306" spans="1:9" ht="15.75">
       <c r="A306" s="17"/>
       <c r="B306" s="17" t="s">
         <v>21</v>
@@ -18680,7 +18335,7 @@
       </c>
       <c r="I306" s="17"/>
     </row>
-    <row r="307" spans="1:9" ht="15">
+    <row r="307" spans="1:9" ht="15.75">
       <c r="A307" s="17"/>
       <c r="B307" s="17" t="s">
         <v>21</v>
@@ -18703,7 +18358,7 @@
       </c>
       <c r="I307" s="17"/>
     </row>
-    <row r="308" spans="1:9" ht="15">
+    <row r="308" spans="1:9" ht="15.75">
       <c r="A308" s="17" t="b">
         <v>0</v>
       </c>
@@ -18722,7 +18377,7 @@
       <c r="H308" s="17"/>
       <c r="I308" s="17"/>
     </row>
-    <row r="309" spans="1:9" ht="15">
+    <row r="309" spans="1:9" ht="15.75">
       <c r="A309" s="17"/>
       <c r="B309" s="17" t="s">
         <v>21</v>
@@ -18745,7 +18400,7 @@
       </c>
       <c r="I309" s="17"/>
     </row>
-    <row r="310" spans="1:9" ht="15">
+    <row r="310" spans="1:9" ht="15.75">
       <c r="A310" s="17"/>
       <c r="B310" s="17" t="s">
         <v>21</v>
@@ -18768,7 +18423,7 @@
       </c>
       <c r="I310" s="17"/>
     </row>
-    <row r="311" spans="1:9" ht="15">
+    <row r="311" spans="1:9" ht="15.75">
       <c r="A311" s="17"/>
       <c r="B311" s="17" t="s">
         <v>21</v>
@@ -18791,7 +18446,7 @@
       </c>
       <c r="I311" s="17"/>
     </row>
-    <row r="312" spans="1:9" ht="15">
+    <row r="312" spans="1:9" ht="15.75">
       <c r="A312" s="17"/>
       <c r="B312" s="17" t="s">
         <v>21</v>
@@ -18814,7 +18469,7 @@
       </c>
       <c r="I312" s="17"/>
     </row>
-    <row r="313" spans="1:9" ht="15">
+    <row r="313" spans="1:9" ht="15.75">
       <c r="A313" s="17" t="b">
         <v>0</v>
       </c>
@@ -18833,7 +18488,7 @@
       <c r="H313" s="17"/>
       <c r="I313" s="17"/>
     </row>
-    <row r="314" spans="1:9" ht="15">
+    <row r="314" spans="1:9" ht="15.75">
       <c r="A314" s="17"/>
       <c r="B314" s="17" t="s">
         <v>21</v>
@@ -18856,7 +18511,7 @@
       </c>
       <c r="I314" s="17"/>
     </row>
-    <row r="315" spans="1:9" ht="15">
+    <row r="315" spans="1:9" ht="15.75">
       <c r="A315" s="17"/>
       <c r="B315" s="17" t="s">
         <v>21</v>
@@ -18879,7 +18534,7 @@
       </c>
       <c r="I315" s="17"/>
     </row>
-    <row r="316" spans="1:9" ht="15">
+    <row r="316" spans="1:9" ht="15.75">
       <c r="A316" s="17"/>
       <c r="B316" s="17" t="s">
         <v>21</v>
@@ -18904,7 +18559,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="317" spans="1:9" ht="15">
+    <row r="317" spans="1:9" ht="15.75">
       <c r="A317" s="17" t="b">
         <v>0</v>
       </c>
@@ -18923,7 +18578,7 @@
       <c r="H317" s="17"/>
       <c r="I317" s="17"/>
     </row>
-    <row r="318" spans="1:9" ht="15">
+    <row r="318" spans="1:9" ht="15.75">
       <c r="A318" s="17"/>
       <c r="B318" s="17" t="s">
         <v>21</v>
@@ -18948,7 +18603,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="319" spans="1:9" ht="15">
+    <row r="319" spans="1:9" ht="15.75">
       <c r="A319" s="17"/>
       <c r="B319" s="17" t="s">
         <v>21</v>
@@ -18971,7 +18626,7 @@
       </c>
       <c r="I319" s="17"/>
     </row>
-    <row r="320" spans="1:9" ht="15">
+    <row r="320" spans="1:9" ht="15.75">
       <c r="A320" s="17" t="b">
         <v>0</v>
       </c>
@@ -18990,7 +18645,7 @@
       <c r="H320" s="17"/>
       <c r="I320" s="17"/>
     </row>
-    <row r="321" spans="1:9" ht="15">
+    <row r="321" spans="1:9" ht="15.75">
       <c r="A321" s="17"/>
       <c r="B321" s="17" t="s">
         <v>21</v>
@@ -19011,7 +18666,7 @@
       <c r="H321" s="17"/>
       <c r="I321" s="17"/>
     </row>
-    <row r="322" spans="1:9" ht="15">
+    <row r="322" spans="1:9" ht="15.75">
       <c r="A322" s="17"/>
       <c r="B322" s="17" t="s">
         <v>21</v>
@@ -19032,7 +18687,7 @@
       <c r="H322" s="17"/>
       <c r="I322" s="17"/>
     </row>
-    <row r="323" spans="1:9" ht="15">
+    <row r="323" spans="1:9" ht="15.75">
       <c r="A323" s="17"/>
       <c r="B323" s="17" t="s">
         <v>21</v>
@@ -19055,7 +18710,7 @@
       </c>
       <c r="I323" s="17"/>
     </row>
-    <row r="324" spans="1:9" ht="15">
+    <row r="324" spans="1:9" ht="15.75">
       <c r="A324" s="17" t="b">
         <v>0</v>
       </c>
@@ -19074,7 +18729,7 @@
       <c r="H324" s="17"/>
       <c r="I324" s="17"/>
     </row>
-    <row r="325" spans="1:9" ht="15">
+    <row r="325" spans="1:9" ht="15.75">
       <c r="A325" s="17" t="b">
         <v>0</v>
       </c>
@@ -19093,7 +18748,7 @@
       <c r="H325" s="17"/>
       <c r="I325" s="17"/>
     </row>
-    <row r="326" spans="1:9" ht="15">
+    <row r="326" spans="1:9" ht="15.75">
       <c r="A326" s="17"/>
       <c r="B326" s="17" t="s">
         <v>21</v>
@@ -19118,7 +18773,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="327" spans="1:9" ht="15">
+    <row r="327" spans="1:9" ht="15.75">
       <c r="A327" s="17"/>
       <c r="B327" s="17" t="s">
         <v>21</v>
@@ -19475,7 +19130,7 @@
       <c r="O343" s="1"/>
       <c r="P343" s="1"/>
     </row>
-    <row r="344" spans="1:16" ht="15">
+    <row r="344" spans="1:16" ht="15.75">
       <c r="A344" s="17"/>
       <c r="B344" t="s">
         <v>21</v>
@@ -19838,7 +19493,7 @@
       <c r="J361"/>
       <c r="K361"/>
     </row>
-    <row r="362" spans="1:18" s="1" customFormat="1" ht="15">
+    <row r="362" spans="1:18" s="1" customFormat="1" ht="15.75">
       <c r="A362" s="17"/>
       <c r="B362" t="s">
         <v>22</v>
@@ -19966,14 +19621,14 @@
       <selection activeCell="A17" sqref="A17:A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" customWidth="1"/>
-    <col min="8" max="8" width="22.33203125" customWidth="1"/>
-    <col min="17" max="17" width="24.5" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" customWidth="1"/>
+    <col min="17" max="17" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">

</xml_diff>